<commit_message>
Updated report and data
</commit_message>
<xml_diff>
--- a/inst/googlesheet/microcosmScheme.xlsx
+++ b/inst/googlesheet/microcosmScheme.xlsx
@@ -10,8 +10,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="B97">
+      <text>
+        <t xml:space="preserve">I would change to DNA barcoding for clarity.
+	-Vanessa Weber de Melo
+If you think this is needed, could you please add the necessary properties? Thanks.
+	-Rainer M Krug</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B99">
+      <text>
+        <t xml:space="preserve">The correct name is "Gen- proteo- and epigenomics". But I would change the name to something more general, such as molecular analyses. One might use qPCR to look at specific genes, so no "omics" there, and it would not fall into any of the categories.
+	-Vanessa Weber de Melo
+Changed - but the question is, is this needed, i.e. used regularly, or is this a specific analysis method in a specific experiment. In this case, it could be abbey under a section "additional" as a text description of the analysis method?
+	-Rainer M Krug
+I think both DNA barcoding and all the "omics" are not used regularly and could be in the additional section.
+	-Vanessa Weber de Melo
+OK - I have left them at this level, but only added one "free text field" so that they can be doc bribed as needed. Leaving them in as is, makes it possible to consistently search for experiments using these.
+	-Rainer M Krug
+See comment below.
+	-Rainer M Krug</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="115">
   <si>
     <t>Property Level 1</t>
   </si>
@@ -76,6 +108,15 @@
     <t>covers</t>
   </si>
   <si>
+    <t>Shakers</t>
+  </si>
+  <si>
+    <t>make / type</t>
+  </si>
+  <si>
+    <t>speed (rpm)</t>
+  </si>
+  <si>
     <t>Species</t>
   </si>
   <si>
@@ -88,7 +129,7 @@
     <t>source</t>
   </si>
   <si>
-    <t>concentration</t>
+    <t>density (cells/ml)</t>
   </si>
   <si>
     <t>Culture medium</t>
@@ -130,6 +171,12 @@
     <t>Final conditions</t>
   </si>
   <si>
+    <t>no of treatments</t>
+  </si>
+  <si>
+    <t>no of replicates per treatment</t>
+  </si>
+  <si>
     <t>Conditions</t>
   </si>
   <si>
@@ -142,7 +189,7 @@
     <t>Density</t>
   </si>
   <si>
-    <t>initial density</t>
+    <t>initial density (cells/ml)</t>
   </si>
   <si>
     <t>density changes</t>
@@ -209,6 +256,9 @@
   </si>
   <si>
     <t>volume in ml</t>
+  </si>
+  <si>
+    <t>replacement medium type</t>
   </si>
   <si>
     <t>Measuring and Extraction</t>
@@ -286,10 +336,16 @@
     <t>Raman microspectroscopy</t>
   </si>
   <si>
-    <t>Barcoding</t>
+    <t>DNA Barcoding</t>
   </si>
   <si>
-    <t>Ge- prote- and epigenomics</t>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Gen- proteo- and epigenomics</t>
+  </si>
+  <si>
+    <t>text (free text description)</t>
   </si>
   <si>
     <t>Respirometry</t>
@@ -338,7 +394,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -408,6 +464,13 @@
       <b/>
       <u/>
       <sz val="14.0"/>
+      <color rgb="FFED220B"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10.0"/>
       <color rgb="FFED220B"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -806,7 +869,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="87">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -906,6 +969,9 @@
     <xf borderId="10" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="9" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="9" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -917,6 +983,9 @@
     </xf>
     <xf borderId="9" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="3" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -957,11 +1026,20 @@
     <xf borderId="13" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="13" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="9" fillId="4" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -1406,24 +1484,20 @@
       <c r="Z9" s="7"/>
     </row>
     <row r="10" ht="24.75" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19">
-        <v>1.1</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -1442,30 +1516,18 @@
     <row r="11" ht="24.75" customHeight="1">
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="33"/>
+      <c r="D11" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="24"/>
       <c r="E11" s="25"/>
       <c r="F11" s="26"/>
-      <c r="G11" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
@@ -1484,15 +1546,15 @@
     <row r="12" ht="24.75" customHeight="1">
       <c r="A12" s="21"/>
       <c r="B12" s="22"/>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="33"/>
+      <c r="D12" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="24"/>
       <c r="E12" s="25"/>
       <c r="F12" s="26"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
+      <c r="I12" s="27"/>
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
@@ -1512,26 +1574,24 @@
       <c r="Z12" s="7"/>
     </row>
     <row r="13" ht="24.75" customHeight="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="27" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="19">
+        <v>1.1</v>
+      </c>
+      <c r="G13" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
@@ -1559,15 +1619,21 @@
       <c r="G14" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="I14" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="28"/>
+      <c r="J14" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="K14" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="28"/>
+      <c r="L14" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
@@ -1584,26 +1650,20 @@
       <c r="Z14" s="7"/>
     </row>
     <row r="15" ht="24.75" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19">
-        <v>1.2</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
@@ -1620,28 +1680,26 @@
       <c r="Z15" s="7"/>
     </row>
     <row r="16" ht="24.75" customHeight="1">
-      <c r="A16" s="14"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="34" t="s">
-        <v>19</v>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23" t="s">
+        <v>27</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="33" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="33" t="s">
+      <c r="I16" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="33" t="s">
+      <c r="J16" s="27" t="s">
         <v>15</v>
       </c>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
@@ -1658,30 +1716,26 @@
       <c r="Z16" s="7"/>
     </row>
     <row r="17" ht="24.75" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="34" t="s">
-        <v>18</v>
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="30" t="s">
+        <v>28</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="33" t="s">
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="33" t="s">
+      <c r="H17" s="28"/>
+      <c r="I17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="33" t="s">
+      <c r="J17" s="28"/>
+      <c r="K17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="L17" s="28"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
@@ -1700,22 +1754,24 @@
     <row r="18" ht="24.75" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="17"/>
       <c r="E18" s="18"/>
       <c r="F18" s="19">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
+      <c r="G18" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
-      <c r="L18" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="L18" s="20"/>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
@@ -1732,30 +1788,28 @@
       <c r="Z18" s="7"/>
     </row>
     <row r="19" ht="24.75" customHeight="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23" t="s">
-        <v>22</v>
+      <c r="A19" s="14"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="35" t="s">
+        <v>19</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="27" t="s">
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="J19" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="27" t="s">
+      <c r="K19" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J19" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="L19" s="28"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
@@ -1772,20 +1826,30 @@
       <c r="Z19" s="7"/>
     </row>
     <row r="20" ht="24.75" customHeight="1">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23" t="s">
-        <v>23</v>
+      <c r="A20" s="14"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="35" t="s">
+        <v>18</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
@@ -1802,26 +1866,24 @@
       <c r="Z20" s="7"/>
     </row>
     <row r="21" ht="24.75" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23" t="s">
-        <v>29</v>
+      <c r="A21" s="14"/>
+      <c r="B21" s="15" t="s">
+        <v>31</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="28"/>
-      <c r="J21" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
@@ -1855,8 +1917,12 @@
       <c r="I22" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
+      <c r="J22" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="L22" s="28"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
@@ -1874,22 +1940,20 @@
       <c r="Z22" s="7"/>
     </row>
     <row r="23" ht="24.75" customHeight="1">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15" t="s">
-        <v>30</v>
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23" t="s">
+        <v>26</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
@@ -1905,23 +1969,27 @@
       <c r="Y23" s="7"/>
       <c r="Z23" s="7"/>
     </row>
-    <row r="24" ht="31.5" customHeight="1">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15" t="s">
-        <v>31</v>
+    <row r="24" ht="24.75" customHeight="1">
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="23" t="s">
+        <v>32</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="19">
-        <v>1.599999999999999</v>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27" t="s">
+        <v>15</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
+      <c r="H24" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="28"/>
+      <c r="J24" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
@@ -1938,22 +2006,26 @@
       <c r="Z24" s="7"/>
     </row>
     <row r="25" ht="24.75" customHeight="1">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15" t="s">
-        <v>32</v>
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="30" t="s">
+        <v>28</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="19">
-        <v>1.699999999999999</v>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27" t="s">
+        <v>15</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
+      <c r="H25" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
@@ -1970,24 +2042,22 @@
       <c r="Z25" s="7"/>
     </row>
     <row r="26" ht="24.75" customHeight="1">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="27" t="s">
-        <v>15</v>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="19">
+        <v>1.5</v>
       </c>
-      <c r="K26" s="28"/>
-      <c r="L26" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
@@ -2003,21 +2073,23 @@
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
     </row>
-    <row r="27" ht="24.75" customHeight="1">
-      <c r="A27" s="21"/>
-      <c r="B27" s="36" t="s">
+    <row r="27" ht="31.5" customHeight="1">
+      <c r="A27" s="14"/>
+      <c r="B27" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="19">
+        <v>1.599999999999999</v>
+      </c>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
@@ -2034,20 +2106,22 @@
       <c r="Z27" s="7"/>
     </row>
     <row r="28" ht="24.75" customHeight="1">
-      <c r="A28" s="21"/>
-      <c r="B28" s="36" t="s">
+      <c r="A28" s="14"/>
+      <c r="B28" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="19">
+        <v>1.699999999999999</v>
+      </c>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
@@ -2064,10 +2138,10 @@
       <c r="Z28" s="7"/>
     </row>
     <row r="29" ht="24.75" customHeight="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="36" t="s">
+      <c r="A29" s="36" t="s">
         <v>36</v>
       </c>
+      <c r="B29" s="31"/>
       <c r="C29" s="22"/>
       <c r="D29" s="24"/>
       <c r="E29" s="25"/>
@@ -2075,9 +2149,13 @@
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
+      <c r="J29" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
+      <c r="L29" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
@@ -2095,7 +2173,7 @@
     </row>
     <row r="30" ht="24.75" customHeight="1">
       <c r="A30" s="21"/>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="37" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="22"/>
@@ -2125,7 +2203,7 @@
     </row>
     <row r="31" ht="24.75" customHeight="1">
       <c r="A31" s="21"/>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="37" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="22"/>
@@ -2154,22 +2232,20 @@
       <c r="Z31" s="7"/>
     </row>
     <row r="32" ht="24.75" customHeight="1">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="41">
-        <v>3.0</v>
-      </c>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
@@ -2185,9 +2261,9 @@
       <c r="Y32" s="7"/>
       <c r="Z32" s="7"/>
     </row>
-    <row r="33" ht="31.5" customHeight="1">
+    <row r="33" ht="24.75" customHeight="1">
       <c r="A33" s="21"/>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="22"/>
@@ -2196,16 +2272,10 @@
       <c r="F33" s="26"/>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
-      <c r="I33" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="I33" s="28"/>
       <c r="J33" s="28"/>
-      <c r="K33" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="L33" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
@@ -2222,20 +2292,20 @@
       <c r="Z33" s="7"/>
     </row>
     <row r="34" ht="24.75" customHeight="1">
-      <c r="A34" s="14"/>
-      <c r="B34" s="43" t="s">
+      <c r="A34" s="21"/>
+      <c r="B34" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
@@ -2252,26 +2322,20 @@
       <c r="Z34" s="7"/>
     </row>
     <row r="35" ht="24.75" customHeight="1">
-      <c r="A35" s="14"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="15" t="s">
+      <c r="A35" s="21"/>
+      <c r="B35" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="19">
-        <v>3.2</v>
-      </c>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="K35" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="L35" s="20"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
@@ -2289,12 +2353,12 @@
     </row>
     <row r="36" ht="24.75" customHeight="1">
       <c r="A36" s="21"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="23" t="s">
-        <v>22</v>
+      <c r="B36" s="38" t="s">
+        <v>43</v>
       </c>
-      <c r="E36" s="48"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="25"/>
       <c r="F36" s="26"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
@@ -2318,20 +2382,22 @@
       <c r="Z36" s="7"/>
     </row>
     <row r="37" ht="24.75" customHeight="1">
-      <c r="A37" s="21"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="49" t="s">
-        <v>22</v>
+      <c r="A37" s="39" t="s">
+        <v>44</v>
       </c>
-      <c r="F37" s="26"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="43">
+        <v>3.0</v>
+      </c>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
@@ -2347,21 +2413,27 @@
       <c r="Y37" s="7"/>
       <c r="Z37" s="7"/>
     </row>
-    <row r="38" ht="24.75" customHeight="1">
+    <row r="38" ht="31.5" customHeight="1">
       <c r="A38" s="21"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="49" t="s">
-        <v>43</v>
+      <c r="B38" s="23" t="s">
+        <v>45</v>
       </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="25"/>
       <c r="F38" s="26"/>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
+      <c r="I38" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
+      <c r="K38" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
       <c r="O38" s="7"/>
@@ -2378,20 +2450,20 @@
       <c r="Z38" s="7"/>
     </row>
     <row r="39" ht="24.75" customHeight="1">
-      <c r="A39" s="21"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="49" t="s">
-        <v>44</v>
+      <c r="A39" s="14"/>
+      <c r="B39" s="45" t="s">
+        <v>46</v>
       </c>
-      <c r="F39" s="26"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
       <c r="O39" s="7"/>
@@ -2409,22 +2481,24 @@
     </row>
     <row r="40" ht="24.75" customHeight="1">
       <c r="A40" s="14"/>
-      <c r="B40" s="46"/>
+      <c r="B40" s="48"/>
       <c r="C40" s="15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D40" s="16"/>
-      <c r="E40" s="45"/>
+      <c r="E40" s="47"/>
       <c r="F40" s="19">
-        <v>3.600000000000001</v>
+        <v>3.2</v>
       </c>
-      <c r="G40" s="33" t="s">
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
+      <c r="K40" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="L40" s="20"/>
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
@@ -2444,11 +2518,11 @@
     <row r="41" ht="24.75" customHeight="1">
       <c r="A41" s="21"/>
       <c r="B41" s="31"/>
-      <c r="C41" s="22"/>
+      <c r="C41" s="49"/>
       <c r="D41" s="23" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
-      <c r="E41" s="48"/>
+      <c r="E41" s="50"/>
       <c r="F41" s="26"/>
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
@@ -2474,26 +2548,18 @@
     <row r="42" ht="24.75" customHeight="1">
       <c r="A42" s="21"/>
       <c r="B42" s="31"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="23" t="s">
-        <v>46</v>
+      <c r="C42" s="49"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="51" t="s">
+        <v>25</v>
       </c>
-      <c r="E42" s="48"/>
       <c r="F42" s="26"/>
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
-      <c r="I42" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J42" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="K42" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="L42" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
       <c r="O42" s="7"/>
@@ -2509,26 +2575,20 @@
       <c r="Y42" s="7"/>
       <c r="Z42" s="7"/>
     </row>
-    <row r="43" ht="31.5" customHeight="1">
+    <row r="43" ht="24.75" customHeight="1">
       <c r="A43" s="21"/>
       <c r="B43" s="31"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="23" t="s">
-        <v>47</v>
+      <c r="C43" s="49"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="52" t="s">
+        <v>48</v>
       </c>
-      <c r="E43" s="48"/>
       <c r="F43" s="26"/>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
-      <c r="I43" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="J43" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="K43" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
       <c r="L43" s="28"/>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
@@ -2548,11 +2608,11 @@
     <row r="44" ht="24.75" customHeight="1">
       <c r="A44" s="21"/>
       <c r="B44" s="31"/>
-      <c r="C44" s="23" t="s">
-        <v>50</v>
+      <c r="C44" s="49"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="51" t="s">
+        <v>49</v>
       </c>
-      <c r="D44" s="22"/>
-      <c r="E44" s="48"/>
       <c r="F44" s="26"/>
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
@@ -2576,24 +2636,24 @@
       <c r="Z44" s="7"/>
     </row>
     <row r="45" ht="24.75" customHeight="1">
-      <c r="A45" s="21"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="23" t="s">
-        <v>51</v>
+      <c r="A45" s="14"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="15" t="s">
+        <v>50</v>
       </c>
-      <c r="E45" s="48"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="27" t="s">
-        <v>27</v>
+      <c r="D45" s="16"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="19">
+        <v>3.600000000000001</v>
       </c>
-      <c r="J45" s="27" t="s">
+      <c r="G45" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
       <c r="O45" s="7"/>
@@ -2614,15 +2674,13 @@
       <c r="B46" s="31"/>
       <c r="C46" s="22"/>
       <c r="D46" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
-      <c r="E46" s="48"/>
+      <c r="E46" s="50"/>
       <c r="F46" s="26"/>
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
-      <c r="I46" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="I46" s="28"/>
       <c r="J46" s="28"/>
       <c r="K46" s="28"/>
       <c r="L46" s="28"/>
@@ -2646,9 +2704,9 @@
       <c r="B47" s="31"/>
       <c r="C47" s="22"/>
       <c r="D47" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
-      <c r="E47" s="48"/>
+      <c r="E47" s="50"/>
       <c r="F47" s="26"/>
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
@@ -2656,10 +2714,14 @@
         <v>15</v>
       </c>
       <c r="J47" s="27" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
-      <c r="K47" s="28"/>
-      <c r="L47" s="28"/>
+      <c r="K47" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="L47" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
@@ -2675,29 +2737,27 @@
       <c r="Y47" s="7"/>
       <c r="Z47" s="7"/>
     </row>
-    <row r="48" ht="24.75" customHeight="1">
+    <row r="48" ht="31.5" customHeight="1">
       <c r="A48" s="21"/>
       <c r="B48" s="31"/>
       <c r="C48" s="22"/>
       <c r="D48" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="50"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="J48" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E48" s="48"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="27" t="s">
+      <c r="K48" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H48" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I48" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J48" s="28"/>
-      <c r="K48" s="28"/>
-      <c r="L48" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="L48" s="28"/>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
@@ -2720,15 +2780,13 @@
         <v>55</v>
       </c>
       <c r="D49" s="22"/>
-      <c r="E49" s="48"/>
+      <c r="E49" s="50"/>
       <c r="F49" s="26"/>
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
       <c r="J49" s="28"/>
-      <c r="K49" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="K49" s="28"/>
       <c r="L49" s="28"/>
       <c r="M49" s="7"/>
       <c r="N49" s="7"/>
@@ -2746,24 +2804,24 @@
       <c r="Z49" s="7"/>
     </row>
     <row r="50" ht="24.75" customHeight="1">
-      <c r="A50" s="14"/>
-      <c r="B50" s="44"/>
-      <c r="C50" s="15" t="s">
+      <c r="A50" s="21"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="17"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="19">
-        <v>3.700000000000001</v>
+      <c r="E50" s="50"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="27" t="s">
+        <v>30</v>
       </c>
-      <c r="G50" s="33" t="s">
+      <c r="J50" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
+      <c r="K50" s="28"/>
+      <c r="L50" s="28"/>
       <c r="M50" s="7"/>
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
@@ -2780,22 +2838,22 @@
       <c r="Z50" s="7"/>
     </row>
     <row r="51" ht="24.75" customHeight="1">
-      <c r="A51" s="14"/>
-      <c r="B51" s="46"/>
-      <c r="C51" s="15" t="s">
+      <c r="A51" s="21"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="16"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="19">
-        <v>3.3</v>
+      <c r="E51" s="50"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="27" t="s">
+        <v>30</v>
       </c>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="28"/>
+      <c r="L51" s="28"/>
       <c r="M51" s="7"/>
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
@@ -2812,22 +2870,24 @@
       <c r="Z51" s="7"/>
     </row>
     <row r="52" ht="24.75" customHeight="1">
-      <c r="A52" s="14"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="15" t="s">
+      <c r="A52" s="21"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="16"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="19">
-        <v>3.4</v>
+      <c r="E52" s="50"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="27" t="s">
+        <v>15</v>
       </c>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="20"/>
+      <c r="J52" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K52" s="28"/>
+      <c r="L52" s="28"/>
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
       <c r="O52" s="7"/>
@@ -2844,22 +2904,28 @@
       <c r="Z52" s="7"/>
     </row>
     <row r="53" ht="24.75" customHeight="1">
-      <c r="A53" s="14"/>
-      <c r="B53" s="46"/>
-      <c r="C53" s="15" t="s">
+      <c r="A53" s="21"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="16"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="19">
-        <v>3.5</v>
+      <c r="E53" s="50"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="27" t="s">
+        <v>15</v>
       </c>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
-      <c r="K53" s="20"/>
-      <c r="L53" s="20"/>
+      <c r="H53" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M53" s="7"/>
       <c r="N53" s="7"/>
       <c r="O53" s="7"/>
@@ -2876,26 +2942,22 @@
       <c r="Z53" s="7"/>
     </row>
     <row r="54" ht="24.75" customHeight="1">
-      <c r="A54" s="50" t="s">
+      <c r="A54" s="21"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="19">
-        <v>2.1</v>
-      </c>
-      <c r="G54" s="33" t="s">
+      <c r="D54" s="22"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="K54" s="20"/>
-      <c r="L54" s="20"/>
+      <c r="L54" s="28"/>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
@@ -2912,28 +2974,24 @@
       <c r="Z54" s="7"/>
     </row>
     <row r="55" ht="24.75" customHeight="1">
-      <c r="A55" s="21"/>
-      <c r="B55" s="23" t="s">
+      <c r="A55" s="14"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="31"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="27" t="s">
+      <c r="D55" s="17"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="19">
+        <v>3.700000000000001</v>
+      </c>
+      <c r="G55" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H55" s="28"/>
-      <c r="I55" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J55" s="28"/>
-      <c r="K55" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="L55" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
       <c r="O55" s="7"/>
@@ -2950,20 +3008,22 @@
       <c r="Z55" s="7"/>
     </row>
     <row r="56" ht="24.75" customHeight="1">
-      <c r="A56" s="21"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="36" t="s">
-        <v>63</v>
+      <c r="A56" s="14"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="15" t="s">
+        <v>62</v>
       </c>
-      <c r="D56" s="24"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="28"/>
-      <c r="J56" s="28"/>
-      <c r="K56" s="28"/>
-      <c r="L56" s="28"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="19">
+        <v>3.3</v>
+      </c>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="20"/>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
       <c r="O56" s="7"/>
@@ -2980,20 +3040,22 @@
       <c r="Z56" s="7"/>
     </row>
     <row r="57" ht="24.75" customHeight="1">
-      <c r="A57" s="21"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="36" t="s">
-        <v>64</v>
+      <c r="A57" s="14"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="15" t="s">
+        <v>63</v>
       </c>
-      <c r="D57" s="24"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="28"/>
-      <c r="H57" s="28"/>
-      <c r="I57" s="28"/>
-      <c r="J57" s="28"/>
-      <c r="K57" s="28"/>
-      <c r="L57" s="28"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="19">
+        <v>3.4</v>
+      </c>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
       <c r="O57" s="7"/>
@@ -3010,26 +3072,22 @@
       <c r="Z57" s="7"/>
     </row>
     <row r="58" ht="24.75" customHeight="1">
-      <c r="A58" s="21"/>
-      <c r="B58" s="23" t="s">
-        <v>65</v>
+      <c r="A58" s="14"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="15" t="s">
+        <v>64</v>
       </c>
-      <c r="C58" s="31"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="28"/>
-      <c r="H58" s="28"/>
-      <c r="I58" s="27" t="s">
-        <v>15</v>
+      <c r="D58" s="16"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="19">
+        <v>3.5</v>
       </c>
-      <c r="J58" s="28"/>
-      <c r="K58" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="L58" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="20"/>
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
       <c r="O58" s="7"/>
@@ -3045,23 +3103,27 @@
       <c r="Y58" s="7"/>
       <c r="Z58" s="7"/>
     </row>
-    <row r="59" ht="41.25" customHeight="1">
-      <c r="A59" s="37" t="s">
-        <v>66</v>
+    <row r="59" ht="24.75" customHeight="1">
+      <c r="A59" s="53" t="s">
+        <v>65</v>
       </c>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="40"/>
-      <c r="F59" s="41">
-        <v>2.0</v>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="19">
+        <v>2.1</v>
       </c>
-      <c r="G59" s="42"/>
-      <c r="H59" s="42"/>
-      <c r="I59" s="42"/>
-      <c r="J59" s="42"/>
-      <c r="K59" s="42"/>
-      <c r="L59" s="42"/>
+      <c r="G59" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="K59" s="20"/>
+      <c r="L59" s="20"/>
       <c r="M59" s="7"/>
       <c r="N59" s="7"/>
       <c r="O59" s="7"/>
@@ -3078,26 +3140,28 @@
       <c r="Z59" s="7"/>
     </row>
     <row r="60" ht="24.75" customHeight="1">
-      <c r="A60" s="14"/>
-      <c r="B60" s="15" t="s">
+      <c r="A60" s="21"/>
+      <c r="B60" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="31"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="28"/>
+      <c r="I60" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J60" s="28"/>
+      <c r="K60" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C60" s="16"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="19">
-        <v>2.2</v>
-      </c>
-      <c r="G60" s="33" t="s">
+      <c r="L60" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H60" s="20"/>
-      <c r="I60" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="J60" s="20"/>
-      <c r="K60" s="20"/>
-      <c r="L60" s="20"/>
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
       <c r="O60" s="7"/>
@@ -3116,7 +3180,7 @@
     <row r="61" ht="24.75" customHeight="1">
       <c r="A61" s="21"/>
       <c r="B61" s="22"/>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="37" t="s">
         <v>68</v>
       </c>
       <c r="D61" s="24"/>
@@ -3146,10 +3210,10 @@
     <row r="62" ht="24.75" customHeight="1">
       <c r="A62" s="21"/>
       <c r="B62" s="22"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="29" t="s">
-        <v>65</v>
+      <c r="C62" s="37" t="s">
+        <v>69</v>
       </c>
+      <c r="D62" s="24"/>
       <c r="E62" s="25"/>
       <c r="F62" s="26"/>
       <c r="G62" s="28"/>
@@ -3175,19 +3239,25 @@
     </row>
     <row r="63" ht="24.75" customHeight="1">
       <c r="A63" s="21"/>
-      <c r="B63" s="22"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="29" t="s">
-        <v>69</v>
+      <c r="B63" s="23" t="s">
+        <v>70</v>
       </c>
+      <c r="C63" s="31"/>
+      <c r="D63" s="24"/>
       <c r="E63" s="25"/>
       <c r="F63" s="26"/>
       <c r="G63" s="28"/>
       <c r="H63" s="28"/>
-      <c r="I63" s="28"/>
+      <c r="I63" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="J63" s="28"/>
-      <c r="K63" s="28"/>
-      <c r="L63" s="28"/>
+      <c r="K63" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L63" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M63" s="7"/>
       <c r="N63" s="7"/>
       <c r="O63" s="7"/>
@@ -3205,21 +3275,19 @@
     </row>
     <row r="64" ht="24.75" customHeight="1">
       <c r="A64" s="21"/>
-      <c r="B64" s="22"/>
-      <c r="C64" s="23" t="s">
-        <v>70</v>
+      <c r="B64" s="30" t="s">
+        <v>71</v>
       </c>
+      <c r="C64" s="31"/>
       <c r="D64" s="24"/>
       <c r="E64" s="25"/>
       <c r="F64" s="26"/>
       <c r="G64" s="28"/>
       <c r="H64" s="28"/>
-      <c r="I64" s="28"/>
+      <c r="I64" s="27"/>
       <c r="J64" s="28"/>
-      <c r="K64" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="L64" s="28"/>
+      <c r="K64" s="27"/>
+      <c r="L64" s="27"/>
       <c r="M64" s="7"/>
       <c r="N64" s="7"/>
       <c r="O64" s="7"/>
@@ -3235,27 +3303,23 @@
       <c r="Y64" s="7"/>
       <c r="Z64" s="7"/>
     </row>
-    <row r="65" ht="24.75" customHeight="1">
-      <c r="A65" s="21"/>
-      <c r="B65" s="22"/>
-      <c r="C65" s="23" t="s">
+    <row r="65" ht="41.25" customHeight="1">
+      <c r="A65" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="D65" s="24"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="26"/>
-      <c r="G65" s="28"/>
-      <c r="H65" s="28"/>
-      <c r="I65" s="27" t="s">
-        <v>15</v>
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="43">
+        <v>2.0</v>
       </c>
-      <c r="J65" s="28"/>
-      <c r="K65" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="L65" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="G65" s="44"/>
+      <c r="H65" s="44"/>
+      <c r="I65" s="44"/>
+      <c r="J65" s="44"/>
+      <c r="K65" s="44"/>
+      <c r="L65" s="44"/>
       <c r="M65" s="7"/>
       <c r="N65" s="7"/>
       <c r="O65" s="7"/>
@@ -3271,7 +3335,7 @@
       <c r="Y65" s="7"/>
       <c r="Z65" s="7"/>
     </row>
-    <row r="66" ht="55.5" customHeight="1">
+    <row r="66" ht="24.75" customHeight="1">
       <c r="A66" s="14"/>
       <c r="B66" s="15" t="s">
         <v>73</v>
@@ -3280,16 +3344,16 @@
       <c r="D66" s="17"/>
       <c r="E66" s="18"/>
       <c r="F66" s="19">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
-      <c r="G66" s="33" t="s">
+      <c r="G66" s="34" t="s">
         <v>15</v>
       </c>
       <c r="H66" s="20"/>
-      <c r="I66" s="20"/>
-      <c r="J66" s="33" t="s">
-        <v>74</v>
+      <c r="I66" s="34" t="s">
+        <v>15</v>
       </c>
+      <c r="J66" s="20"/>
       <c r="K66" s="20"/>
       <c r="L66" s="20"/>
       <c r="M66" s="7"/>
@@ -3310,11 +3374,11 @@
     <row r="67" ht="24.75" customHeight="1">
       <c r="A67" s="21"/>
       <c r="B67" s="22"/>
-      <c r="C67" s="36" t="s">
-        <v>75</v>
+      <c r="C67" s="23" t="s">
+        <v>74</v>
       </c>
-      <c r="D67" s="22"/>
-      <c r="E67" s="48"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="25"/>
       <c r="F67" s="26"/>
       <c r="G67" s="28"/>
       <c r="H67" s="28"/>
@@ -3340,11 +3404,11 @@
     <row r="68" ht="24.75" customHeight="1">
       <c r="A68" s="21"/>
       <c r="B68" s="22"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="23" t="s">
-        <v>68</v>
+      <c r="C68" s="22"/>
+      <c r="D68" s="29" t="s">
+        <v>70</v>
       </c>
-      <c r="E68" s="48"/>
+      <c r="E68" s="25"/>
       <c r="F68" s="26"/>
       <c r="G68" s="28"/>
       <c r="H68" s="28"/>
@@ -3370,11 +3434,11 @@
     <row r="69" ht="24.75" customHeight="1">
       <c r="A69" s="21"/>
       <c r="B69" s="22"/>
-      <c r="C69" s="31"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="49" t="s">
-        <v>65</v>
+      <c r="C69" s="22"/>
+      <c r="D69" s="29" t="s">
+        <v>75</v>
       </c>
+      <c r="E69" s="25"/>
       <c r="F69" s="26"/>
       <c r="G69" s="28"/>
       <c r="H69" s="28"/>
@@ -3400,17 +3464,19 @@
     <row r="70" ht="24.75" customHeight="1">
       <c r="A70" s="21"/>
       <c r="B70" s="22"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="49" t="s">
-        <v>69</v>
+      <c r="C70" s="23" t="s">
+        <v>76</v>
       </c>
+      <c r="D70" s="24"/>
+      <c r="E70" s="25"/>
       <c r="F70" s="26"/>
       <c r="G70" s="28"/>
       <c r="H70" s="28"/>
       <c r="I70" s="28"/>
       <c r="J70" s="28"/>
-      <c r="K70" s="28"/>
+      <c r="K70" s="27" t="s">
+        <v>77</v>
+      </c>
       <c r="L70" s="28"/>
       <c r="M70" s="7"/>
       <c r="N70" s="7"/>
@@ -3430,19 +3496,21 @@
     <row r="71" ht="24.75" customHeight="1">
       <c r="A71" s="21"/>
       <c r="B71" s="22"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="23" t="s">
-        <v>76</v>
+      <c r="C71" s="23" t="s">
+        <v>78</v>
       </c>
-      <c r="E71" s="48"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="25"/>
       <c r="F71" s="26"/>
-      <c r="G71" s="27" t="s">
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H71" s="28"/>
-      <c r="I71" s="28"/>
       <c r="J71" s="28"/>
-      <c r="K71" s="28"/>
+      <c r="K71" s="27" t="s">
+        <v>67</v>
+      </c>
       <c r="L71" s="27" t="s">
         <v>15</v>
       </c>
@@ -3461,23 +3529,27 @@
       <c r="Y71" s="7"/>
       <c r="Z71" s="7"/>
     </row>
-    <row r="72" ht="31.5" customHeight="1">
-      <c r="A72" s="21"/>
-      <c r="B72" s="22"/>
-      <c r="C72" s="31"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="49" t="s">
-        <v>77</v>
+    <row r="72" ht="55.5" customHeight="1">
+      <c r="A72" s="14"/>
+      <c r="B72" s="15" t="s">
+        <v>79</v>
       </c>
-      <c r="F72" s="26"/>
-      <c r="G72" s="28"/>
-      <c r="H72" s="28"/>
-      <c r="I72" s="28"/>
-      <c r="J72" s="28"/>
-      <c r="K72" s="28"/>
-      <c r="L72" s="27" t="s">
+      <c r="C72" s="16"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="19">
+        <v>2.3</v>
+      </c>
+      <c r="G72" s="34" t="s">
         <v>15</v>
       </c>
+      <c r="H72" s="20"/>
+      <c r="I72" s="20"/>
+      <c r="J72" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="K72" s="20"/>
+      <c r="L72" s="20"/>
       <c r="M72" s="7"/>
       <c r="N72" s="7"/>
       <c r="O72" s="7"/>
@@ -3496,20 +3568,18 @@
     <row r="73" ht="24.75" customHeight="1">
       <c r="A73" s="21"/>
       <c r="B73" s="22"/>
-      <c r="C73" s="31"/>
+      <c r="C73" s="37" t="s">
+        <v>81</v>
+      </c>
       <c r="D73" s="22"/>
-      <c r="E73" s="49" t="s">
-        <v>78</v>
-      </c>
+      <c r="E73" s="50"/>
       <c r="F73" s="26"/>
       <c r="G73" s="28"/>
       <c r="H73" s="28"/>
       <c r="I73" s="28"/>
       <c r="J73" s="28"/>
       <c r="K73" s="28"/>
-      <c r="L73" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="L73" s="28"/>
       <c r="M73" s="7"/>
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>
@@ -3529,21 +3599,17 @@
       <c r="A74" s="21"/>
       <c r="B74" s="22"/>
       <c r="C74" s="31"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="49" t="s">
-        <v>79</v>
+      <c r="D74" s="23" t="s">
+        <v>74</v>
       </c>
+      <c r="E74" s="50"/>
       <c r="F74" s="26"/>
-      <c r="G74" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="G74" s="28"/>
       <c r="H74" s="28"/>
       <c r="I74" s="28"/>
       <c r="J74" s="28"/>
       <c r="K74" s="28"/>
-      <c r="L74" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="L74" s="28"/>
       <c r="M74" s="7"/>
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
@@ -3563,10 +3629,10 @@
       <c r="A75" s="21"/>
       <c r="B75" s="22"/>
       <c r="C75" s="31"/>
-      <c r="D75" s="23" t="s">
-        <v>80</v>
+      <c r="D75" s="22"/>
+      <c r="E75" s="51" t="s">
+        <v>70</v>
       </c>
-      <c r="E75" s="48"/>
       <c r="F75" s="26"/>
       <c r="G75" s="28"/>
       <c r="H75" s="28"/>
@@ -3594,20 +3660,16 @@
       <c r="B76" s="22"/>
       <c r="C76" s="31"/>
       <c r="D76" s="22"/>
-      <c r="E76" s="49" t="s">
-        <v>81</v>
+      <c r="E76" s="51" t="s">
+        <v>75</v>
       </c>
       <c r="F76" s="26"/>
-      <c r="G76" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="G76" s="28"/>
       <c r="H76" s="28"/>
       <c r="I76" s="28"/>
       <c r="J76" s="28"/>
       <c r="K76" s="28"/>
-      <c r="L76" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="L76" s="28"/>
       <c r="M76" s="7"/>
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
@@ -3627,17 +3689,21 @@
       <c r="A77" s="21"/>
       <c r="B77" s="22"/>
       <c r="C77" s="31"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="49" t="s">
+      <c r="D77" s="23" t="s">
         <v>82</v>
       </c>
+      <c r="E77" s="50"/>
       <c r="F77" s="26"/>
-      <c r="G77" s="28"/>
+      <c r="G77" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="H77" s="28"/>
       <c r="I77" s="28"/>
       <c r="J77" s="28"/>
       <c r="K77" s="28"/>
-      <c r="L77" s="28"/>
+      <c r="L77" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
       <c r="O77" s="7"/>
@@ -3653,21 +3719,23 @@
       <c r="Y77" s="7"/>
       <c r="Z77" s="7"/>
     </row>
-    <row r="78" ht="24.75" customHeight="1">
+    <row r="78" ht="31.5" customHeight="1">
       <c r="A78" s="21"/>
       <c r="B78" s="22"/>
-      <c r="C78" s="23" t="s">
+      <c r="C78" s="31"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="D78" s="24"/>
-      <c r="E78" s="51"/>
       <c r="F78" s="26"/>
       <c r="G78" s="28"/>
       <c r="H78" s="28"/>
       <c r="I78" s="28"/>
       <c r="J78" s="28"/>
       <c r="K78" s="28"/>
-      <c r="L78" s="28"/>
+      <c r="L78" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
       <c r="O78" s="7"/>
@@ -3686,18 +3754,20 @@
     <row r="79" ht="24.75" customHeight="1">
       <c r="A79" s="21"/>
       <c r="B79" s="22"/>
-      <c r="C79" s="22"/>
-      <c r="D79" s="29" t="s">
-        <v>16</v>
+      <c r="C79" s="31"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="51" t="s">
+        <v>84</v>
       </c>
-      <c r="E79" s="51"/>
       <c r="F79" s="26"/>
       <c r="G79" s="28"/>
       <c r="H79" s="28"/>
       <c r="I79" s="28"/>
       <c r="J79" s="28"/>
       <c r="K79" s="28"/>
-      <c r="L79" s="28"/>
+      <c r="L79" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M79" s="7"/>
       <c r="N79" s="7"/>
       <c r="O79" s="7"/>
@@ -3716,18 +3786,22 @@
     <row r="80" ht="24.75" customHeight="1">
       <c r="A80" s="21"/>
       <c r="B80" s="22"/>
-      <c r="C80" s="22"/>
-      <c r="D80" s="29" t="s">
-        <v>84</v>
+      <c r="C80" s="31"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="51" t="s">
+        <v>85</v>
       </c>
-      <c r="E80" s="51"/>
       <c r="F80" s="26"/>
-      <c r="G80" s="28"/>
+      <c r="G80" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="H80" s="28"/>
       <c r="I80" s="28"/>
       <c r="J80" s="28"/>
       <c r="K80" s="28"/>
-      <c r="L80" s="28"/>
+      <c r="L80" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
@@ -3746,11 +3820,11 @@
     <row r="81" ht="24.75" customHeight="1">
       <c r="A81" s="21"/>
       <c r="B81" s="22"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="29" t="s">
-        <v>85</v>
+      <c r="C81" s="31"/>
+      <c r="D81" s="23" t="s">
+        <v>86</v>
       </c>
-      <c r="E81" s="51"/>
+      <c r="E81" s="50"/>
       <c r="F81" s="26"/>
       <c r="G81" s="28"/>
       <c r="H81" s="28"/>
@@ -3776,18 +3850,22 @@
     <row r="82" ht="24.75" customHeight="1">
       <c r="A82" s="21"/>
       <c r="B82" s="22"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="29" t="s">
-        <v>70</v>
+      <c r="C82" s="31"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="51" t="s">
+        <v>87</v>
       </c>
-      <c r="E82" s="51"/>
       <c r="F82" s="26"/>
-      <c r="G82" s="28"/>
+      <c r="G82" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="H82" s="28"/>
       <c r="I82" s="28"/>
       <c r="J82" s="28"/>
       <c r="K82" s="28"/>
-      <c r="L82" s="28"/>
+      <c r="L82" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
       <c r="O82" s="7"/>
@@ -3803,25 +3881,21 @@
       <c r="Y82" s="7"/>
       <c r="Z82" s="7"/>
     </row>
-    <row r="83" ht="31.5" customHeight="1">
-      <c r="A83" s="14"/>
-      <c r="B83" s="15" t="s">
-        <v>86</v>
+    <row r="83" ht="24.75" customHeight="1">
+      <c r="A83" s="21"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="31"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="51" t="s">
+        <v>88</v>
       </c>
-      <c r="C83" s="16"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="19">
-        <v>2.5</v>
-      </c>
-      <c r="G83" s="20"/>
-      <c r="H83" s="20"/>
-      <c r="I83" s="20"/>
-      <c r="J83" s="20"/>
-      <c r="K83" s="20"/>
-      <c r="L83" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="F83" s="26"/>
+      <c r="G83" s="28"/>
+      <c r="H83" s="28"/>
+      <c r="I83" s="28"/>
+      <c r="J83" s="28"/>
+      <c r="K83" s="28"/>
+      <c r="L83" s="28"/>
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
       <c r="O83" s="7"/>
@@ -3839,12 +3913,12 @@
     </row>
     <row r="84" ht="24.75" customHeight="1">
       <c r="A84" s="21"/>
-      <c r="B84" s="47"/>
+      <c r="B84" s="22"/>
       <c r="C84" s="23" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D84" s="24"/>
-      <c r="E84" s="25"/>
+      <c r="E84" s="54"/>
       <c r="F84" s="26"/>
       <c r="G84" s="28"/>
       <c r="H84" s="28"/>
@@ -3869,21 +3943,19 @@
     </row>
     <row r="85" ht="24.75" customHeight="1">
       <c r="A85" s="21"/>
-      <c r="B85" s="47"/>
-      <c r="C85" s="30" t="s">
-        <v>65</v>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="29" t="s">
+        <v>16</v>
       </c>
-      <c r="D85" s="24"/>
-      <c r="E85" s="25"/>
+      <c r="E85" s="54"/>
       <c r="F85" s="26"/>
       <c r="G85" s="28"/>
       <c r="H85" s="28"/>
       <c r="I85" s="28"/>
       <c r="J85" s="28"/>
       <c r="K85" s="28"/>
-      <c r="L85" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="L85" s="28"/>
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
       <c r="O85" s="7"/>
@@ -3901,21 +3973,19 @@
     </row>
     <row r="86" ht="24.75" customHeight="1">
       <c r="A86" s="21"/>
-      <c r="B86" s="47"/>
-      <c r="C86" s="23" t="s">
-        <v>70</v>
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="29" t="s">
+        <v>90</v>
       </c>
-      <c r="D86" s="24"/>
-      <c r="E86" s="25"/>
+      <c r="E86" s="54"/>
       <c r="F86" s="26"/>
       <c r="G86" s="28"/>
       <c r="H86" s="28"/>
       <c r="I86" s="28"/>
       <c r="J86" s="28"/>
       <c r="K86" s="28"/>
-      <c r="L86" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="L86" s="28"/>
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
       <c r="O86" s="7"/>
@@ -3933,21 +4003,19 @@
     </row>
     <row r="87" ht="24.75" customHeight="1">
       <c r="A87" s="21"/>
-      <c r="B87" s="47"/>
-      <c r="C87" s="30" t="s">
-        <v>88</v>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="29" t="s">
+        <v>91</v>
       </c>
-      <c r="D87" s="24"/>
-      <c r="E87" s="25"/>
+      <c r="E87" s="54"/>
       <c r="F87" s="26"/>
       <c r="G87" s="28"/>
       <c r="H87" s="28"/>
       <c r="I87" s="28"/>
       <c r="J87" s="28"/>
       <c r="K87" s="28"/>
-      <c r="L87" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="L87" s="28"/>
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
       <c r="O87" s="7"/>
@@ -3965,10 +4033,12 @@
     </row>
     <row r="88" ht="24.75" customHeight="1">
       <c r="A88" s="21"/>
-      <c r="B88" s="47"/>
+      <c r="B88" s="22"/>
       <c r="C88" s="22"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="25"/>
+      <c r="D88" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E88" s="54"/>
       <c r="F88" s="26"/>
       <c r="G88" s="28"/>
       <c r="H88" s="28"/>
@@ -3991,23 +4061,25 @@
       <c r="Y88" s="7"/>
       <c r="Z88" s="7"/>
     </row>
-    <row r="89" ht="24.75" customHeight="1">
+    <row r="89" ht="31.5" customHeight="1">
       <c r="A89" s="14"/>
       <c r="B89" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C89" s="16"/>
       <c r="D89" s="17"/>
       <c r="E89" s="18"/>
       <c r="F89" s="19">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="G89" s="20"/>
       <c r="H89" s="20"/>
       <c r="I89" s="20"/>
       <c r="J89" s="20"/>
       <c r="K89" s="20"/>
-      <c r="L89" s="20"/>
+      <c r="L89" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
       <c r="O89" s="7"/>
@@ -4023,23 +4095,21 @@
       <c r="Y89" s="7"/>
       <c r="Z89" s="7"/>
     </row>
-    <row r="90" ht="31.5" customHeight="1">
-      <c r="A90" s="14"/>
-      <c r="B90" s="15" t="s">
-        <v>90</v>
+    <row r="90" ht="24.75" customHeight="1">
+      <c r="A90" s="21"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="23" t="s">
+        <v>93</v>
       </c>
-      <c r="C90" s="16"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="19">
-        <v>2.600000000000001</v>
-      </c>
-      <c r="G90" s="20"/>
-      <c r="H90" s="20"/>
-      <c r="I90" s="20"/>
-      <c r="J90" s="20"/>
-      <c r="K90" s="20"/>
-      <c r="L90" s="20"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="25"/>
+      <c r="F90" s="26"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="28"/>
+      <c r="I90" s="28"/>
+      <c r="J90" s="28"/>
+      <c r="K90" s="28"/>
+      <c r="L90" s="28"/>
       <c r="M90" s="7"/>
       <c r="N90" s="7"/>
       <c r="O90" s="7"/>
@@ -4056,22 +4126,22 @@
       <c r="Z90" s="7"/>
     </row>
     <row r="91" ht="24.75" customHeight="1">
-      <c r="A91" s="14"/>
-      <c r="B91" s="15" t="s">
-        <v>91</v>
+      <c r="A91" s="21"/>
+      <c r="B91" s="49"/>
+      <c r="C91" s="30" t="s">
+        <v>70</v>
       </c>
-      <c r="C91" s="16"/>
-      <c r="D91" s="17"/>
-      <c r="E91" s="18"/>
-      <c r="F91" s="19">
-        <v>2.700000000000001</v>
+      <c r="D91" s="24"/>
+      <c r="E91" s="25"/>
+      <c r="F91" s="26"/>
+      <c r="G91" s="28"/>
+      <c r="H91" s="28"/>
+      <c r="I91" s="28"/>
+      <c r="J91" s="28"/>
+      <c r="K91" s="28"/>
+      <c r="L91" s="27" t="s">
+        <v>15</v>
       </c>
-      <c r="G91" s="20"/>
-      <c r="H91" s="20"/>
-      <c r="I91" s="20"/>
-      <c r="J91" s="20"/>
-      <c r="K91" s="20"/>
-      <c r="L91" s="20"/>
       <c r="M91" s="7"/>
       <c r="N91" s="7"/>
       <c r="O91" s="7"/>
@@ -4087,23 +4157,23 @@
       <c r="Y91" s="7"/>
       <c r="Z91" s="7"/>
     </row>
-    <row r="92" ht="31.5" customHeight="1">
-      <c r="A92" s="14"/>
-      <c r="B92" s="15" t="s">
-        <v>92</v>
+    <row r="92" ht="24.75" customHeight="1">
+      <c r="A92" s="21"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="23" t="s">
+        <v>76</v>
       </c>
-      <c r="C92" s="16"/>
-      <c r="D92" s="17"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="19">
-        <v>2.800000000000001</v>
+      <c r="D92" s="24"/>
+      <c r="E92" s="25"/>
+      <c r="F92" s="26"/>
+      <c r="G92" s="28"/>
+      <c r="H92" s="28"/>
+      <c r="I92" s="28"/>
+      <c r="J92" s="28"/>
+      <c r="K92" s="28"/>
+      <c r="L92" s="27" t="s">
+        <v>15</v>
       </c>
-      <c r="G92" s="20"/>
-      <c r="H92" s="20"/>
-      <c r="I92" s="20"/>
-      <c r="J92" s="20"/>
-      <c r="K92" s="20"/>
-      <c r="L92" s="20"/>
       <c r="M92" s="7"/>
       <c r="N92" s="7"/>
       <c r="O92" s="7"/>
@@ -4120,22 +4190,22 @@
       <c r="Z92" s="7"/>
     </row>
     <row r="93" ht="24.75" customHeight="1">
-      <c r="A93" s="14"/>
-      <c r="B93" s="15" t="s">
-        <v>93</v>
+      <c r="A93" s="21"/>
+      <c r="B93" s="49"/>
+      <c r="C93" s="30" t="s">
+        <v>94</v>
       </c>
-      <c r="C93" s="16"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="18"/>
-      <c r="F93" s="19">
-        <v>2.900000000000001</v>
+      <c r="D93" s="24"/>
+      <c r="E93" s="25"/>
+      <c r="F93" s="26"/>
+      <c r="G93" s="28"/>
+      <c r="H93" s="28"/>
+      <c r="I93" s="28"/>
+      <c r="J93" s="28"/>
+      <c r="K93" s="28"/>
+      <c r="L93" s="27" t="s">
+        <v>15</v>
       </c>
-      <c r="G93" s="20"/>
-      <c r="H93" s="20"/>
-      <c r="I93" s="20"/>
-      <c r="J93" s="20"/>
-      <c r="K93" s="20"/>
-      <c r="L93" s="20"/>
       <c r="M93" s="7"/>
       <c r="N93" s="7"/>
       <c r="O93" s="7"/>
@@ -4151,23 +4221,19 @@
       <c r="Y93" s="7"/>
       <c r="Z93" s="7"/>
     </row>
-    <row r="94" ht="31.5" customHeight="1">
-      <c r="A94" s="14"/>
-      <c r="B94" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C94" s="16"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="18"/>
-      <c r="F94" s="19">
-        <v>2.1</v>
-      </c>
-      <c r="G94" s="20"/>
-      <c r="H94" s="20"/>
-      <c r="I94" s="20"/>
-      <c r="J94" s="20"/>
-      <c r="K94" s="20"/>
-      <c r="L94" s="20"/>
+    <row r="94" ht="24.75" customHeight="1">
+      <c r="A94" s="21"/>
+      <c r="B94" s="49"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="28"/>
+      <c r="H94" s="28"/>
+      <c r="I94" s="28"/>
+      <c r="J94" s="28"/>
+      <c r="K94" s="28"/>
+      <c r="L94" s="28"/>
       <c r="M94" s="7"/>
       <c r="N94" s="7"/>
       <c r="O94" s="7"/>
@@ -4192,11 +4258,9 @@
       <c r="D95" s="17"/>
       <c r="E95" s="18"/>
       <c r="F95" s="19">
-        <v>2.12</v>
+        <v>2.4</v>
       </c>
-      <c r="G95" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="G95" s="20"/>
       <c r="H95" s="20"/>
       <c r="I95" s="20"/>
       <c r="J95" s="20"/>
@@ -4217,19 +4281,23 @@
       <c r="Y95" s="7"/>
       <c r="Z95" s="7"/>
     </row>
-    <row r="96" ht="24.75" customHeight="1">
-      <c r="A96" s="52"/>
-      <c r="B96" s="31"/>
-      <c r="C96" s="31"/>
-      <c r="D96" s="53"/>
-      <c r="E96" s="51"/>
-      <c r="F96" s="54"/>
-      <c r="G96" s="55"/>
-      <c r="H96" s="55"/>
-      <c r="I96" s="55"/>
-      <c r="J96" s="55"/>
-      <c r="K96" s="55"/>
-      <c r="L96" s="55"/>
+    <row r="96" ht="31.5" customHeight="1">
+      <c r="A96" s="14"/>
+      <c r="B96" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C96" s="16"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="19">
+        <v>2.600000000000001</v>
+      </c>
+      <c r="G96" s="20"/>
+      <c r="H96" s="20"/>
+      <c r="I96" s="20"/>
+      <c r="J96" s="20"/>
+      <c r="K96" s="20"/>
+      <c r="L96" s="20"/>
       <c r="M96" s="7"/>
       <c r="N96" s="7"/>
       <c r="O96" s="7"/>
@@ -4246,18 +4314,22 @@
       <c r="Z96" s="7"/>
     </row>
     <row r="97" ht="24.75" customHeight="1">
-      <c r="A97" s="52"/>
-      <c r="B97" s="31"/>
-      <c r="C97" s="31"/>
-      <c r="D97" s="53"/>
-      <c r="E97" s="51"/>
-      <c r="F97" s="54"/>
-      <c r="G97" s="55"/>
-      <c r="H97" s="55"/>
-      <c r="I97" s="55"/>
-      <c r="J97" s="55"/>
-      <c r="K97" s="55"/>
-      <c r="L97" s="55"/>
+      <c r="A97" s="14"/>
+      <c r="B97" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C97" s="16"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="19">
+        <v>2.700000000000001</v>
+      </c>
+      <c r="G97" s="20"/>
+      <c r="H97" s="20"/>
+      <c r="I97" s="20"/>
+      <c r="J97" s="20"/>
+      <c r="K97" s="20"/>
+      <c r="L97" s="20"/>
       <c r="M97" s="7"/>
       <c r="N97" s="7"/>
       <c r="O97" s="7"/>
@@ -4274,18 +4346,20 @@
       <c r="Z97" s="7"/>
     </row>
     <row r="98" ht="24.75" customHeight="1">
-      <c r="A98" s="52"/>
-      <c r="B98" s="31"/>
-      <c r="C98" s="31"/>
-      <c r="D98" s="53"/>
-      <c r="E98" s="51"/>
-      <c r="F98" s="54"/>
-      <c r="G98" s="55"/>
-      <c r="H98" s="55"/>
-      <c r="I98" s="55"/>
-      <c r="J98" s="55"/>
-      <c r="K98" s="55"/>
-      <c r="L98" s="55"/>
+      <c r="A98" s="14"/>
+      <c r="B98" s="55"/>
+      <c r="C98" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="D98" s="17"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="20"/>
+      <c r="H98" s="20"/>
+      <c r="I98" s="20"/>
+      <c r="J98" s="20"/>
+      <c r="K98" s="20"/>
+      <c r="L98" s="20"/>
       <c r="M98" s="7"/>
       <c r="N98" s="7"/>
       <c r="O98" s="7"/>
@@ -4301,19 +4375,23 @@
       <c r="Y98" s="7"/>
       <c r="Z98" s="7"/>
     </row>
-    <row r="99" ht="24.75" customHeight="1">
-      <c r="A99" s="52"/>
-      <c r="B99" s="31"/>
-      <c r="C99" s="31"/>
-      <c r="D99" s="53"/>
-      <c r="E99" s="51"/>
-      <c r="F99" s="54"/>
-      <c r="G99" s="55"/>
-      <c r="H99" s="55"/>
-      <c r="I99" s="55"/>
-      <c r="J99" s="55"/>
-      <c r="K99" s="55"/>
-      <c r="L99" s="55"/>
+    <row r="99" ht="31.5" customHeight="1">
+      <c r="A99" s="14"/>
+      <c r="B99" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C99" s="16"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="19">
+        <v>2.800000000000001</v>
+      </c>
+      <c r="G99" s="20"/>
+      <c r="H99" s="20"/>
+      <c r="I99" s="20"/>
+      <c r="J99" s="20"/>
+      <c r="K99" s="20"/>
+      <c r="L99" s="20"/>
       <c r="M99" s="7"/>
       <c r="N99" s="7"/>
       <c r="O99" s="7"/>
@@ -4329,19 +4407,21 @@
       <c r="Y99" s="7"/>
       <c r="Z99" s="7"/>
     </row>
-    <row r="100" ht="24.75" customHeight="1">
-      <c r="A100" s="52"/>
-      <c r="B100" s="31"/>
-      <c r="C100" s="31"/>
-      <c r="D100" s="53"/>
-      <c r="E100" s="51"/>
-      <c r="F100" s="54"/>
-      <c r="G100" s="55"/>
-      <c r="H100" s="55"/>
-      <c r="I100" s="55"/>
-      <c r="J100" s="55"/>
-      <c r="K100" s="55"/>
-      <c r="L100" s="55"/>
+    <row r="100" ht="31.5" customHeight="1">
+      <c r="A100" s="14"/>
+      <c r="B100" s="55"/>
+      <c r="C100" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="D100" s="17"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="19"/>
+      <c r="G100" s="20"/>
+      <c r="H100" s="20"/>
+      <c r="I100" s="20"/>
+      <c r="J100" s="20"/>
+      <c r="K100" s="20"/>
+      <c r="L100" s="20"/>
       <c r="M100" s="7"/>
       <c r="N100" s="7"/>
       <c r="O100" s="7"/>
@@ -4358,18 +4438,22 @@
       <c r="Z100" s="7"/>
     </row>
     <row r="101" ht="24.75" customHeight="1">
-      <c r="A101" s="52"/>
-      <c r="B101" s="31"/>
-      <c r="C101" s="31"/>
-      <c r="D101" s="53"/>
-      <c r="E101" s="51"/>
-      <c r="F101" s="54"/>
-      <c r="G101" s="55"/>
-      <c r="H101" s="55"/>
-      <c r="I101" s="55"/>
-      <c r="J101" s="55"/>
-      <c r="K101" s="55"/>
-      <c r="L101" s="55"/>
+      <c r="A101" s="14"/>
+      <c r="B101" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C101" s="16"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="19">
+        <v>2.900000000000001</v>
+      </c>
+      <c r="G101" s="20"/>
+      <c r="H101" s="20"/>
+      <c r="I101" s="20"/>
+      <c r="J101" s="20"/>
+      <c r="K101" s="20"/>
+      <c r="L101" s="20"/>
       <c r="M101" s="7"/>
       <c r="N101" s="7"/>
       <c r="O101" s="7"/>
@@ -4385,19 +4469,23 @@
       <c r="Y101" s="7"/>
       <c r="Z101" s="7"/>
     </row>
-    <row r="102" ht="24.75" customHeight="1">
-      <c r="A102" s="52"/>
-      <c r="B102" s="31"/>
-      <c r="C102" s="31"/>
-      <c r="D102" s="53"/>
-      <c r="E102" s="51"/>
-      <c r="F102" s="54"/>
-      <c r="G102" s="55"/>
-      <c r="H102" s="55"/>
-      <c r="I102" s="55"/>
-      <c r="J102" s="55"/>
-      <c r="K102" s="55"/>
-      <c r="L102" s="55"/>
+    <row r="102" ht="31.5" customHeight="1">
+      <c r="A102" s="14"/>
+      <c r="B102" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C102" s="16"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="19">
+        <v>2.1</v>
+      </c>
+      <c r="G102" s="20"/>
+      <c r="H102" s="20"/>
+      <c r="I102" s="20"/>
+      <c r="J102" s="20"/>
+      <c r="K102" s="20"/>
+      <c r="L102" s="20"/>
       <c r="M102" s="7"/>
       <c r="N102" s="7"/>
       <c r="O102" s="7"/>
@@ -4414,18 +4502,24 @@
       <c r="Z102" s="7"/>
     </row>
     <row r="103" ht="24.75" customHeight="1">
-      <c r="A103" s="52"/>
-      <c r="B103" s="31"/>
-      <c r="C103" s="31"/>
-      <c r="D103" s="53"/>
-      <c r="E103" s="51"/>
-      <c r="F103" s="54"/>
-      <c r="G103" s="55"/>
-      <c r="H103" s="55"/>
-      <c r="I103" s="55"/>
-      <c r="J103" s="55"/>
-      <c r="K103" s="55"/>
-      <c r="L103" s="55"/>
+      <c r="A103" s="14"/>
+      <c r="B103" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C103" s="16"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="19">
+        <v>2.12</v>
+      </c>
+      <c r="G103" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H103" s="20"/>
+      <c r="I103" s="20"/>
+      <c r="J103" s="20"/>
+      <c r="K103" s="20"/>
+      <c r="L103" s="20"/>
       <c r="M103" s="7"/>
       <c r="N103" s="7"/>
       <c r="O103" s="7"/>
@@ -4442,18 +4536,18 @@
       <c r="Z103" s="7"/>
     </row>
     <row r="104" ht="24.75" customHeight="1">
-      <c r="A104" s="52"/>
+      <c r="A104" s="57"/>
       <c r="B104" s="31"/>
       <c r="C104" s="31"/>
-      <c r="D104" s="53"/>
-      <c r="E104" s="51"/>
-      <c r="F104" s="54"/>
-      <c r="G104" s="55"/>
-      <c r="H104" s="55"/>
-      <c r="I104" s="55"/>
-      <c r="J104" s="55"/>
-      <c r="K104" s="55"/>
-      <c r="L104" s="55"/>
+      <c r="D104" s="58"/>
+      <c r="E104" s="54"/>
+      <c r="F104" s="59"/>
+      <c r="G104" s="60"/>
+      <c r="H104" s="60"/>
+      <c r="I104" s="60"/>
+      <c r="J104" s="60"/>
+      <c r="K104" s="60"/>
+      <c r="L104" s="60"/>
       <c r="M104" s="7"/>
       <c r="N104" s="7"/>
       <c r="O104" s="7"/>
@@ -4470,18 +4564,18 @@
       <c r="Z104" s="7"/>
     </row>
     <row r="105" ht="24.75" customHeight="1">
-      <c r="A105" s="52"/>
+      <c r="A105" s="57"/>
       <c r="B105" s="31"/>
       <c r="C105" s="31"/>
-      <c r="D105" s="53"/>
-      <c r="E105" s="51"/>
-      <c r="F105" s="54"/>
-      <c r="G105" s="55"/>
-      <c r="H105" s="55"/>
-      <c r="I105" s="55"/>
-      <c r="J105" s="55"/>
-      <c r="K105" s="55"/>
-      <c r="L105" s="55"/>
+      <c r="D105" s="58"/>
+      <c r="E105" s="54"/>
+      <c r="F105" s="59"/>
+      <c r="G105" s="60"/>
+      <c r="H105" s="60"/>
+      <c r="I105" s="60"/>
+      <c r="J105" s="60"/>
+      <c r="K105" s="60"/>
+      <c r="L105" s="60"/>
       <c r="M105" s="7"/>
       <c r="N105" s="7"/>
       <c r="O105" s="7"/>
@@ -4498,18 +4592,18 @@
       <c r="Z105" s="7"/>
     </row>
     <row r="106" ht="24.75" customHeight="1">
-      <c r="A106" s="52"/>
+      <c r="A106" s="57"/>
       <c r="B106" s="31"/>
       <c r="C106" s="31"/>
-      <c r="D106" s="53"/>
-      <c r="E106" s="51"/>
-      <c r="F106" s="54"/>
-      <c r="G106" s="55"/>
-      <c r="H106" s="55"/>
-      <c r="I106" s="55"/>
-      <c r="J106" s="55"/>
-      <c r="K106" s="55"/>
-      <c r="L106" s="55"/>
+      <c r="D106" s="58"/>
+      <c r="E106" s="54"/>
+      <c r="F106" s="59"/>
+      <c r="G106" s="60"/>
+      <c r="H106" s="60"/>
+      <c r="I106" s="60"/>
+      <c r="J106" s="60"/>
+      <c r="K106" s="60"/>
+      <c r="L106" s="60"/>
       <c r="M106" s="7"/>
       <c r="N106" s="7"/>
       <c r="O106" s="7"/>
@@ -4526,18 +4620,18 @@
       <c r="Z106" s="7"/>
     </row>
     <row r="107" ht="24.75" customHeight="1">
-      <c r="A107" s="52"/>
+      <c r="A107" s="57"/>
       <c r="B107" s="31"/>
       <c r="C107" s="31"/>
-      <c r="D107" s="53"/>
-      <c r="E107" s="51"/>
-      <c r="F107" s="54"/>
-      <c r="G107" s="55"/>
-      <c r="H107" s="55"/>
-      <c r="I107" s="55"/>
-      <c r="J107" s="55"/>
-      <c r="K107" s="55"/>
-      <c r="L107" s="55"/>
+      <c r="D107" s="58"/>
+      <c r="E107" s="54"/>
+      <c r="F107" s="59"/>
+      <c r="G107" s="60"/>
+      <c r="H107" s="60"/>
+      <c r="I107" s="60"/>
+      <c r="J107" s="60"/>
+      <c r="K107" s="60"/>
+      <c r="L107" s="60"/>
       <c r="M107" s="7"/>
       <c r="N107" s="7"/>
       <c r="O107" s="7"/>
@@ -4554,18 +4648,18 @@
       <c r="Z107" s="7"/>
     </row>
     <row r="108" ht="24.75" customHeight="1">
-      <c r="A108" s="52"/>
+      <c r="A108" s="57"/>
       <c r="B108" s="31"/>
       <c r="C108" s="31"/>
-      <c r="D108" s="53"/>
-      <c r="E108" s="51"/>
-      <c r="F108" s="54"/>
-      <c r="G108" s="55"/>
-      <c r="H108" s="55"/>
-      <c r="I108" s="55"/>
-      <c r="J108" s="55"/>
-      <c r="K108" s="55"/>
-      <c r="L108" s="55"/>
+      <c r="D108" s="58"/>
+      <c r="E108" s="54"/>
+      <c r="F108" s="59"/>
+      <c r="G108" s="60"/>
+      <c r="H108" s="60"/>
+      <c r="I108" s="60"/>
+      <c r="J108" s="60"/>
+      <c r="K108" s="60"/>
+      <c r="L108" s="60"/>
       <c r="M108" s="7"/>
       <c r="N108" s="7"/>
       <c r="O108" s="7"/>
@@ -4582,18 +4676,18 @@
       <c r="Z108" s="7"/>
     </row>
     <row r="109" ht="24.75" customHeight="1">
-      <c r="A109" s="52"/>
+      <c r="A109" s="57"/>
       <c r="B109" s="31"/>
       <c r="C109" s="31"/>
-      <c r="D109" s="53"/>
-      <c r="E109" s="51"/>
-      <c r="F109" s="54"/>
-      <c r="G109" s="55"/>
-      <c r="H109" s="55"/>
-      <c r="I109" s="55"/>
-      <c r="J109" s="55"/>
-      <c r="K109" s="55"/>
-      <c r="L109" s="55"/>
+      <c r="D109" s="58"/>
+      <c r="E109" s="54"/>
+      <c r="F109" s="59"/>
+      <c r="G109" s="60"/>
+      <c r="H109" s="60"/>
+      <c r="I109" s="60"/>
+      <c r="J109" s="60"/>
+      <c r="K109" s="60"/>
+      <c r="L109" s="60"/>
       <c r="M109" s="7"/>
       <c r="N109" s="7"/>
       <c r="O109" s="7"/>
@@ -4610,18 +4704,18 @@
       <c r="Z109" s="7"/>
     </row>
     <row r="110" ht="24.75" customHeight="1">
-      <c r="A110" s="52"/>
+      <c r="A110" s="57"/>
       <c r="B110" s="31"/>
       <c r="C110" s="31"/>
-      <c r="D110" s="53"/>
-      <c r="E110" s="51"/>
-      <c r="F110" s="54"/>
-      <c r="G110" s="55"/>
-      <c r="H110" s="55"/>
-      <c r="I110" s="55"/>
-      <c r="J110" s="55"/>
-      <c r="K110" s="55"/>
-      <c r="L110" s="55"/>
+      <c r="D110" s="58"/>
+      <c r="E110" s="54"/>
+      <c r="F110" s="59"/>
+      <c r="G110" s="60"/>
+      <c r="H110" s="60"/>
+      <c r="I110" s="60"/>
+      <c r="J110" s="60"/>
+      <c r="K110" s="60"/>
+      <c r="L110" s="60"/>
       <c r="M110" s="7"/>
       <c r="N110" s="7"/>
       <c r="O110" s="7"/>
@@ -4638,18 +4732,18 @@
       <c r="Z110" s="7"/>
     </row>
     <row r="111" ht="24.75" customHeight="1">
-      <c r="A111" s="52"/>
+      <c r="A111" s="57"/>
       <c r="B111" s="31"/>
       <c r="C111" s="31"/>
-      <c r="D111" s="53"/>
-      <c r="E111" s="51"/>
-      <c r="F111" s="54"/>
-      <c r="G111" s="55"/>
-      <c r="H111" s="55"/>
-      <c r="I111" s="55"/>
-      <c r="J111" s="55"/>
-      <c r="K111" s="55"/>
-      <c r="L111" s="55"/>
+      <c r="D111" s="58"/>
+      <c r="E111" s="54"/>
+      <c r="F111" s="59"/>
+      <c r="G111" s="60"/>
+      <c r="H111" s="60"/>
+      <c r="I111" s="60"/>
+      <c r="J111" s="60"/>
+      <c r="K111" s="60"/>
+      <c r="L111" s="60"/>
       <c r="M111" s="7"/>
       <c r="N111" s="7"/>
       <c r="O111" s="7"/>
@@ -4666,18 +4760,18 @@
       <c r="Z111" s="7"/>
     </row>
     <row r="112" ht="24.75" customHeight="1">
-      <c r="A112" s="52"/>
+      <c r="A112" s="57"/>
       <c r="B112" s="31"/>
       <c r="C112" s="31"/>
-      <c r="D112" s="53"/>
-      <c r="E112" s="51"/>
-      <c r="F112" s="54"/>
-      <c r="G112" s="55"/>
-      <c r="H112" s="55"/>
-      <c r="I112" s="55"/>
-      <c r="J112" s="55"/>
-      <c r="K112" s="55"/>
-      <c r="L112" s="55"/>
+      <c r="D112" s="58"/>
+      <c r="E112" s="54"/>
+      <c r="F112" s="59"/>
+      <c r="G112" s="60"/>
+      <c r="H112" s="60"/>
+      <c r="I112" s="60"/>
+      <c r="J112" s="60"/>
+      <c r="K112" s="60"/>
+      <c r="L112" s="60"/>
       <c r="M112" s="7"/>
       <c r="N112" s="7"/>
       <c r="O112" s="7"/>
@@ -4694,18 +4788,18 @@
       <c r="Z112" s="7"/>
     </row>
     <row r="113" ht="24.75" customHeight="1">
-      <c r="A113" s="52"/>
+      <c r="A113" s="57"/>
       <c r="B113" s="31"/>
       <c r="C113" s="31"/>
-      <c r="D113" s="53"/>
-      <c r="E113" s="51"/>
-      <c r="F113" s="54"/>
-      <c r="G113" s="55"/>
-      <c r="H113" s="55"/>
-      <c r="I113" s="55"/>
-      <c r="J113" s="55"/>
-      <c r="K113" s="55"/>
-      <c r="L113" s="55"/>
+      <c r="D113" s="58"/>
+      <c r="E113" s="54"/>
+      <c r="F113" s="59"/>
+      <c r="G113" s="60"/>
+      <c r="H113" s="60"/>
+      <c r="I113" s="60"/>
+      <c r="J113" s="60"/>
+      <c r="K113" s="60"/>
+      <c r="L113" s="60"/>
       <c r="M113" s="7"/>
       <c r="N113" s="7"/>
       <c r="O113" s="7"/>
@@ -4722,18 +4816,18 @@
       <c r="Z113" s="7"/>
     </row>
     <row r="114" ht="24.75" customHeight="1">
-      <c r="A114" s="52"/>
+      <c r="A114" s="57"/>
       <c r="B114" s="31"/>
       <c r="C114" s="31"/>
-      <c r="D114" s="53"/>
-      <c r="E114" s="51"/>
-      <c r="F114" s="54"/>
-      <c r="G114" s="55"/>
-      <c r="H114" s="55"/>
-      <c r="I114" s="55"/>
-      <c r="J114" s="55"/>
-      <c r="K114" s="55"/>
-      <c r="L114" s="55"/>
+      <c r="D114" s="58"/>
+      <c r="E114" s="54"/>
+      <c r="F114" s="59"/>
+      <c r="G114" s="60"/>
+      <c r="H114" s="60"/>
+      <c r="I114" s="60"/>
+      <c r="J114" s="60"/>
+      <c r="K114" s="60"/>
+      <c r="L114" s="60"/>
       <c r="M114" s="7"/>
       <c r="N114" s="7"/>
       <c r="O114" s="7"/>
@@ -4750,18 +4844,18 @@
       <c r="Z114" s="7"/>
     </row>
     <row r="115" ht="24.75" customHeight="1">
-      <c r="A115" s="52"/>
+      <c r="A115" s="57"/>
       <c r="B115" s="31"/>
       <c r="C115" s="31"/>
-      <c r="D115" s="53"/>
-      <c r="E115" s="51"/>
-      <c r="F115" s="54"/>
-      <c r="G115" s="55"/>
-      <c r="H115" s="55"/>
-      <c r="I115" s="55"/>
-      <c r="J115" s="55"/>
-      <c r="K115" s="55"/>
-      <c r="L115" s="55"/>
+      <c r="D115" s="58"/>
+      <c r="E115" s="54"/>
+      <c r="F115" s="59"/>
+      <c r="G115" s="60"/>
+      <c r="H115" s="60"/>
+      <c r="I115" s="60"/>
+      <c r="J115" s="60"/>
+      <c r="K115" s="60"/>
+      <c r="L115" s="60"/>
       <c r="M115" s="7"/>
       <c r="N115" s="7"/>
       <c r="O115" s="7"/>
@@ -4778,18 +4872,18 @@
       <c r="Z115" s="7"/>
     </row>
     <row r="116" ht="24.75" customHeight="1">
-      <c r="A116" s="52"/>
+      <c r="A116" s="57"/>
       <c r="B116" s="31"/>
       <c r="C116" s="31"/>
-      <c r="D116" s="53"/>
-      <c r="E116" s="51"/>
-      <c r="F116" s="54"/>
-      <c r="G116" s="55"/>
-      <c r="H116" s="55"/>
-      <c r="I116" s="55"/>
-      <c r="J116" s="55"/>
-      <c r="K116" s="55"/>
-      <c r="L116" s="55"/>
+      <c r="D116" s="58"/>
+      <c r="E116" s="54"/>
+      <c r="F116" s="59"/>
+      <c r="G116" s="60"/>
+      <c r="H116" s="60"/>
+      <c r="I116" s="60"/>
+      <c r="J116" s="60"/>
+      <c r="K116" s="60"/>
+      <c r="L116" s="60"/>
       <c r="M116" s="7"/>
       <c r="N116" s="7"/>
       <c r="O116" s="7"/>
@@ -4806,18 +4900,18 @@
       <c r="Z116" s="7"/>
     </row>
     <row r="117" ht="24.75" customHeight="1">
-      <c r="A117" s="52"/>
+      <c r="A117" s="57"/>
       <c r="B117" s="31"/>
       <c r="C117" s="31"/>
-      <c r="D117" s="53"/>
-      <c r="E117" s="51"/>
-      <c r="F117" s="54"/>
-      <c r="G117" s="55"/>
-      <c r="H117" s="55"/>
-      <c r="I117" s="55"/>
-      <c r="J117" s="55"/>
-      <c r="K117" s="55"/>
-      <c r="L117" s="55"/>
+      <c r="D117" s="58"/>
+      <c r="E117" s="54"/>
+      <c r="F117" s="59"/>
+      <c r="G117" s="60"/>
+      <c r="H117" s="60"/>
+      <c r="I117" s="60"/>
+      <c r="J117" s="60"/>
+      <c r="K117" s="60"/>
+      <c r="L117" s="60"/>
       <c r="M117" s="7"/>
       <c r="N117" s="7"/>
       <c r="O117" s="7"/>
@@ -4834,18 +4928,18 @@
       <c r="Z117" s="7"/>
     </row>
     <row r="118" ht="24.75" customHeight="1">
-      <c r="A118" s="52"/>
+      <c r="A118" s="57"/>
       <c r="B118" s="31"/>
       <c r="C118" s="31"/>
-      <c r="D118" s="53"/>
-      <c r="E118" s="51"/>
-      <c r="F118" s="54"/>
-      <c r="G118" s="55"/>
-      <c r="H118" s="55"/>
-      <c r="I118" s="55"/>
-      <c r="J118" s="55"/>
-      <c r="K118" s="55"/>
-      <c r="L118" s="55"/>
+      <c r="D118" s="58"/>
+      <c r="E118" s="54"/>
+      <c r="F118" s="59"/>
+      <c r="G118" s="60"/>
+      <c r="H118" s="60"/>
+      <c r="I118" s="60"/>
+      <c r="J118" s="60"/>
+      <c r="K118" s="60"/>
+      <c r="L118" s="60"/>
       <c r="M118" s="7"/>
       <c r="N118" s="7"/>
       <c r="O118" s="7"/>
@@ -4862,18 +4956,18 @@
       <c r="Z118" s="7"/>
     </row>
     <row r="119" ht="24.75" customHeight="1">
-      <c r="A119" s="52"/>
+      <c r="A119" s="57"/>
       <c r="B119" s="31"/>
       <c r="C119" s="31"/>
-      <c r="D119" s="53"/>
-      <c r="E119" s="51"/>
-      <c r="F119" s="54"/>
-      <c r="G119" s="55"/>
-      <c r="H119" s="55"/>
-      <c r="I119" s="55"/>
-      <c r="J119" s="55"/>
-      <c r="K119" s="55"/>
-      <c r="L119" s="55"/>
+      <c r="D119" s="58"/>
+      <c r="E119" s="54"/>
+      <c r="F119" s="59"/>
+      <c r="G119" s="60"/>
+      <c r="H119" s="60"/>
+      <c r="I119" s="60"/>
+      <c r="J119" s="60"/>
+      <c r="K119" s="60"/>
+      <c r="L119" s="60"/>
       <c r="M119" s="7"/>
       <c r="N119" s="7"/>
       <c r="O119" s="7"/>
@@ -4890,18 +4984,18 @@
       <c r="Z119" s="7"/>
     </row>
     <row r="120" ht="24.75" customHeight="1">
-      <c r="A120" s="52"/>
+      <c r="A120" s="57"/>
       <c r="B120" s="31"/>
       <c r="C120" s="31"/>
-      <c r="D120" s="53"/>
-      <c r="E120" s="51"/>
-      <c r="F120" s="54"/>
-      <c r="G120" s="55"/>
-      <c r="H120" s="55"/>
-      <c r="I120" s="55"/>
-      <c r="J120" s="55"/>
-      <c r="K120" s="55"/>
-      <c r="L120" s="55"/>
+      <c r="D120" s="58"/>
+      <c r="E120" s="54"/>
+      <c r="F120" s="59"/>
+      <c r="G120" s="60"/>
+      <c r="H120" s="60"/>
+      <c r="I120" s="60"/>
+      <c r="J120" s="60"/>
+      <c r="K120" s="60"/>
+      <c r="L120" s="60"/>
       <c r="M120" s="7"/>
       <c r="N120" s="7"/>
       <c r="O120" s="7"/>
@@ -4917,19 +5011,19 @@
       <c r="Y120" s="7"/>
       <c r="Z120" s="7"/>
     </row>
-    <row r="121" ht="26.25" customHeight="1">
-      <c r="A121" s="56"/>
-      <c r="B121" s="57"/>
-      <c r="C121" s="57"/>
+    <row r="121" ht="24.75" customHeight="1">
+      <c r="A121" s="57"/>
+      <c r="B121" s="31"/>
+      <c r="C121" s="31"/>
       <c r="D121" s="58"/>
-      <c r="E121" s="59"/>
-      <c r="F121" s="60"/>
-      <c r="G121" s="61"/>
-      <c r="H121" s="61"/>
-      <c r="I121" s="61"/>
-      <c r="J121" s="61"/>
-      <c r="K121" s="61"/>
-      <c r="L121" s="61"/>
+      <c r="E121" s="54"/>
+      <c r="F121" s="59"/>
+      <c r="G121" s="60"/>
+      <c r="H121" s="60"/>
+      <c r="I121" s="60"/>
+      <c r="J121" s="60"/>
+      <c r="K121" s="60"/>
+      <c r="L121" s="60"/>
       <c r="M121" s="7"/>
       <c r="N121" s="7"/>
       <c r="O121" s="7"/>
@@ -4945,19 +5039,19 @@
       <c r="Y121" s="7"/>
       <c r="Z121" s="7"/>
     </row>
-    <row r="122" ht="28.5" customHeight="1">
-      <c r="A122" s="62"/>
-      <c r="B122" s="63"/>
-      <c r="C122" s="63"/>
-      <c r="D122" s="64"/>
-      <c r="E122" s="65"/>
-      <c r="F122" s="66"/>
-      <c r="G122" s="67"/>
-      <c r="H122" s="67"/>
-      <c r="I122" s="67"/>
-      <c r="J122" s="67"/>
-      <c r="K122" s="67"/>
-      <c r="L122" s="67"/>
+    <row r="122" ht="24.75" customHeight="1">
+      <c r="A122" s="57"/>
+      <c r="B122" s="31"/>
+      <c r="C122" s="31"/>
+      <c r="D122" s="58"/>
+      <c r="E122" s="54"/>
+      <c r="F122" s="59"/>
+      <c r="G122" s="60"/>
+      <c r="H122" s="60"/>
+      <c r="I122" s="60"/>
+      <c r="J122" s="60"/>
+      <c r="K122" s="60"/>
+      <c r="L122" s="60"/>
       <c r="M122" s="7"/>
       <c r="N122" s="7"/>
       <c r="O122" s="7"/>
@@ -4973,29 +5067,19 @@
       <c r="Y122" s="7"/>
       <c r="Z122" s="7"/>
     </row>
-    <row r="123" ht="26.25" customHeight="1">
-      <c r="A123" s="68"/>
-      <c r="B123" s="69"/>
-      <c r="C123" s="69"/>
-      <c r="D123" s="70"/>
-      <c r="E123" s="71"/>
-      <c r="F123" s="72"/>
-      <c r="G123" s="73" t="s">
-        <v>96</v>
-      </c>
-      <c r="H123" s="74"/>
-      <c r="I123" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="J123" s="73" t="s">
-        <v>98</v>
-      </c>
-      <c r="K123" s="73" t="s">
-        <v>99</v>
-      </c>
-      <c r="L123" s="73" t="s">
-        <v>100</v>
-      </c>
+    <row r="123" ht="24.75" customHeight="1">
+      <c r="A123" s="57"/>
+      <c r="B123" s="31"/>
+      <c r="C123" s="31"/>
+      <c r="D123" s="58"/>
+      <c r="E123" s="54"/>
+      <c r="F123" s="59"/>
+      <c r="G123" s="60"/>
+      <c r="H123" s="60"/>
+      <c r="I123" s="60"/>
+      <c r="J123" s="60"/>
+      <c r="K123" s="60"/>
+      <c r="L123" s="60"/>
       <c r="M123" s="7"/>
       <c r="N123" s="7"/>
       <c r="O123" s="7"/>
@@ -5011,25 +5095,19 @@
       <c r="Y123" s="7"/>
       <c r="Z123" s="7"/>
     </row>
-    <row r="124" ht="43.5" customHeight="1">
-      <c r="A124" s="75"/>
-      <c r="B124" s="76"/>
-      <c r="C124" s="76"/>
-      <c r="D124" s="77"/>
-      <c r="E124" s="78"/>
-      <c r="F124" s="79"/>
-      <c r="G124" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="H124" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="I124" s="80" t="s">
-        <v>102</v>
-      </c>
-      <c r="J124" s="81"/>
-      <c r="K124" s="81"/>
-      <c r="L124" s="81"/>
+    <row r="124" ht="24.75" customHeight="1">
+      <c r="A124" s="57"/>
+      <c r="B124" s="31"/>
+      <c r="C124" s="31"/>
+      <c r="D124" s="58"/>
+      <c r="E124" s="54"/>
+      <c r="F124" s="59"/>
+      <c r="G124" s="60"/>
+      <c r="H124" s="60"/>
+      <c r="I124" s="60"/>
+      <c r="J124" s="60"/>
+      <c r="K124" s="60"/>
+      <c r="L124" s="60"/>
       <c r="M124" s="7"/>
       <c r="N124" s="7"/>
       <c r="O124" s="7"/>
@@ -5045,25 +5123,19 @@
       <c r="Y124" s="7"/>
       <c r="Z124" s="7"/>
     </row>
-    <row r="125" ht="43.5" customHeight="1">
-      <c r="A125" s="75"/>
-      <c r="B125" s="76"/>
-      <c r="C125" s="76"/>
-      <c r="D125" s="77"/>
-      <c r="E125" s="78"/>
-      <c r="F125" s="79"/>
-      <c r="G125" s="80" t="s">
-        <v>103</v>
-      </c>
-      <c r="H125" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="I125" s="80" t="s">
-        <v>105</v>
-      </c>
-      <c r="J125" s="81"/>
-      <c r="K125" s="81"/>
-      <c r="L125" s="81"/>
+    <row r="125" ht="24.75" customHeight="1">
+      <c r="A125" s="57"/>
+      <c r="B125" s="31"/>
+      <c r="C125" s="31"/>
+      <c r="D125" s="58"/>
+      <c r="E125" s="54"/>
+      <c r="F125" s="59"/>
+      <c r="G125" s="60"/>
+      <c r="H125" s="60"/>
+      <c r="I125" s="60"/>
+      <c r="J125" s="60"/>
+      <c r="K125" s="60"/>
+      <c r="L125" s="60"/>
       <c r="M125" s="7"/>
       <c r="N125" s="7"/>
       <c r="O125" s="7"/>
@@ -5080,20 +5152,18 @@
       <c r="Z125" s="7"/>
     </row>
     <row r="126" ht="24.75" customHeight="1">
-      <c r="A126" s="75"/>
-      <c r="B126" s="76"/>
-      <c r="C126" s="76"/>
-      <c r="D126" s="77"/>
-      <c r="E126" s="78"/>
-      <c r="F126" s="79"/>
-      <c r="G126" s="80" t="s">
-        <v>106</v>
-      </c>
-      <c r="H126" s="81"/>
-      <c r="I126" s="81"/>
-      <c r="J126" s="81"/>
-      <c r="K126" s="81"/>
-      <c r="L126" s="81"/>
+      <c r="A126" s="57"/>
+      <c r="B126" s="31"/>
+      <c r="C126" s="31"/>
+      <c r="D126" s="58"/>
+      <c r="E126" s="54"/>
+      <c r="F126" s="59"/>
+      <c r="G126" s="60"/>
+      <c r="H126" s="60"/>
+      <c r="I126" s="60"/>
+      <c r="J126" s="60"/>
+      <c r="K126" s="60"/>
+      <c r="L126" s="60"/>
       <c r="M126" s="7"/>
       <c r="N126" s="7"/>
       <c r="O126" s="7"/>
@@ -5109,19 +5179,19 @@
       <c r="Y126" s="7"/>
       <c r="Z126" s="7"/>
     </row>
-    <row r="127" ht="19.5" customHeight="1">
-      <c r="A127" s="7"/>
-      <c r="B127" s="7"/>
-      <c r="C127" s="7"/>
-      <c r="D127" s="7"/>
-      <c r="E127" s="7"/>
-      <c r="F127" s="7"/>
-      <c r="G127" s="7"/>
-      <c r="H127" s="7"/>
-      <c r="I127" s="7"/>
-      <c r="J127" s="7"/>
-      <c r="K127" s="7"/>
-      <c r="L127" s="7"/>
+    <row r="127" ht="24.75" customHeight="1">
+      <c r="A127" s="57"/>
+      <c r="B127" s="31"/>
+      <c r="C127" s="31"/>
+      <c r="D127" s="58"/>
+      <c r="E127" s="54"/>
+      <c r="F127" s="59"/>
+      <c r="G127" s="60"/>
+      <c r="H127" s="60"/>
+      <c r="I127" s="60"/>
+      <c r="J127" s="60"/>
+      <c r="K127" s="60"/>
+      <c r="L127" s="60"/>
       <c r="M127" s="7"/>
       <c r="N127" s="7"/>
       <c r="O127" s="7"/>
@@ -5137,19 +5207,19 @@
       <c r="Y127" s="7"/>
       <c r="Z127" s="7"/>
     </row>
-    <row r="128" ht="19.5" customHeight="1">
-      <c r="A128" s="7"/>
-      <c r="B128" s="7"/>
-      <c r="C128" s="7"/>
-      <c r="D128" s="7"/>
-      <c r="E128" s="7"/>
-      <c r="F128" s="7"/>
-      <c r="G128" s="7"/>
-      <c r="H128" s="7"/>
-      <c r="I128" s="7"/>
-      <c r="J128" s="7"/>
-      <c r="K128" s="7"/>
-      <c r="L128" s="7"/>
+    <row r="128" ht="24.75" customHeight="1">
+      <c r="A128" s="57"/>
+      <c r="B128" s="31"/>
+      <c r="C128" s="31"/>
+      <c r="D128" s="58"/>
+      <c r="E128" s="54"/>
+      <c r="F128" s="59"/>
+      <c r="G128" s="60"/>
+      <c r="H128" s="60"/>
+      <c r="I128" s="60"/>
+      <c r="J128" s="60"/>
+      <c r="K128" s="60"/>
+      <c r="L128" s="60"/>
       <c r="M128" s="7"/>
       <c r="N128" s="7"/>
       <c r="O128" s="7"/>
@@ -5165,19 +5235,19 @@
       <c r="Y128" s="7"/>
       <c r="Z128" s="7"/>
     </row>
-    <row r="129" ht="19.5" customHeight="1">
-      <c r="A129" s="7"/>
-      <c r="B129" s="7"/>
-      <c r="C129" s="7"/>
-      <c r="D129" s="7"/>
-      <c r="E129" s="7"/>
-      <c r="F129" s="7"/>
-      <c r="G129" s="7"/>
-      <c r="H129" s="7"/>
-      <c r="I129" s="7"/>
-      <c r="J129" s="7"/>
-      <c r="K129" s="7"/>
-      <c r="L129" s="7"/>
+    <row r="129" ht="26.25" customHeight="1">
+      <c r="A129" s="61"/>
+      <c r="B129" s="62"/>
+      <c r="C129" s="62"/>
+      <c r="D129" s="63"/>
+      <c r="E129" s="64"/>
+      <c r="F129" s="65"/>
+      <c r="G129" s="66"/>
+      <c r="H129" s="66"/>
+      <c r="I129" s="66"/>
+      <c r="J129" s="66"/>
+      <c r="K129" s="66"/>
+      <c r="L129" s="66"/>
       <c r="M129" s="7"/>
       <c r="N129" s="7"/>
       <c r="O129" s="7"/>
@@ -5193,19 +5263,19 @@
       <c r="Y129" s="7"/>
       <c r="Z129" s="7"/>
     </row>
-    <row r="130" ht="19.5" customHeight="1">
-      <c r="A130" s="7"/>
-      <c r="B130" s="7"/>
-      <c r="C130" s="7"/>
-      <c r="D130" s="7"/>
-      <c r="E130" s="7"/>
-      <c r="F130" s="7"/>
-      <c r="G130" s="7"/>
-      <c r="H130" s="7"/>
-      <c r="I130" s="7"/>
-      <c r="J130" s="7"/>
-      <c r="K130" s="7"/>
-      <c r="L130" s="7"/>
+    <row r="130" ht="28.5" customHeight="1">
+      <c r="A130" s="67"/>
+      <c r="B130" s="68"/>
+      <c r="C130" s="68"/>
+      <c r="D130" s="69"/>
+      <c r="E130" s="70"/>
+      <c r="F130" s="71"/>
+      <c r="G130" s="72"/>
+      <c r="H130" s="72"/>
+      <c r="I130" s="72"/>
+      <c r="J130" s="72"/>
+      <c r="K130" s="72"/>
+      <c r="L130" s="72"/>
       <c r="M130" s="7"/>
       <c r="N130" s="7"/>
       <c r="O130" s="7"/>
@@ -5221,19 +5291,29 @@
       <c r="Y130" s="7"/>
       <c r="Z130" s="7"/>
     </row>
-    <row r="131" ht="19.5" customHeight="1">
-      <c r="A131" s="7"/>
-      <c r="B131" s="7"/>
-      <c r="C131" s="7"/>
-      <c r="D131" s="7"/>
-      <c r="E131" s="7"/>
-      <c r="F131" s="7"/>
-      <c r="G131" s="7"/>
-      <c r="H131" s="7"/>
-      <c r="I131" s="7"/>
-      <c r="J131" s="7"/>
-      <c r="K131" s="7"/>
-      <c r="L131" s="7"/>
+    <row r="131" ht="26.25" customHeight="1">
+      <c r="A131" s="73"/>
+      <c r="B131" s="74"/>
+      <c r="C131" s="74"/>
+      <c r="D131" s="75"/>
+      <c r="E131" s="76"/>
+      <c r="F131" s="77"/>
+      <c r="G131" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="H131" s="79"/>
+      <c r="I131" s="78" t="s">
+        <v>105</v>
+      </c>
+      <c r="J131" s="78" t="s">
+        <v>106</v>
+      </c>
+      <c r="K131" s="78" t="s">
+        <v>107</v>
+      </c>
+      <c r="L131" s="78" t="s">
+        <v>108</v>
+      </c>
       <c r="M131" s="7"/>
       <c r="N131" s="7"/>
       <c r="O131" s="7"/>
@@ -5249,19 +5329,25 @@
       <c r="Y131" s="7"/>
       <c r="Z131" s="7"/>
     </row>
-    <row r="132" ht="19.5" customHeight="1">
-      <c r="A132" s="7"/>
-      <c r="B132" s="7"/>
-      <c r="C132" s="7"/>
-      <c r="D132" s="7"/>
-      <c r="E132" s="7"/>
-      <c r="F132" s="7"/>
-      <c r="G132" s="7"/>
-      <c r="H132" s="7"/>
-      <c r="I132" s="7"/>
-      <c r="J132" s="7"/>
-      <c r="K132" s="7"/>
-      <c r="L132" s="7"/>
+    <row r="132" ht="43.5" customHeight="1">
+      <c r="A132" s="80"/>
+      <c r="B132" s="81"/>
+      <c r="C132" s="81"/>
+      <c r="D132" s="82"/>
+      <c r="E132" s="83"/>
+      <c r="F132" s="84"/>
+      <c r="G132" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="H132" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="I132" s="85" t="s">
+        <v>110</v>
+      </c>
+      <c r="J132" s="86"/>
+      <c r="K132" s="86"/>
+      <c r="L132" s="86"/>
       <c r="M132" s="7"/>
       <c r="N132" s="7"/>
       <c r="O132" s="7"/>
@@ -5277,19 +5363,25 @@
       <c r="Y132" s="7"/>
       <c r="Z132" s="7"/>
     </row>
-    <row r="133" ht="19.5" customHeight="1">
-      <c r="A133" s="7"/>
-      <c r="B133" s="7"/>
-      <c r="C133" s="7"/>
-      <c r="D133" s="7"/>
-      <c r="E133" s="7"/>
-      <c r="F133" s="7"/>
-      <c r="G133" s="7"/>
-      <c r="H133" s="7"/>
-      <c r="I133" s="7"/>
-      <c r="J133" s="7"/>
-      <c r="K133" s="7"/>
-      <c r="L133" s="7"/>
+    <row r="133" ht="43.5" customHeight="1">
+      <c r="A133" s="80"/>
+      <c r="B133" s="81"/>
+      <c r="C133" s="81"/>
+      <c r="D133" s="82"/>
+      <c r="E133" s="83"/>
+      <c r="F133" s="84"/>
+      <c r="G133" s="85" t="s">
+        <v>111</v>
+      </c>
+      <c r="H133" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="I133" s="85" t="s">
+        <v>113</v>
+      </c>
+      <c r="J133" s="86"/>
+      <c r="K133" s="86"/>
+      <c r="L133" s="86"/>
       <c r="M133" s="7"/>
       <c r="N133" s="7"/>
       <c r="O133" s="7"/>
@@ -5305,19 +5397,21 @@
       <c r="Y133" s="7"/>
       <c r="Z133" s="7"/>
     </row>
-    <row r="134" ht="19.5" customHeight="1">
-      <c r="A134" s="7"/>
-      <c r="B134" s="7"/>
-      <c r="C134" s="7"/>
-      <c r="D134" s="7"/>
-      <c r="E134" s="7"/>
-      <c r="F134" s="7"/>
-      <c r="G134" s="7"/>
-      <c r="H134" s="7"/>
-      <c r="I134" s="7"/>
-      <c r="J134" s="7"/>
-      <c r="K134" s="7"/>
-      <c r="L134" s="7"/>
+    <row r="134" ht="24.75" customHeight="1">
+      <c r="A134" s="80"/>
+      <c r="B134" s="81"/>
+      <c r="C134" s="81"/>
+      <c r="D134" s="82"/>
+      <c r="E134" s="83"/>
+      <c r="F134" s="84"/>
+      <c r="G134" s="85" t="s">
+        <v>114</v>
+      </c>
+      <c r="H134" s="86"/>
+      <c r="I134" s="86"/>
+      <c r="J134" s="86"/>
+      <c r="K134" s="86"/>
+      <c r="L134" s="86"/>
       <c r="M134" s="7"/>
       <c r="N134" s="7"/>
       <c r="O134" s="7"/>
@@ -29609,6 +29703,230 @@
       <c r="Y1001" s="7"/>
       <c r="Z1001" s="7"/>
     </row>
+    <row r="1002" ht="19.5" customHeight="1">
+      <c r="A1002" s="7"/>
+      <c r="B1002" s="7"/>
+      <c r="C1002" s="7"/>
+      <c r="D1002" s="7"/>
+      <c r="E1002" s="7"/>
+      <c r="F1002" s="7"/>
+      <c r="G1002" s="7"/>
+      <c r="H1002" s="7"/>
+      <c r="I1002" s="7"/>
+      <c r="J1002" s="7"/>
+      <c r="K1002" s="7"/>
+      <c r="L1002" s="7"/>
+      <c r="M1002" s="7"/>
+      <c r="N1002" s="7"/>
+      <c r="O1002" s="7"/>
+      <c r="P1002" s="7"/>
+      <c r="Q1002" s="7"/>
+      <c r="R1002" s="7"/>
+      <c r="S1002" s="7"/>
+      <c r="T1002" s="7"/>
+      <c r="U1002" s="7"/>
+      <c r="V1002" s="7"/>
+      <c r="W1002" s="7"/>
+      <c r="X1002" s="7"/>
+      <c r="Y1002" s="7"/>
+      <c r="Z1002" s="7"/>
+    </row>
+    <row r="1003" ht="19.5" customHeight="1">
+      <c r="A1003" s="7"/>
+      <c r="B1003" s="7"/>
+      <c r="C1003" s="7"/>
+      <c r="D1003" s="7"/>
+      <c r="E1003" s="7"/>
+      <c r="F1003" s="7"/>
+      <c r="G1003" s="7"/>
+      <c r="H1003" s="7"/>
+      <c r="I1003" s="7"/>
+      <c r="J1003" s="7"/>
+      <c r="K1003" s="7"/>
+      <c r="L1003" s="7"/>
+      <c r="M1003" s="7"/>
+      <c r="N1003" s="7"/>
+      <c r="O1003" s="7"/>
+      <c r="P1003" s="7"/>
+      <c r="Q1003" s="7"/>
+      <c r="R1003" s="7"/>
+      <c r="S1003" s="7"/>
+      <c r="T1003" s="7"/>
+      <c r="U1003" s="7"/>
+      <c r="V1003" s="7"/>
+      <c r="W1003" s="7"/>
+      <c r="X1003" s="7"/>
+      <c r="Y1003" s="7"/>
+      <c r="Z1003" s="7"/>
+    </row>
+    <row r="1004" ht="19.5" customHeight="1">
+      <c r="A1004" s="7"/>
+      <c r="B1004" s="7"/>
+      <c r="C1004" s="7"/>
+      <c r="D1004" s="7"/>
+      <c r="E1004" s="7"/>
+      <c r="F1004" s="7"/>
+      <c r="G1004" s="7"/>
+      <c r="H1004" s="7"/>
+      <c r="I1004" s="7"/>
+      <c r="J1004" s="7"/>
+      <c r="K1004" s="7"/>
+      <c r="L1004" s="7"/>
+      <c r="M1004" s="7"/>
+      <c r="N1004" s="7"/>
+      <c r="O1004" s="7"/>
+      <c r="P1004" s="7"/>
+      <c r="Q1004" s="7"/>
+      <c r="R1004" s="7"/>
+      <c r="S1004" s="7"/>
+      <c r="T1004" s="7"/>
+      <c r="U1004" s="7"/>
+      <c r="V1004" s="7"/>
+      <c r="W1004" s="7"/>
+      <c r="X1004" s="7"/>
+      <c r="Y1004" s="7"/>
+      <c r="Z1004" s="7"/>
+    </row>
+    <row r="1005" ht="19.5" customHeight="1">
+      <c r="A1005" s="7"/>
+      <c r="B1005" s="7"/>
+      <c r="C1005" s="7"/>
+      <c r="D1005" s="7"/>
+      <c r="E1005" s="7"/>
+      <c r="F1005" s="7"/>
+      <c r="G1005" s="7"/>
+      <c r="H1005" s="7"/>
+      <c r="I1005" s="7"/>
+      <c r="J1005" s="7"/>
+      <c r="K1005" s="7"/>
+      <c r="L1005" s="7"/>
+      <c r="M1005" s="7"/>
+      <c r="N1005" s="7"/>
+      <c r="O1005" s="7"/>
+      <c r="P1005" s="7"/>
+      <c r="Q1005" s="7"/>
+      <c r="R1005" s="7"/>
+      <c r="S1005" s="7"/>
+      <c r="T1005" s="7"/>
+      <c r="U1005" s="7"/>
+      <c r="V1005" s="7"/>
+      <c r="W1005" s="7"/>
+      <c r="X1005" s="7"/>
+      <c r="Y1005" s="7"/>
+      <c r="Z1005" s="7"/>
+    </row>
+    <row r="1006" ht="19.5" customHeight="1">
+      <c r="A1006" s="7"/>
+      <c r="B1006" s="7"/>
+      <c r="C1006" s="7"/>
+      <c r="D1006" s="7"/>
+      <c r="E1006" s="7"/>
+      <c r="F1006" s="7"/>
+      <c r="G1006" s="7"/>
+      <c r="H1006" s="7"/>
+      <c r="I1006" s="7"/>
+      <c r="J1006" s="7"/>
+      <c r="K1006" s="7"/>
+      <c r="L1006" s="7"/>
+      <c r="M1006" s="7"/>
+      <c r="N1006" s="7"/>
+      <c r="O1006" s="7"/>
+      <c r="P1006" s="7"/>
+      <c r="Q1006" s="7"/>
+      <c r="R1006" s="7"/>
+      <c r="S1006" s="7"/>
+      <c r="T1006" s="7"/>
+      <c r="U1006" s="7"/>
+      <c r="V1006" s="7"/>
+      <c r="W1006" s="7"/>
+      <c r="X1006" s="7"/>
+      <c r="Y1006" s="7"/>
+      <c r="Z1006" s="7"/>
+    </row>
+    <row r="1007" ht="19.5" customHeight="1">
+      <c r="A1007" s="7"/>
+      <c r="B1007" s="7"/>
+      <c r="C1007" s="7"/>
+      <c r="D1007" s="7"/>
+      <c r="E1007" s="7"/>
+      <c r="F1007" s="7"/>
+      <c r="G1007" s="7"/>
+      <c r="H1007" s="7"/>
+      <c r="I1007" s="7"/>
+      <c r="J1007" s="7"/>
+      <c r="K1007" s="7"/>
+      <c r="L1007" s="7"/>
+      <c r="M1007" s="7"/>
+      <c r="N1007" s="7"/>
+      <c r="O1007" s="7"/>
+      <c r="P1007" s="7"/>
+      <c r="Q1007" s="7"/>
+      <c r="R1007" s="7"/>
+      <c r="S1007" s="7"/>
+      <c r="T1007" s="7"/>
+      <c r="U1007" s="7"/>
+      <c r="V1007" s="7"/>
+      <c r="W1007" s="7"/>
+      <c r="X1007" s="7"/>
+      <c r="Y1007" s="7"/>
+      <c r="Z1007" s="7"/>
+    </row>
+    <row r="1008" ht="19.5" customHeight="1">
+      <c r="A1008" s="7"/>
+      <c r="B1008" s="7"/>
+      <c r="C1008" s="7"/>
+      <c r="D1008" s="7"/>
+      <c r="E1008" s="7"/>
+      <c r="F1008" s="7"/>
+      <c r="G1008" s="7"/>
+      <c r="H1008" s="7"/>
+      <c r="I1008" s="7"/>
+      <c r="J1008" s="7"/>
+      <c r="K1008" s="7"/>
+      <c r="L1008" s="7"/>
+      <c r="M1008" s="7"/>
+      <c r="N1008" s="7"/>
+      <c r="O1008" s="7"/>
+      <c r="P1008" s="7"/>
+      <c r="Q1008" s="7"/>
+      <c r="R1008" s="7"/>
+      <c r="S1008" s="7"/>
+      <c r="T1008" s="7"/>
+      <c r="U1008" s="7"/>
+      <c r="V1008" s="7"/>
+      <c r="W1008" s="7"/>
+      <c r="X1008" s="7"/>
+      <c r="Y1008" s="7"/>
+      <c r="Z1008" s="7"/>
+    </row>
+    <row r="1009" ht="19.5" customHeight="1">
+      <c r="A1009" s="7"/>
+      <c r="B1009" s="7"/>
+      <c r="C1009" s="7"/>
+      <c r="D1009" s="7"/>
+      <c r="E1009" s="7"/>
+      <c r="F1009" s="7"/>
+      <c r="G1009" s="7"/>
+      <c r="H1009" s="7"/>
+      <c r="I1009" s="7"/>
+      <c r="J1009" s="7"/>
+      <c r="K1009" s="7"/>
+      <c r="L1009" s="7"/>
+      <c r="M1009" s="7"/>
+      <c r="N1009" s="7"/>
+      <c r="O1009" s="7"/>
+      <c r="P1009" s="7"/>
+      <c r="Q1009" s="7"/>
+      <c r="R1009" s="7"/>
+      <c r="S1009" s="7"/>
+      <c r="T1009" s="7"/>
+      <c r="U1009" s="7"/>
+      <c r="V1009" s="7"/>
+      <c r="W1009" s="7"/>
+      <c r="X1009" s="7"/>
+      <c r="Y1009" s="7"/>
+      <c r="Z1009" s="7"/>
+    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.5" right="0.5" top="0.75"/>
@@ -29616,6 +29934,7 @@
   <headerFooter>
     <oddFooter>&amp;C000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up for pass check without complaints.
</commit_message>
<xml_diff>
--- a/inst/googlesheet/microcosmScheme.xlsx
+++ b/inst/googlesheet/microcosmScheme.xlsx
@@ -513,7 +513,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="22">
     <border/>
     <border>
       <left style="thin">
@@ -704,62 +704,6 @@
       <right style="thin">
         <color rgb="FFA5A5A5"/>
       </right>
-      <top style="thin">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFED220B"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFA5A5A5"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFED220B"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFED220B"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFED220B"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFED220B"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFA5A5A5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFED220B"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFA5A5A5"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFA5A5A5"/>
-      </right>
       <top style="thick">
         <color rgb="FFED220B"/>
       </top>
@@ -869,7 +813,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="76">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -943,9 +887,6 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="12" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1041,73 +982,43 @@
     <xf borderId="9" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="14" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="14" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="16" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="16" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="17" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="18" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="20" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="21" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="21" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="6" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="22" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="22" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="23" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="24" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="25" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="22" fillId="6" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="22" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1294,18 +1205,18 @@
         <v>14</v>
       </c>
       <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27" t="s">
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="27" t="s">
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -1325,17 +1236,17 @@
       <c r="A5" s="21"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
@@ -1354,26 +1265,26 @@
     <row r="6" ht="31.5" customHeight="1">
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="27" t="s">
+      <c r="H6" s="27"/>
+      <c r="I6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M6" s="7"/>
@@ -1394,18 +1305,18 @@
     <row r="7" ht="24.75" customHeight="1">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
@@ -1424,18 +1335,18 @@
     <row r="8" ht="24.75" customHeight="1">
       <c r="A8" s="21"/>
       <c r="B8" s="22"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -1454,20 +1365,20 @@
     <row r="9" ht="24.75" customHeight="1">
       <c r="A9" s="21"/>
       <c r="B9" s="22"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="29" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="27" t="s">
+      <c r="E9" s="24"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
@@ -1486,18 +1397,18 @@
     <row r="10" ht="24.75" customHeight="1">
       <c r="A10" s="21"/>
       <c r="B10" s="22"/>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -1516,18 +1427,18 @@
     <row r="11" ht="24.75" customHeight="1">
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="32" t="s">
+      <c r="C11" s="32"/>
+      <c r="D11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
@@ -1546,18 +1457,18 @@
     <row r="12" ht="24.75" customHeight="1">
       <c r="A12" s="21"/>
       <c r="B12" s="22"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="32" t="s">
+      <c r="C12" s="32"/>
+      <c r="D12" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
@@ -1584,7 +1495,7 @@
       <c r="F13" s="19">
         <v>1.1</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="33" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="20"/>
@@ -1614,24 +1525,24 @@
         <v>25</v>
       </c>
       <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27" t="s">
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="I14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="27" t="s">
+      <c r="K14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="27" t="s">
+      <c r="L14" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M14" s="7"/>
@@ -1656,14 +1567,14 @@
         <v>26</v>
       </c>
       <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
@@ -1686,20 +1597,20 @@
         <v>27</v>
       </c>
       <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="27" t="s">
+      <c r="E16" s="24"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
@@ -1718,24 +1629,24 @@
     <row r="17" ht="24.75" customHeight="1">
       <c r="A17" s="21"/>
       <c r="B17" s="22"/>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27" t="s">
+      <c r="E17" s="24"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="27" t="s">
+      <c r="H17" s="27"/>
+      <c r="I17" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="27" t="s">
+      <c r="J17" s="27"/>
+      <c r="K17" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="28"/>
+      <c r="L17" s="27"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
@@ -1762,10 +1673,10 @@
       <c r="F18" s="19">
         <v>1.2</v>
       </c>
-      <c r="G18" s="34" t="s">
+      <c r="G18" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="33" t="s">
         <v>15</v>
       </c>
       <c r="I18" s="20"/>
@@ -1790,7 +1701,7 @@
     <row r="19" ht="24.75" customHeight="1">
       <c r="A19" s="14"/>
       <c r="B19" s="16"/>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="17"/>
@@ -1798,16 +1709,16 @@
       <c r="F19" s="19"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J19" s="34" t="s">
+      <c r="J19" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="34" t="s">
+      <c r="K19" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="34" t="s">
+      <c r="L19" s="33" t="s">
         <v>15</v>
       </c>
       <c r="M19" s="7"/>
@@ -1828,26 +1739,26 @@
     <row r="20" ht="24.75" customHeight="1">
       <c r="A20" s="14"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
       <c r="G20" s="20"/>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="34" t="s">
+      <c r="J20" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="L20" s="34" t="s">
+      <c r="L20" s="33" t="s">
         <v>15</v>
       </c>
       <c r="M20" s="7"/>
@@ -1881,7 +1792,7 @@
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
-      <c r="L21" s="34" t="s">
+      <c r="L21" s="33" t="s">
         <v>15</v>
       </c>
       <c r="M21" s="7"/>
@@ -1906,24 +1817,24 @@
         <v>25</v>
       </c>
       <c r="D22" s="24"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27" t="s">
+      <c r="E22" s="24"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="H22" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="27" t="s">
+      <c r="I22" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="27" t="s">
+      <c r="K22" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L22" s="28"/>
+      <c r="L22" s="27"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
@@ -1946,14 +1857,14 @@
         <v>26</v>
       </c>
       <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
@@ -1976,20 +1887,20 @@
         <v>32</v>
       </c>
       <c r="D24" s="24"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27" t="s">
+      <c r="E24" s="24"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I24" s="28"/>
-      <c r="J24" s="27" t="s">
+      <c r="I24" s="27"/>
+      <c r="J24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
@@ -2008,24 +1919,24 @@
     <row r="25" ht="24.75" customHeight="1">
       <c r="A25" s="21"/>
       <c r="B25" s="22"/>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="24"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27" t="s">
+      <c r="E25" s="24"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H25" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="27" t="s">
+      <c r="I25" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
@@ -2138,22 +2049,22 @@
       <c r="Z28" s="7"/>
     </row>
     <row r="29" ht="24.75" customHeight="1">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="31"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="22"/>
       <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="27" t="s">
+      <c r="E29" s="24"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K29" s="28"/>
-      <c r="L29" s="27" t="s">
+      <c r="K29" s="27"/>
+      <c r="L29" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M29" s="7"/>
@@ -2173,19 +2084,19 @@
     </row>
     <row r="30" ht="24.75" customHeight="1">
       <c r="A30" s="21"/>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="36" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="24"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
@@ -2203,19 +2114,19 @@
     </row>
     <row r="31" ht="24.75" customHeight="1">
       <c r="A31" s="21"/>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="36" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="22"/>
       <c r="D31" s="24"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
@@ -2233,19 +2144,19 @@
     </row>
     <row r="32" ht="24.75" customHeight="1">
       <c r="A32" s="21"/>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="36" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="24"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="27"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
@@ -2263,19 +2174,19 @@
     </row>
     <row r="33" ht="24.75" customHeight="1">
       <c r="A33" s="21"/>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="24"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
@@ -2293,19 +2204,19 @@
     </row>
     <row r="34" ht="24.75" customHeight="1">
       <c r="A34" s="21"/>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="22"/>
       <c r="D34" s="24"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
@@ -2323,19 +2234,19 @@
     </row>
     <row r="35" ht="24.75" customHeight="1">
       <c r="A35" s="21"/>
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="37" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="24"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="27"/>
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
@@ -2353,19 +2264,19 @@
     </row>
     <row r="36" ht="24.75" customHeight="1">
       <c r="A36" s="21"/>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="37" t="s">
         <v>43</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="24"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
@@ -2382,22 +2293,22 @@
       <c r="Z36" s="7"/>
     </row>
     <row r="37" ht="24.75" customHeight="1">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="43">
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="42">
         <v>3.0</v>
       </c>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="44"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
@@ -2420,18 +2331,18 @@
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="24"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="27" t="s">
+      <c r="E38" s="24"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J38" s="28"/>
-      <c r="K38" s="27" t="s">
+      <c r="J38" s="27"/>
+      <c r="K38" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L38" s="27" t="s">
+      <c r="L38" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M38" s="7"/>
@@ -2451,12 +2362,12 @@
     </row>
     <row r="39" ht="24.75" customHeight="1">
       <c r="A39" s="14"/>
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="46"/>
+      <c r="C39" s="45"/>
       <c r="D39" s="16"/>
-      <c r="E39" s="47"/>
+      <c r="E39" s="46"/>
       <c r="F39" s="19"/>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -2481,22 +2392,22 @@
     </row>
     <row r="40" ht="24.75" customHeight="1">
       <c r="A40" s="14"/>
-      <c r="B40" s="48"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="15" t="s">
         <v>47</v>
       </c>
       <c r="D40" s="16"/>
-      <c r="E40" s="47"/>
+      <c r="E40" s="46"/>
       <c r="F40" s="19">
         <v>3.2</v>
       </c>
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
-      <c r="J40" s="34" t="s">
+      <c r="J40" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="K40" s="34" t="s">
+      <c r="K40" s="33" t="s">
         <v>15</v>
       </c>
       <c r="L40" s="20"/>
@@ -2517,19 +2428,19 @@
     </row>
     <row r="41" ht="24.75" customHeight="1">
       <c r="A41" s="21"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="49"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="48"/>
       <c r="D41" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E41" s="50"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
@@ -2547,19 +2458,19 @@
     </row>
     <row r="42" ht="24.75" customHeight="1">
       <c r="A42" s="21"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="49"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="48"/>
       <c r="D42" s="22"/>
-      <c r="E42" s="51" t="s">
+      <c r="E42" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="F42" s="26"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
       <c r="O42" s="7"/>
@@ -2577,19 +2488,19 @@
     </row>
     <row r="43" ht="24.75" customHeight="1">
       <c r="A43" s="21"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="49"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="48"/>
       <c r="D43" s="22"/>
-      <c r="E43" s="52" t="s">
+      <c r="E43" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="F43" s="26"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="28"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
       <c r="O43" s="7"/>
@@ -2607,19 +2518,19 @@
     </row>
     <row r="44" ht="24.75" customHeight="1">
       <c r="A44" s="21"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="49"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="48"/>
       <c r="D44" s="22"/>
-      <c r="E44" s="51" t="s">
+      <c r="E44" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="26"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
       <c r="O44" s="7"/>
@@ -2637,16 +2548,16 @@
     </row>
     <row r="45" ht="24.75" customHeight="1">
       <c r="A45" s="14"/>
-      <c r="B45" s="48"/>
+      <c r="B45" s="47"/>
       <c r="C45" s="15" t="s">
         <v>50</v>
       </c>
       <c r="D45" s="16"/>
-      <c r="E45" s="47"/>
+      <c r="E45" s="46"/>
       <c r="F45" s="19">
         <v>3.600000000000001</v>
       </c>
-      <c r="G45" s="34" t="s">
+      <c r="G45" s="33" t="s">
         <v>15</v>
       </c>
       <c r="H45" s="20"/>
@@ -2671,19 +2582,19 @@
     </row>
     <row r="46" ht="24.75" customHeight="1">
       <c r="A46" s="21"/>
-      <c r="B46" s="31"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="22"/>
       <c r="D46" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="50"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="27"/>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
       <c r="O46" s="7"/>
@@ -2701,25 +2612,25 @@
     </row>
     <row r="47" ht="24.75" customHeight="1">
       <c r="A47" s="21"/>
-      <c r="B47" s="31"/>
+      <c r="B47" s="30"/>
       <c r="C47" s="22"/>
       <c r="D47" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E47" s="50"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="27" t="s">
+      <c r="E47" s="49"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J47" s="27" t="s">
+      <c r="J47" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K47" s="27" t="s">
+      <c r="K47" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L47" s="27" t="s">
+      <c r="L47" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M47" s="7"/>
@@ -2739,25 +2650,25 @@
     </row>
     <row r="48" ht="31.5" customHeight="1">
       <c r="A48" s="21"/>
-      <c r="B48" s="31"/>
+      <c r="B48" s="30"/>
       <c r="C48" s="22"/>
       <c r="D48" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="50"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
-      <c r="I48" s="27" t="s">
+      <c r="E48" s="49"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="J48" s="27" t="s">
+      <c r="J48" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="K48" s="27" t="s">
+      <c r="K48" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L48" s="28"/>
+      <c r="L48" s="27"/>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
@@ -2775,19 +2686,19 @@
     </row>
     <row r="49" ht="24.75" customHeight="1">
       <c r="A49" s="21"/>
-      <c r="B49" s="31"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="23" t="s">
         <v>55</v>
       </c>
       <c r="D49" s="22"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="28"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="27"/>
       <c r="M49" s="7"/>
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
@@ -2805,23 +2716,23 @@
     </row>
     <row r="50" ht="24.75" customHeight="1">
       <c r="A50" s="21"/>
-      <c r="B50" s="31"/>
+      <c r="B50" s="30"/>
       <c r="C50" s="22"/>
       <c r="D50" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="50"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="27" t="s">
+      <c r="E50" s="49"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J50" s="27" t="s">
+      <c r="J50" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K50" s="28"/>
-      <c r="L50" s="28"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="27"/>
       <c r="M50" s="7"/>
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
@@ -2839,21 +2750,21 @@
     </row>
     <row r="51" ht="24.75" customHeight="1">
       <c r="A51" s="21"/>
-      <c r="B51" s="31"/>
+      <c r="B51" s="30"/>
       <c r="C51" s="22"/>
       <c r="D51" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E51" s="50"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="28"/>
-      <c r="H51" s="28"/>
-      <c r="I51" s="27" t="s">
+      <c r="E51" s="49"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J51" s="28"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="28"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="27"/>
+      <c r="L51" s="27"/>
       <c r="M51" s="7"/>
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
@@ -2871,23 +2782,23 @@
     </row>
     <row r="52" ht="24.75" customHeight="1">
       <c r="A52" s="21"/>
-      <c r="B52" s="31"/>
+      <c r="B52" s="30"/>
       <c r="C52" s="22"/>
       <c r="D52" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E52" s="50"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="27" t="s">
+      <c r="E52" s="49"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J52" s="27" t="s">
+      <c r="J52" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="K52" s="28"/>
-      <c r="L52" s="28"/>
+      <c r="K52" s="27"/>
+      <c r="L52" s="27"/>
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
       <c r="O52" s="7"/>
@@ -2905,25 +2816,25 @@
     </row>
     <row r="53" ht="24.75" customHeight="1">
       <c r="A53" s="21"/>
-      <c r="B53" s="31"/>
+      <c r="B53" s="30"/>
       <c r="C53" s="22"/>
       <c r="D53" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E53" s="50"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="27" t="s">
+      <c r="E53" s="49"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H53" s="27" t="s">
+      <c r="H53" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I53" s="27" t="s">
+      <c r="I53" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J53" s="28"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="27" t="s">
+      <c r="J53" s="27"/>
+      <c r="K53" s="27"/>
+      <c r="L53" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M53" s="7"/>
@@ -2943,21 +2854,21 @@
     </row>
     <row r="54" ht="24.75" customHeight="1">
       <c r="A54" s="21"/>
-      <c r="B54" s="31"/>
+      <c r="B54" s="30"/>
       <c r="C54" s="23" t="s">
         <v>60</v>
       </c>
       <c r="D54" s="22"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="28"/>
-      <c r="K54" s="27" t="s">
+      <c r="E54" s="49"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27"/>
+      <c r="K54" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L54" s="28"/>
+      <c r="L54" s="27"/>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
@@ -2975,7 +2886,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1">
       <c r="A55" s="14"/>
-      <c r="B55" s="46"/>
+      <c r="B55" s="45"/>
       <c r="C55" s="15" t="s">
         <v>61</v>
       </c>
@@ -2984,7 +2895,7 @@
       <c r="F55" s="19">
         <v>3.700000000000001</v>
       </c>
-      <c r="G55" s="34" t="s">
+      <c r="G55" s="33" t="s">
         <v>15</v>
       </c>
       <c r="H55" s="20"/>
@@ -3009,12 +2920,12 @@
     </row>
     <row r="56" ht="24.75" customHeight="1">
       <c r="A56" s="14"/>
-      <c r="B56" s="48"/>
+      <c r="B56" s="47"/>
       <c r="C56" s="15" t="s">
         <v>62</v>
       </c>
       <c r="D56" s="16"/>
-      <c r="E56" s="47"/>
+      <c r="E56" s="46"/>
       <c r="F56" s="19">
         <v>3.3</v>
       </c>
@@ -3041,12 +2952,12 @@
     </row>
     <row r="57" ht="24.75" customHeight="1">
       <c r="A57" s="14"/>
-      <c r="B57" s="48"/>
+      <c r="B57" s="47"/>
       <c r="C57" s="15" t="s">
         <v>63</v>
       </c>
       <c r="D57" s="16"/>
-      <c r="E57" s="47"/>
+      <c r="E57" s="46"/>
       <c r="F57" s="19">
         <v>3.4</v>
       </c>
@@ -3073,12 +2984,12 @@
     </row>
     <row r="58" ht="24.75" customHeight="1">
       <c r="A58" s="14"/>
-      <c r="B58" s="48"/>
+      <c r="B58" s="47"/>
       <c r="C58" s="15" t="s">
         <v>64</v>
       </c>
       <c r="D58" s="16"/>
-      <c r="E58" s="47"/>
+      <c r="E58" s="46"/>
       <c r="F58" s="19">
         <v>3.5</v>
       </c>
@@ -3104,7 +3015,7 @@
       <c r="Z58" s="7"/>
     </row>
     <row r="59" ht="24.75" customHeight="1">
-      <c r="A59" s="53" t="s">
+      <c r="A59" s="52" t="s">
         <v>65</v>
       </c>
       <c r="B59" s="16"/>
@@ -3114,12 +3025,12 @@
       <c r="F59" s="19">
         <v>2.1</v>
       </c>
-      <c r="G59" s="34" t="s">
+      <c r="G59" s="33" t="s">
         <v>15</v>
       </c>
       <c r="H59" s="20"/>
       <c r="I59" s="20"/>
-      <c r="J59" s="34" t="s">
+      <c r="J59" s="33" t="s">
         <v>15</v>
       </c>
       <c r="K59" s="20"/>
@@ -3144,22 +3055,22 @@
       <c r="B60" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="31"/>
+      <c r="C60" s="30"/>
       <c r="D60" s="24"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="27" t="s">
+      <c r="E60" s="24"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H60" s="28"/>
-      <c r="I60" s="27" t="s">
+      <c r="H60" s="27"/>
+      <c r="I60" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J60" s="28"/>
-      <c r="K60" s="27" t="s">
+      <c r="J60" s="27"/>
+      <c r="K60" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="L60" s="27" t="s">
+      <c r="L60" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M60" s="7"/>
@@ -3180,18 +3091,18 @@
     <row r="61" ht="24.75" customHeight="1">
       <c r="A61" s="21"/>
       <c r="B61" s="22"/>
-      <c r="C61" s="37" t="s">
+      <c r="C61" s="36" t="s">
         <v>68</v>
       </c>
       <c r="D61" s="24"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="28"/>
-      <c r="H61" s="28"/>
-      <c r="I61" s="28"/>
-      <c r="J61" s="28"/>
-      <c r="K61" s="28"/>
-      <c r="L61" s="28"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="27"/>
       <c r="M61" s="7"/>
       <c r="N61" s="7"/>
       <c r="O61" s="7"/>
@@ -3210,18 +3121,18 @@
     <row r="62" ht="24.75" customHeight="1">
       <c r="A62" s="21"/>
       <c r="B62" s="22"/>
-      <c r="C62" s="37" t="s">
+      <c r="C62" s="36" t="s">
         <v>69</v>
       </c>
       <c r="D62" s="24"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="28"/>
-      <c r="H62" s="28"/>
-      <c r="I62" s="28"/>
-      <c r="J62" s="28"/>
-      <c r="K62" s="28"/>
-      <c r="L62" s="28"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="27"/>
+      <c r="H62" s="27"/>
+      <c r="I62" s="27"/>
+      <c r="J62" s="27"/>
+      <c r="K62" s="27"/>
+      <c r="L62" s="27"/>
       <c r="M62" s="7"/>
       <c r="N62" s="7"/>
       <c r="O62" s="7"/>
@@ -3242,20 +3153,20 @@
       <c r="B63" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C63" s="31"/>
+      <c r="C63" s="30"/>
       <c r="D63" s="24"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="28"/>
-      <c r="H63" s="28"/>
-      <c r="I63" s="27" t="s">
+      <c r="E63" s="24"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J63" s="28"/>
-      <c r="K63" s="27" t="s">
+      <c r="J63" s="27"/>
+      <c r="K63" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="L63" s="27" t="s">
+      <c r="L63" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M63" s="7"/>
@@ -3275,19 +3186,19 @@
     </row>
     <row r="64" ht="24.75" customHeight="1">
       <c r="A64" s="21"/>
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C64" s="31"/>
+      <c r="C64" s="30"/>
       <c r="D64" s="24"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="26"/>
-      <c r="G64" s="28"/>
-      <c r="H64" s="28"/>
-      <c r="I64" s="27"/>
-      <c r="J64" s="28"/>
-      <c r="K64" s="27"/>
-      <c r="L64" s="27"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="26"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="26"/>
+      <c r="L64" s="26"/>
       <c r="M64" s="7"/>
       <c r="N64" s="7"/>
       <c r="O64" s="7"/>
@@ -3304,22 +3215,22 @@
       <c r="Z64" s="7"/>
     </row>
     <row r="65" ht="41.25" customHeight="1">
-      <c r="A65" s="39" t="s">
+      <c r="A65" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B65" s="40"/>
-      <c r="C65" s="40"/>
-      <c r="D65" s="41"/>
-      <c r="E65" s="42"/>
-      <c r="F65" s="43">
+      <c r="B65" s="39"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="41"/>
+      <c r="F65" s="42">
         <v>2.0</v>
       </c>
-      <c r="G65" s="44"/>
-      <c r="H65" s="44"/>
-      <c r="I65" s="44"/>
-      <c r="J65" s="44"/>
-      <c r="K65" s="44"/>
-      <c r="L65" s="44"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="43"/>
+      <c r="I65" s="43"/>
+      <c r="J65" s="43"/>
+      <c r="K65" s="43"/>
+      <c r="L65" s="43"/>
       <c r="M65" s="7"/>
       <c r="N65" s="7"/>
       <c r="O65" s="7"/>
@@ -3346,11 +3257,11 @@
       <c r="F66" s="19">
         <v>2.2</v>
       </c>
-      <c r="G66" s="34" t="s">
+      <c r="G66" s="33" t="s">
         <v>15</v>
       </c>
       <c r="H66" s="20"/>
-      <c r="I66" s="34" t="s">
+      <c r="I66" s="33" t="s">
         <v>15</v>
       </c>
       <c r="J66" s="20"/>
@@ -3378,14 +3289,14 @@
         <v>74</v>
       </c>
       <c r="D67" s="24"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="26"/>
-      <c r="G67" s="28"/>
-      <c r="H67" s="28"/>
-      <c r="I67" s="28"/>
-      <c r="J67" s="28"/>
-      <c r="K67" s="28"/>
-      <c r="L67" s="28"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
+      <c r="I67" s="27"/>
+      <c r="J67" s="27"/>
+      <c r="K67" s="27"/>
+      <c r="L67" s="27"/>
       <c r="M67" s="7"/>
       <c r="N67" s="7"/>
       <c r="O67" s="7"/>
@@ -3405,17 +3316,17 @@
       <c r="A68" s="21"/>
       <c r="B68" s="22"/>
       <c r="C68" s="22"/>
-      <c r="D68" s="29" t="s">
+      <c r="D68" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E68" s="25"/>
-      <c r="F68" s="26"/>
-      <c r="G68" s="28"/>
-      <c r="H68" s="28"/>
-      <c r="I68" s="28"/>
-      <c r="J68" s="28"/>
-      <c r="K68" s="28"/>
-      <c r="L68" s="28"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
+      <c r="I68" s="27"/>
+      <c r="J68" s="27"/>
+      <c r="K68" s="27"/>
+      <c r="L68" s="27"/>
       <c r="M68" s="7"/>
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
@@ -3435,17 +3346,17 @@
       <c r="A69" s="21"/>
       <c r="B69" s="22"/>
       <c r="C69" s="22"/>
-      <c r="D69" s="29" t="s">
+      <c r="D69" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="E69" s="25"/>
-      <c r="F69" s="26"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="27"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="27"/>
+      <c r="K69" s="27"/>
+      <c r="L69" s="27"/>
       <c r="M69" s="7"/>
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
@@ -3468,16 +3379,16 @@
         <v>76</v>
       </c>
       <c r="D70" s="24"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="26"/>
-      <c r="G70" s="28"/>
-      <c r="H70" s="28"/>
-      <c r="I70" s="28"/>
-      <c r="J70" s="28"/>
-      <c r="K70" s="27" t="s">
+      <c r="E70" s="24"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="27"/>
+      <c r="H70" s="27"/>
+      <c r="I70" s="27"/>
+      <c r="J70" s="27"/>
+      <c r="K70" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="L70" s="28"/>
+      <c r="L70" s="27"/>
       <c r="M70" s="7"/>
       <c r="N70" s="7"/>
       <c r="O70" s="7"/>
@@ -3500,18 +3411,18 @@
         <v>78</v>
       </c>
       <c r="D71" s="24"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="26"/>
-      <c r="G71" s="28"/>
-      <c r="H71" s="28"/>
-      <c r="I71" s="27" t="s">
+      <c r="E71" s="24"/>
+      <c r="F71" s="25"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="27"/>
+      <c r="I71" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J71" s="28"/>
-      <c r="K71" s="27" t="s">
+      <c r="J71" s="27"/>
+      <c r="K71" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="L71" s="27" t="s">
+      <c r="L71" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M71" s="7"/>
@@ -3540,12 +3451,12 @@
       <c r="F72" s="19">
         <v>2.3</v>
       </c>
-      <c r="G72" s="34" t="s">
+      <c r="G72" s="33" t="s">
         <v>15</v>
       </c>
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
-      <c r="J72" s="34" t="s">
+      <c r="J72" s="33" t="s">
         <v>80</v>
       </c>
       <c r="K72" s="20"/>
@@ -3568,18 +3479,18 @@
     <row r="73" ht="24.75" customHeight="1">
       <c r="A73" s="21"/>
       <c r="B73" s="22"/>
-      <c r="C73" s="37" t="s">
+      <c r="C73" s="36" t="s">
         <v>81</v>
       </c>
       <c r="D73" s="22"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="26"/>
-      <c r="G73" s="28"/>
-      <c r="H73" s="28"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="28"/>
-      <c r="K73" s="28"/>
-      <c r="L73" s="28"/>
+      <c r="E73" s="49"/>
+      <c r="F73" s="25"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="27"/>
+      <c r="I73" s="27"/>
+      <c r="J73" s="27"/>
+      <c r="K73" s="27"/>
+      <c r="L73" s="27"/>
       <c r="M73" s="7"/>
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>
@@ -3598,18 +3509,18 @@
     <row r="74" ht="24.75" customHeight="1">
       <c r="A74" s="21"/>
       <c r="B74" s="22"/>
-      <c r="C74" s="31"/>
+      <c r="C74" s="30"/>
       <c r="D74" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E74" s="50"/>
-      <c r="F74" s="26"/>
-      <c r="G74" s="28"/>
-      <c r="H74" s="28"/>
-      <c r="I74" s="28"/>
-      <c r="J74" s="28"/>
-      <c r="K74" s="28"/>
-      <c r="L74" s="28"/>
+      <c r="E74" s="49"/>
+      <c r="F74" s="25"/>
+      <c r="G74" s="27"/>
+      <c r="H74" s="27"/>
+      <c r="I74" s="27"/>
+      <c r="J74" s="27"/>
+      <c r="K74" s="27"/>
+      <c r="L74" s="27"/>
       <c r="M74" s="7"/>
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
@@ -3628,18 +3539,18 @@
     <row r="75" ht="24.75" customHeight="1">
       <c r="A75" s="21"/>
       <c r="B75" s="22"/>
-      <c r="C75" s="31"/>
+      <c r="C75" s="30"/>
       <c r="D75" s="22"/>
-      <c r="E75" s="51" t="s">
+      <c r="E75" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="F75" s="26"/>
-      <c r="G75" s="28"/>
-      <c r="H75" s="28"/>
-      <c r="I75" s="28"/>
-      <c r="J75" s="28"/>
-      <c r="K75" s="28"/>
-      <c r="L75" s="28"/>
+      <c r="F75" s="25"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="27"/>
+      <c r="I75" s="27"/>
+      <c r="J75" s="27"/>
+      <c r="K75" s="27"/>
+      <c r="L75" s="27"/>
       <c r="M75" s="7"/>
       <c r="N75" s="7"/>
       <c r="O75" s="7"/>
@@ -3658,18 +3569,18 @@
     <row r="76" ht="24.75" customHeight="1">
       <c r="A76" s="21"/>
       <c r="B76" s="22"/>
-      <c r="C76" s="31"/>
+      <c r="C76" s="30"/>
       <c r="D76" s="22"/>
-      <c r="E76" s="51" t="s">
+      <c r="E76" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="F76" s="26"/>
-      <c r="G76" s="28"/>
-      <c r="H76" s="28"/>
-      <c r="I76" s="28"/>
-      <c r="J76" s="28"/>
-      <c r="K76" s="28"/>
-      <c r="L76" s="28"/>
+      <c r="F76" s="25"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="27"/>
+      <c r="I76" s="27"/>
+      <c r="J76" s="27"/>
+      <c r="K76" s="27"/>
+      <c r="L76" s="27"/>
       <c r="M76" s="7"/>
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
@@ -3688,20 +3599,20 @@
     <row r="77" ht="24.75" customHeight="1">
       <c r="A77" s="21"/>
       <c r="B77" s="22"/>
-      <c r="C77" s="31"/>
+      <c r="C77" s="30"/>
       <c r="D77" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="E77" s="50"/>
-      <c r="F77" s="26"/>
-      <c r="G77" s="27" t="s">
+      <c r="E77" s="49"/>
+      <c r="F77" s="25"/>
+      <c r="G77" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H77" s="28"/>
-      <c r="I77" s="28"/>
-      <c r="J77" s="28"/>
-      <c r="K77" s="28"/>
-      <c r="L77" s="27" t="s">
+      <c r="H77" s="27"/>
+      <c r="I77" s="27"/>
+      <c r="J77" s="27"/>
+      <c r="K77" s="27"/>
+      <c r="L77" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M77" s="7"/>
@@ -3722,18 +3633,18 @@
     <row r="78" ht="31.5" customHeight="1">
       <c r="A78" s="21"/>
       <c r="B78" s="22"/>
-      <c r="C78" s="31"/>
+      <c r="C78" s="30"/>
       <c r="D78" s="22"/>
-      <c r="E78" s="51" t="s">
+      <c r="E78" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="F78" s="26"/>
-      <c r="G78" s="28"/>
-      <c r="H78" s="28"/>
-      <c r="I78" s="28"/>
-      <c r="J78" s="28"/>
-      <c r="K78" s="28"/>
-      <c r="L78" s="27" t="s">
+      <c r="F78" s="25"/>
+      <c r="G78" s="27"/>
+      <c r="H78" s="27"/>
+      <c r="I78" s="27"/>
+      <c r="J78" s="27"/>
+      <c r="K78" s="27"/>
+      <c r="L78" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M78" s="7"/>
@@ -3754,18 +3665,18 @@
     <row r="79" ht="24.75" customHeight="1">
       <c r="A79" s="21"/>
       <c r="B79" s="22"/>
-      <c r="C79" s="31"/>
+      <c r="C79" s="30"/>
       <c r="D79" s="22"/>
-      <c r="E79" s="51" t="s">
+      <c r="E79" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="F79" s="26"/>
-      <c r="G79" s="28"/>
-      <c r="H79" s="28"/>
-      <c r="I79" s="28"/>
-      <c r="J79" s="28"/>
-      <c r="K79" s="28"/>
-      <c r="L79" s="27" t="s">
+      <c r="F79" s="25"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="27"/>
+      <c r="I79" s="27"/>
+      <c r="J79" s="27"/>
+      <c r="K79" s="27"/>
+      <c r="L79" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M79" s="7"/>
@@ -3786,20 +3697,20 @@
     <row r="80" ht="24.75" customHeight="1">
       <c r="A80" s="21"/>
       <c r="B80" s="22"/>
-      <c r="C80" s="31"/>
+      <c r="C80" s="30"/>
       <c r="D80" s="22"/>
-      <c r="E80" s="51" t="s">
+      <c r="E80" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="F80" s="26"/>
-      <c r="G80" s="27" t="s">
+      <c r="F80" s="25"/>
+      <c r="G80" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H80" s="28"/>
-      <c r="I80" s="28"/>
-      <c r="J80" s="28"/>
-      <c r="K80" s="28"/>
-      <c r="L80" s="27" t="s">
+      <c r="H80" s="27"/>
+      <c r="I80" s="27"/>
+      <c r="J80" s="27"/>
+      <c r="K80" s="27"/>
+      <c r="L80" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M80" s="7"/>
@@ -3820,18 +3731,18 @@
     <row r="81" ht="24.75" customHeight="1">
       <c r="A81" s="21"/>
       <c r="B81" s="22"/>
-      <c r="C81" s="31"/>
+      <c r="C81" s="30"/>
       <c r="D81" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E81" s="50"/>
-      <c r="F81" s="26"/>
-      <c r="G81" s="28"/>
-      <c r="H81" s="28"/>
-      <c r="I81" s="28"/>
-      <c r="J81" s="28"/>
-      <c r="K81" s="28"/>
-      <c r="L81" s="28"/>
+      <c r="E81" s="49"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="27"/>
+      <c r="I81" s="27"/>
+      <c r="J81" s="27"/>
+      <c r="K81" s="27"/>
+      <c r="L81" s="27"/>
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
       <c r="O81" s="7"/>
@@ -3850,20 +3761,20 @@
     <row r="82" ht="24.75" customHeight="1">
       <c r="A82" s="21"/>
       <c r="B82" s="22"/>
-      <c r="C82" s="31"/>
+      <c r="C82" s="30"/>
       <c r="D82" s="22"/>
-      <c r="E82" s="51" t="s">
+      <c r="E82" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="F82" s="26"/>
-      <c r="G82" s="27" t="s">
+      <c r="F82" s="25"/>
+      <c r="G82" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H82" s="28"/>
-      <c r="I82" s="28"/>
-      <c r="J82" s="28"/>
-      <c r="K82" s="28"/>
-      <c r="L82" s="27" t="s">
+      <c r="H82" s="27"/>
+      <c r="I82" s="27"/>
+      <c r="J82" s="27"/>
+      <c r="K82" s="27"/>
+      <c r="L82" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M82" s="7"/>
@@ -3884,18 +3795,18 @@
     <row r="83" ht="24.75" customHeight="1">
       <c r="A83" s="21"/>
       <c r="B83" s="22"/>
-      <c r="C83" s="31"/>
+      <c r="C83" s="30"/>
       <c r="D83" s="22"/>
-      <c r="E83" s="51" t="s">
+      <c r="E83" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="F83" s="26"/>
-      <c r="G83" s="28"/>
-      <c r="H83" s="28"/>
-      <c r="I83" s="28"/>
-      <c r="J83" s="28"/>
-      <c r="K83" s="28"/>
-      <c r="L83" s="28"/>
+      <c r="F83" s="25"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="27"/>
+      <c r="I83" s="27"/>
+      <c r="J83" s="27"/>
+      <c r="K83" s="27"/>
+      <c r="L83" s="27"/>
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
       <c r="O83" s="7"/>
@@ -3918,14 +3829,14 @@
         <v>89</v>
       </c>
       <c r="D84" s="24"/>
-      <c r="E84" s="54"/>
-      <c r="F84" s="26"/>
-      <c r="G84" s="28"/>
-      <c r="H84" s="28"/>
-      <c r="I84" s="28"/>
-      <c r="J84" s="28"/>
-      <c r="K84" s="28"/>
-      <c r="L84" s="28"/>
+      <c r="E84" s="53"/>
+      <c r="F84" s="25"/>
+      <c r="G84" s="27"/>
+      <c r="H84" s="27"/>
+      <c r="I84" s="27"/>
+      <c r="J84" s="27"/>
+      <c r="K84" s="27"/>
+      <c r="L84" s="27"/>
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
       <c r="O84" s="7"/>
@@ -3945,17 +3856,17 @@
       <c r="A85" s="21"/>
       <c r="B85" s="22"/>
       <c r="C85" s="22"/>
-      <c r="D85" s="29" t="s">
+      <c r="D85" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E85" s="54"/>
-      <c r="F85" s="26"/>
-      <c r="G85" s="28"/>
-      <c r="H85" s="28"/>
-      <c r="I85" s="28"/>
-      <c r="J85" s="28"/>
-      <c r="K85" s="28"/>
-      <c r="L85" s="28"/>
+      <c r="E85" s="53"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="27"/>
+      <c r="H85" s="27"/>
+      <c r="I85" s="27"/>
+      <c r="J85" s="27"/>
+      <c r="K85" s="27"/>
+      <c r="L85" s="27"/>
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
       <c r="O85" s="7"/>
@@ -3975,17 +3886,17 @@
       <c r="A86" s="21"/>
       <c r="B86" s="22"/>
       <c r="C86" s="22"/>
-      <c r="D86" s="29" t="s">
+      <c r="D86" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="E86" s="54"/>
-      <c r="F86" s="26"/>
-      <c r="G86" s="28"/>
-      <c r="H86" s="28"/>
-      <c r="I86" s="28"/>
-      <c r="J86" s="28"/>
-      <c r="K86" s="28"/>
-      <c r="L86" s="28"/>
+      <c r="E86" s="53"/>
+      <c r="F86" s="25"/>
+      <c r="G86" s="27"/>
+      <c r="H86" s="27"/>
+      <c r="I86" s="27"/>
+      <c r="J86" s="27"/>
+      <c r="K86" s="27"/>
+      <c r="L86" s="27"/>
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
       <c r="O86" s="7"/>
@@ -4005,17 +3916,17 @@
       <c r="A87" s="21"/>
       <c r="B87" s="22"/>
       <c r="C87" s="22"/>
-      <c r="D87" s="29" t="s">
+      <c r="D87" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="E87" s="54"/>
-      <c r="F87" s="26"/>
-      <c r="G87" s="28"/>
-      <c r="H87" s="28"/>
-      <c r="I87" s="28"/>
-      <c r="J87" s="28"/>
-      <c r="K87" s="28"/>
-      <c r="L87" s="28"/>
+      <c r="E87" s="53"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="27"/>
+      <c r="H87" s="27"/>
+      <c r="I87" s="27"/>
+      <c r="J87" s="27"/>
+      <c r="K87" s="27"/>
+      <c r="L87" s="27"/>
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
       <c r="O87" s="7"/>
@@ -4035,17 +3946,17 @@
       <c r="A88" s="21"/>
       <c r="B88" s="22"/>
       <c r="C88" s="22"/>
-      <c r="D88" s="29" t="s">
+      <c r="D88" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="E88" s="54"/>
-      <c r="F88" s="26"/>
-      <c r="G88" s="28"/>
-      <c r="H88" s="28"/>
-      <c r="I88" s="28"/>
-      <c r="J88" s="28"/>
-      <c r="K88" s="28"/>
-      <c r="L88" s="28"/>
+      <c r="E88" s="53"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="27"/>
+      <c r="H88" s="27"/>
+      <c r="I88" s="27"/>
+      <c r="J88" s="27"/>
+      <c r="K88" s="27"/>
+      <c r="L88" s="27"/>
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
       <c r="O88" s="7"/>
@@ -4077,7 +3988,7 @@
       <c r="I89" s="20"/>
       <c r="J89" s="20"/>
       <c r="K89" s="20"/>
-      <c r="L89" s="34" t="s">
+      <c r="L89" s="33" t="s">
         <v>15</v>
       </c>
       <c r="M89" s="7"/>
@@ -4097,19 +4008,19 @@
     </row>
     <row r="90" ht="24.75" customHeight="1">
       <c r="A90" s="21"/>
-      <c r="B90" s="49"/>
+      <c r="B90" s="48"/>
       <c r="C90" s="23" t="s">
         <v>93</v>
       </c>
       <c r="D90" s="24"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="26"/>
-      <c r="G90" s="28"/>
-      <c r="H90" s="28"/>
-      <c r="I90" s="28"/>
-      <c r="J90" s="28"/>
-      <c r="K90" s="28"/>
-      <c r="L90" s="28"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="25"/>
+      <c r="G90" s="27"/>
+      <c r="H90" s="27"/>
+      <c r="I90" s="27"/>
+      <c r="J90" s="27"/>
+      <c r="K90" s="27"/>
+      <c r="L90" s="27"/>
       <c r="M90" s="7"/>
       <c r="N90" s="7"/>
       <c r="O90" s="7"/>
@@ -4127,19 +4038,19 @@
     </row>
     <row r="91" ht="24.75" customHeight="1">
       <c r="A91" s="21"/>
-      <c r="B91" s="49"/>
-      <c r="C91" s="30" t="s">
+      <c r="B91" s="48"/>
+      <c r="C91" s="29" t="s">
         <v>70</v>
       </c>
       <c r="D91" s="24"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="26"/>
-      <c r="G91" s="28"/>
-      <c r="H91" s="28"/>
-      <c r="I91" s="28"/>
-      <c r="J91" s="28"/>
-      <c r="K91" s="28"/>
-      <c r="L91" s="27" t="s">
+      <c r="E91" s="24"/>
+      <c r="F91" s="25"/>
+      <c r="G91" s="27"/>
+      <c r="H91" s="27"/>
+      <c r="I91" s="27"/>
+      <c r="J91" s="27"/>
+      <c r="K91" s="27"/>
+      <c r="L91" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M91" s="7"/>
@@ -4159,19 +4070,19 @@
     </row>
     <row r="92" ht="24.75" customHeight="1">
       <c r="A92" s="21"/>
-      <c r="B92" s="49"/>
+      <c r="B92" s="48"/>
       <c r="C92" s="23" t="s">
         <v>76</v>
       </c>
       <c r="D92" s="24"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="26"/>
-      <c r="G92" s="28"/>
-      <c r="H92" s="28"/>
-      <c r="I92" s="28"/>
-      <c r="J92" s="28"/>
-      <c r="K92" s="28"/>
-      <c r="L92" s="27" t="s">
+      <c r="E92" s="24"/>
+      <c r="F92" s="25"/>
+      <c r="G92" s="27"/>
+      <c r="H92" s="27"/>
+      <c r="I92" s="27"/>
+      <c r="J92" s="27"/>
+      <c r="K92" s="27"/>
+      <c r="L92" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M92" s="7"/>
@@ -4191,19 +4102,19 @@
     </row>
     <row r="93" ht="24.75" customHeight="1">
       <c r="A93" s="21"/>
-      <c r="B93" s="49"/>
-      <c r="C93" s="30" t="s">
+      <c r="B93" s="48"/>
+      <c r="C93" s="29" t="s">
         <v>94</v>
       </c>
       <c r="D93" s="24"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="26"/>
-      <c r="G93" s="28"/>
-      <c r="H93" s="28"/>
-      <c r="I93" s="28"/>
-      <c r="J93" s="28"/>
-      <c r="K93" s="28"/>
-      <c r="L93" s="27" t="s">
+      <c r="E93" s="24"/>
+      <c r="F93" s="25"/>
+      <c r="G93" s="27"/>
+      <c r="H93" s="27"/>
+      <c r="I93" s="27"/>
+      <c r="J93" s="27"/>
+      <c r="K93" s="27"/>
+      <c r="L93" s="26" t="s">
         <v>15</v>
       </c>
       <c r="M93" s="7"/>
@@ -4223,17 +4134,17 @@
     </row>
     <row r="94" ht="24.75" customHeight="1">
       <c r="A94" s="21"/>
-      <c r="B94" s="49"/>
+      <c r="B94" s="48"/>
       <c r="C94" s="22"/>
       <c r="D94" s="24"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="26"/>
-      <c r="G94" s="28"/>
-      <c r="H94" s="28"/>
-      <c r="I94" s="28"/>
-      <c r="J94" s="28"/>
-      <c r="K94" s="28"/>
-      <c r="L94" s="28"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="27"/>
+      <c r="H94" s="27"/>
+      <c r="I94" s="27"/>
+      <c r="J94" s="27"/>
+      <c r="K94" s="27"/>
+      <c r="L94" s="27"/>
       <c r="M94" s="7"/>
       <c r="N94" s="7"/>
       <c r="O94" s="7"/>
@@ -4315,7 +4226,7 @@
     </row>
     <row r="97" ht="24.75" customHeight="1">
       <c r="A97" s="14"/>
-      <c r="B97" s="55" t="s">
+      <c r="B97" s="54" t="s">
         <v>97</v>
       </c>
       <c r="C97" s="16"/>
@@ -4347,8 +4258,8 @@
     </row>
     <row r="98" ht="24.75" customHeight="1">
       <c r="A98" s="14"/>
-      <c r="B98" s="55"/>
-      <c r="C98" s="56" t="s">
+      <c r="B98" s="54"/>
+      <c r="C98" s="55" t="s">
         <v>98</v>
       </c>
       <c r="D98" s="17"/>
@@ -4377,7 +4288,7 @@
     </row>
     <row r="99" ht="31.5" customHeight="1">
       <c r="A99" s="14"/>
-      <c r="B99" s="55" t="s">
+      <c r="B99" s="54" t="s">
         <v>99</v>
       </c>
       <c r="C99" s="16"/>
@@ -4409,8 +4320,8 @@
     </row>
     <row r="100" ht="31.5" customHeight="1">
       <c r="A100" s="14"/>
-      <c r="B100" s="55"/>
-      <c r="C100" s="56" t="s">
+      <c r="B100" s="54"/>
+      <c r="C100" s="55" t="s">
         <v>100</v>
       </c>
       <c r="D100" s="17"/>
@@ -4512,7 +4423,7 @@
       <c r="F103" s="19">
         <v>2.12</v>
       </c>
-      <c r="G103" s="34" t="s">
+      <c r="G103" s="33" t="s">
         <v>15</v>
       </c>
       <c r="H103" s="20"/>
@@ -4535,19 +4446,19 @@
       <c r="Y103" s="7"/>
       <c r="Z103" s="7"/>
     </row>
-    <row r="104" ht="24.75" customHeight="1">
-      <c r="A104" s="57"/>
-      <c r="B104" s="31"/>
-      <c r="C104" s="31"/>
+    <row r="104" ht="28.5" customHeight="1">
+      <c r="A104" s="56"/>
+      <c r="B104" s="57"/>
+      <c r="C104" s="57"/>
       <c r="D104" s="58"/>
-      <c r="E104" s="54"/>
-      <c r="F104" s="59"/>
-      <c r="G104" s="60"/>
-      <c r="H104" s="60"/>
-      <c r="I104" s="60"/>
-      <c r="J104" s="60"/>
-      <c r="K104" s="60"/>
-      <c r="L104" s="60"/>
+      <c r="E104" s="59"/>
+      <c r="F104" s="60"/>
+      <c r="G104" s="61"/>
+      <c r="H104" s="61"/>
+      <c r="I104" s="61"/>
+      <c r="J104" s="61"/>
+      <c r="K104" s="61"/>
+      <c r="L104" s="61"/>
       <c r="M104" s="7"/>
       <c r="N104" s="7"/>
       <c r="O104" s="7"/>
@@ -4563,19 +4474,29 @@
       <c r="Y104" s="7"/>
       <c r="Z104" s="7"/>
     </row>
-    <row r="105" ht="24.75" customHeight="1">
-      <c r="A105" s="57"/>
-      <c r="B105" s="31"/>
-      <c r="C105" s="31"/>
-      <c r="D105" s="58"/>
-      <c r="E105" s="54"/>
-      <c r="F105" s="59"/>
-      <c r="G105" s="60"/>
-      <c r="H105" s="60"/>
-      <c r="I105" s="60"/>
-      <c r="J105" s="60"/>
-      <c r="K105" s="60"/>
-      <c r="L105" s="60"/>
+    <row r="105" ht="26.25" customHeight="1">
+      <c r="A105" s="62"/>
+      <c r="B105" s="63"/>
+      <c r="C105" s="63"/>
+      <c r="D105" s="64"/>
+      <c r="E105" s="65"/>
+      <c r="F105" s="66"/>
+      <c r="G105" s="67" t="s">
+        <v>104</v>
+      </c>
+      <c r="H105" s="68"/>
+      <c r="I105" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="J105" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="K105" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="L105" s="67" t="s">
+        <v>108</v>
+      </c>
       <c r="M105" s="7"/>
       <c r="N105" s="7"/>
       <c r="O105" s="7"/>
@@ -4591,19 +4512,25 @@
       <c r="Y105" s="7"/>
       <c r="Z105" s="7"/>
     </row>
-    <row r="106" ht="24.75" customHeight="1">
-      <c r="A106" s="57"/>
-      <c r="B106" s="31"/>
-      <c r="C106" s="31"/>
-      <c r="D106" s="58"/>
-      <c r="E106" s="54"/>
-      <c r="F106" s="59"/>
-      <c r="G106" s="60"/>
-      <c r="H106" s="60"/>
-      <c r="I106" s="60"/>
-      <c r="J106" s="60"/>
-      <c r="K106" s="60"/>
-      <c r="L106" s="60"/>
+    <row r="106" ht="43.5" customHeight="1">
+      <c r="A106" s="69"/>
+      <c r="B106" s="70"/>
+      <c r="C106" s="70"/>
+      <c r="D106" s="71"/>
+      <c r="E106" s="72"/>
+      <c r="F106" s="73"/>
+      <c r="G106" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="H106" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="I106" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="J106" s="75"/>
+      <c r="K106" s="75"/>
+      <c r="L106" s="75"/>
       <c r="M106" s="7"/>
       <c r="N106" s="7"/>
       <c r="O106" s="7"/>
@@ -4619,19 +4546,25 @@
       <c r="Y106" s="7"/>
       <c r="Z106" s="7"/>
     </row>
-    <row r="107" ht="24.75" customHeight="1">
-      <c r="A107" s="57"/>
-      <c r="B107" s="31"/>
-      <c r="C107" s="31"/>
-      <c r="D107" s="58"/>
-      <c r="E107" s="54"/>
-      <c r="F107" s="59"/>
-      <c r="G107" s="60"/>
-      <c r="H107" s="60"/>
-      <c r="I107" s="60"/>
-      <c r="J107" s="60"/>
-      <c r="K107" s="60"/>
-      <c r="L107" s="60"/>
+    <row r="107" ht="43.5" customHeight="1">
+      <c r="A107" s="69"/>
+      <c r="B107" s="70"/>
+      <c r="C107" s="70"/>
+      <c r="D107" s="71"/>
+      <c r="E107" s="72"/>
+      <c r="F107" s="73"/>
+      <c r="G107" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="H107" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="I107" s="74" t="s">
+        <v>113</v>
+      </c>
+      <c r="J107" s="75"/>
+      <c r="K107" s="75"/>
+      <c r="L107" s="75"/>
       <c r="M107" s="7"/>
       <c r="N107" s="7"/>
       <c r="O107" s="7"/>
@@ -4648,18 +4581,20 @@
       <c r="Z107" s="7"/>
     </row>
     <row r="108" ht="24.75" customHeight="1">
-      <c r="A108" s="57"/>
-      <c r="B108" s="31"/>
-      <c r="C108" s="31"/>
-      <c r="D108" s="58"/>
-      <c r="E108" s="54"/>
-      <c r="F108" s="59"/>
-      <c r="G108" s="60"/>
-      <c r="H108" s="60"/>
-      <c r="I108" s="60"/>
-      <c r="J108" s="60"/>
-      <c r="K108" s="60"/>
-      <c r="L108" s="60"/>
+      <c r="A108" s="69"/>
+      <c r="B108" s="70"/>
+      <c r="C108" s="70"/>
+      <c r="D108" s="71"/>
+      <c r="E108" s="72"/>
+      <c r="F108" s="73"/>
+      <c r="G108" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="H108" s="75"/>
+      <c r="I108" s="75"/>
+      <c r="J108" s="75"/>
+      <c r="K108" s="75"/>
+      <c r="L108" s="75"/>
       <c r="M108" s="7"/>
       <c r="N108" s="7"/>
       <c r="O108" s="7"/>
@@ -4675,19 +4610,19 @@
       <c r="Y108" s="7"/>
       <c r="Z108" s="7"/>
     </row>
-    <row r="109" ht="24.75" customHeight="1">
-      <c r="A109" s="57"/>
-      <c r="B109" s="31"/>
-      <c r="C109" s="31"/>
-      <c r="D109" s="58"/>
-      <c r="E109" s="54"/>
-      <c r="F109" s="59"/>
-      <c r="G109" s="60"/>
-      <c r="H109" s="60"/>
-      <c r="I109" s="60"/>
-      <c r="J109" s="60"/>
-      <c r="K109" s="60"/>
-      <c r="L109" s="60"/>
+    <row r="109" ht="19.5" customHeight="1">
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7"/>
+      <c r="H109" s="7"/>
+      <c r="I109" s="7"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
       <c r="M109" s="7"/>
       <c r="N109" s="7"/>
       <c r="O109" s="7"/>
@@ -4703,19 +4638,19 @@
       <c r="Y109" s="7"/>
       <c r="Z109" s="7"/>
     </row>
-    <row r="110" ht="24.75" customHeight="1">
-      <c r="A110" s="57"/>
-      <c r="B110" s="31"/>
-      <c r="C110" s="31"/>
-      <c r="D110" s="58"/>
-      <c r="E110" s="54"/>
-      <c r="F110" s="59"/>
-      <c r="G110" s="60"/>
-      <c r="H110" s="60"/>
-      <c r="I110" s="60"/>
-      <c r="J110" s="60"/>
-      <c r="K110" s="60"/>
-      <c r="L110" s="60"/>
+    <row r="110" ht="19.5" customHeight="1">
+      <c r="A110" s="7"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="7"/>
+      <c r="F110" s="7"/>
+      <c r="G110" s="7"/>
+      <c r="H110" s="7"/>
+      <c r="I110" s="7"/>
+      <c r="J110" s="7"/>
+      <c r="K110" s="7"/>
+      <c r="L110" s="7"/>
       <c r="M110" s="7"/>
       <c r="N110" s="7"/>
       <c r="O110" s="7"/>
@@ -4731,19 +4666,19 @@
       <c r="Y110" s="7"/>
       <c r="Z110" s="7"/>
     </row>
-    <row r="111" ht="24.75" customHeight="1">
-      <c r="A111" s="57"/>
-      <c r="B111" s="31"/>
-      <c r="C111" s="31"/>
-      <c r="D111" s="58"/>
-      <c r="E111" s="54"/>
-      <c r="F111" s="59"/>
-      <c r="G111" s="60"/>
-      <c r="H111" s="60"/>
-      <c r="I111" s="60"/>
-      <c r="J111" s="60"/>
-      <c r="K111" s="60"/>
-      <c r="L111" s="60"/>
+    <row r="111" ht="19.5" customHeight="1">
+      <c r="A111" s="7"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7"/>
+      <c r="G111" s="7"/>
+      <c r="H111" s="7"/>
+      <c r="I111" s="7"/>
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
+      <c r="L111" s="7"/>
       <c r="M111" s="7"/>
       <c r="N111" s="7"/>
       <c r="O111" s="7"/>
@@ -4759,19 +4694,19 @@
       <c r="Y111" s="7"/>
       <c r="Z111" s="7"/>
     </row>
-    <row r="112" ht="24.75" customHeight="1">
-      <c r="A112" s="57"/>
-      <c r="B112" s="31"/>
-      <c r="C112" s="31"/>
-      <c r="D112" s="58"/>
-      <c r="E112" s="54"/>
-      <c r="F112" s="59"/>
-      <c r="G112" s="60"/>
-      <c r="H112" s="60"/>
-      <c r="I112" s="60"/>
-      <c r="J112" s="60"/>
-      <c r="K112" s="60"/>
-      <c r="L112" s="60"/>
+    <row r="112" ht="19.5" customHeight="1">
+      <c r="A112" s="7"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="7"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="7"/>
+      <c r="G112" s="7"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="7"/>
+      <c r="J112" s="7"/>
+      <c r="K112" s="7"/>
+      <c r="L112" s="7"/>
       <c r="M112" s="7"/>
       <c r="N112" s="7"/>
       <c r="O112" s="7"/>
@@ -4787,19 +4722,19 @@
       <c r="Y112" s="7"/>
       <c r="Z112" s="7"/>
     </row>
-    <row r="113" ht="24.75" customHeight="1">
-      <c r="A113" s="57"/>
-      <c r="B113" s="31"/>
-      <c r="C113" s="31"/>
-      <c r="D113" s="58"/>
-      <c r="E113" s="54"/>
-      <c r="F113" s="59"/>
-      <c r="G113" s="60"/>
-      <c r="H113" s="60"/>
-      <c r="I113" s="60"/>
-      <c r="J113" s="60"/>
-      <c r="K113" s="60"/>
-      <c r="L113" s="60"/>
+    <row r="113" ht="19.5" customHeight="1">
+      <c r="A113" s="7"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
+      <c r="G113" s="7"/>
+      <c r="H113" s="7"/>
+      <c r="I113" s="7"/>
+      <c r="J113" s="7"/>
+      <c r="K113" s="7"/>
+      <c r="L113" s="7"/>
       <c r="M113" s="7"/>
       <c r="N113" s="7"/>
       <c r="O113" s="7"/>
@@ -4815,19 +4750,19 @@
       <c r="Y113" s="7"/>
       <c r="Z113" s="7"/>
     </row>
-    <row r="114" ht="24.75" customHeight="1">
-      <c r="A114" s="57"/>
-      <c r="B114" s="31"/>
-      <c r="C114" s="31"/>
-      <c r="D114" s="58"/>
-      <c r="E114" s="54"/>
-      <c r="F114" s="59"/>
-      <c r="G114" s="60"/>
-      <c r="H114" s="60"/>
-      <c r="I114" s="60"/>
-      <c r="J114" s="60"/>
-      <c r="K114" s="60"/>
-      <c r="L114" s="60"/>
+    <row r="114" ht="19.5" customHeight="1">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
+      <c r="F114" s="7"/>
+      <c r="G114" s="7"/>
+      <c r="H114" s="7"/>
+      <c r="I114" s="7"/>
+      <c r="J114" s="7"/>
+      <c r="K114" s="7"/>
+      <c r="L114" s="7"/>
       <c r="M114" s="7"/>
       <c r="N114" s="7"/>
       <c r="O114" s="7"/>
@@ -4843,19 +4778,19 @@
       <c r="Y114" s="7"/>
       <c r="Z114" s="7"/>
     </row>
-    <row r="115" ht="24.75" customHeight="1">
-      <c r="A115" s="57"/>
-      <c r="B115" s="31"/>
-      <c r="C115" s="31"/>
-      <c r="D115" s="58"/>
-      <c r="E115" s="54"/>
-      <c r="F115" s="59"/>
-      <c r="G115" s="60"/>
-      <c r="H115" s="60"/>
-      <c r="I115" s="60"/>
-      <c r="J115" s="60"/>
-      <c r="K115" s="60"/>
-      <c r="L115" s="60"/>
+    <row r="115" ht="19.5" customHeight="1">
+      <c r="A115" s="7"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="7"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
+      <c r="H115" s="7"/>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
       <c r="M115" s="7"/>
       <c r="N115" s="7"/>
       <c r="O115" s="7"/>
@@ -4871,19 +4806,19 @@
       <c r="Y115" s="7"/>
       <c r="Z115" s="7"/>
     </row>
-    <row r="116" ht="24.75" customHeight="1">
-      <c r="A116" s="57"/>
-      <c r="B116" s="31"/>
-      <c r="C116" s="31"/>
-      <c r="D116" s="58"/>
-      <c r="E116" s="54"/>
-      <c r="F116" s="59"/>
-      <c r="G116" s="60"/>
-      <c r="H116" s="60"/>
-      <c r="I116" s="60"/>
-      <c r="J116" s="60"/>
-      <c r="K116" s="60"/>
-      <c r="L116" s="60"/>
+    <row r="116" ht="19.5" customHeight="1">
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="7"/>
+      <c r="D116" s="7"/>
+      <c r="E116" s="7"/>
+      <c r="F116" s="7"/>
+      <c r="G116" s="7"/>
+      <c r="H116" s="7"/>
+      <c r="I116" s="7"/>
+      <c r="J116" s="7"/>
+      <c r="K116" s="7"/>
+      <c r="L116" s="7"/>
       <c r="M116" s="7"/>
       <c r="N116" s="7"/>
       <c r="O116" s="7"/>
@@ -4899,19 +4834,19 @@
       <c r="Y116" s="7"/>
       <c r="Z116" s="7"/>
     </row>
-    <row r="117" ht="24.75" customHeight="1">
-      <c r="A117" s="57"/>
-      <c r="B117" s="31"/>
-      <c r="C117" s="31"/>
-      <c r="D117" s="58"/>
-      <c r="E117" s="54"/>
-      <c r="F117" s="59"/>
-      <c r="G117" s="60"/>
-      <c r="H117" s="60"/>
-      <c r="I117" s="60"/>
-      <c r="J117" s="60"/>
-      <c r="K117" s="60"/>
-      <c r="L117" s="60"/>
+    <row r="117" ht="19.5" customHeight="1">
+      <c r="A117" s="7"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="7"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7"/>
+      <c r="G117" s="7"/>
+      <c r="H117" s="7"/>
+      <c r="I117" s="7"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
+      <c r="L117" s="7"/>
       <c r="M117" s="7"/>
       <c r="N117" s="7"/>
       <c r="O117" s="7"/>
@@ -4927,19 +4862,19 @@
       <c r="Y117" s="7"/>
       <c r="Z117" s="7"/>
     </row>
-    <row r="118" ht="24.75" customHeight="1">
-      <c r="A118" s="57"/>
-      <c r="B118" s="31"/>
-      <c r="C118" s="31"/>
-      <c r="D118" s="58"/>
-      <c r="E118" s="54"/>
-      <c r="F118" s="59"/>
-      <c r="G118" s="60"/>
-      <c r="H118" s="60"/>
-      <c r="I118" s="60"/>
-      <c r="J118" s="60"/>
-      <c r="K118" s="60"/>
-      <c r="L118" s="60"/>
+    <row r="118" ht="19.5" customHeight="1">
+      <c r="A118" s="7"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="7"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
+      <c r="F118" s="7"/>
+      <c r="G118" s="7"/>
+      <c r="H118" s="7"/>
+      <c r="I118" s="7"/>
+      <c r="J118" s="7"/>
+      <c r="K118" s="7"/>
+      <c r="L118" s="7"/>
       <c r="M118" s="7"/>
       <c r="N118" s="7"/>
       <c r="O118" s="7"/>
@@ -4955,19 +4890,19 @@
       <c r="Y118" s="7"/>
       <c r="Z118" s="7"/>
     </row>
-    <row r="119" ht="24.75" customHeight="1">
-      <c r="A119" s="57"/>
-      <c r="B119" s="31"/>
-      <c r="C119" s="31"/>
-      <c r="D119" s="58"/>
-      <c r="E119" s="54"/>
-      <c r="F119" s="59"/>
-      <c r="G119" s="60"/>
-      <c r="H119" s="60"/>
-      <c r="I119" s="60"/>
-      <c r="J119" s="60"/>
-      <c r="K119" s="60"/>
-      <c r="L119" s="60"/>
+    <row r="119" ht="19.5" customHeight="1">
+      <c r="A119" s="7"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="7"/>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7"/>
+      <c r="G119" s="7"/>
+      <c r="H119" s="7"/>
+      <c r="I119" s="7"/>
+      <c r="J119" s="7"/>
+      <c r="K119" s="7"/>
+      <c r="L119" s="7"/>
       <c r="M119" s="7"/>
       <c r="N119" s="7"/>
       <c r="O119" s="7"/>
@@ -4983,19 +4918,19 @@
       <c r="Y119" s="7"/>
       <c r="Z119" s="7"/>
     </row>
-    <row r="120" ht="24.75" customHeight="1">
-      <c r="A120" s="57"/>
-      <c r="B120" s="31"/>
-      <c r="C120" s="31"/>
-      <c r="D120" s="58"/>
-      <c r="E120" s="54"/>
-      <c r="F120" s="59"/>
-      <c r="G120" s="60"/>
-      <c r="H120" s="60"/>
-      <c r="I120" s="60"/>
-      <c r="J120" s="60"/>
-      <c r="K120" s="60"/>
-      <c r="L120" s="60"/>
+    <row r="120" ht="19.5" customHeight="1">
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="7"/>
+      <c r="D120" s="7"/>
+      <c r="E120" s="7"/>
+      <c r="F120" s="7"/>
+      <c r="G120" s="7"/>
+      <c r="H120" s="7"/>
+      <c r="I120" s="7"/>
+      <c r="J120" s="7"/>
+      <c r="K120" s="7"/>
+      <c r="L120" s="7"/>
       <c r="M120" s="7"/>
       <c r="N120" s="7"/>
       <c r="O120" s="7"/>
@@ -5011,19 +4946,19 @@
       <c r="Y120" s="7"/>
       <c r="Z120" s="7"/>
     </row>
-    <row r="121" ht="24.75" customHeight="1">
-      <c r="A121" s="57"/>
-      <c r="B121" s="31"/>
-      <c r="C121" s="31"/>
-      <c r="D121" s="58"/>
-      <c r="E121" s="54"/>
-      <c r="F121" s="59"/>
-      <c r="G121" s="60"/>
-      <c r="H121" s="60"/>
-      <c r="I121" s="60"/>
-      <c r="J121" s="60"/>
-      <c r="K121" s="60"/>
-      <c r="L121" s="60"/>
+    <row r="121" ht="19.5" customHeight="1">
+      <c r="A121" s="7"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="7"/>
+      <c r="D121" s="7"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7"/>
+      <c r="G121" s="7"/>
+      <c r="H121" s="7"/>
+      <c r="I121" s="7"/>
+      <c r="J121" s="7"/>
+      <c r="K121" s="7"/>
+      <c r="L121" s="7"/>
       <c r="M121" s="7"/>
       <c r="N121" s="7"/>
       <c r="O121" s="7"/>
@@ -5039,19 +4974,19 @@
       <c r="Y121" s="7"/>
       <c r="Z121" s="7"/>
     </row>
-    <row r="122" ht="24.75" customHeight="1">
-      <c r="A122" s="57"/>
-      <c r="B122" s="31"/>
-      <c r="C122" s="31"/>
-      <c r="D122" s="58"/>
-      <c r="E122" s="54"/>
-      <c r="F122" s="59"/>
-      <c r="G122" s="60"/>
-      <c r="H122" s="60"/>
-      <c r="I122" s="60"/>
-      <c r="J122" s="60"/>
-      <c r="K122" s="60"/>
-      <c r="L122" s="60"/>
+    <row r="122" ht="19.5" customHeight="1">
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="7"/>
+      <c r="D122" s="7"/>
+      <c r="E122" s="7"/>
+      <c r="F122" s="7"/>
+      <c r="G122" s="7"/>
+      <c r="H122" s="7"/>
+      <c r="I122" s="7"/>
+      <c r="J122" s="7"/>
+      <c r="K122" s="7"/>
+      <c r="L122" s="7"/>
       <c r="M122" s="7"/>
       <c r="N122" s="7"/>
       <c r="O122" s="7"/>
@@ -5067,19 +5002,19 @@
       <c r="Y122" s="7"/>
       <c r="Z122" s="7"/>
     </row>
-    <row r="123" ht="24.75" customHeight="1">
-      <c r="A123" s="57"/>
-      <c r="B123" s="31"/>
-      <c r="C123" s="31"/>
-      <c r="D123" s="58"/>
-      <c r="E123" s="54"/>
-      <c r="F123" s="59"/>
-      <c r="G123" s="60"/>
-      <c r="H123" s="60"/>
-      <c r="I123" s="60"/>
-      <c r="J123" s="60"/>
-      <c r="K123" s="60"/>
-      <c r="L123" s="60"/>
+    <row r="123" ht="19.5" customHeight="1">
+      <c r="A123" s="7"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="7"/>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7"/>
+      <c r="G123" s="7"/>
+      <c r="H123" s="7"/>
+      <c r="I123" s="7"/>
+      <c r="J123" s="7"/>
+      <c r="K123" s="7"/>
+      <c r="L123" s="7"/>
       <c r="M123" s="7"/>
       <c r="N123" s="7"/>
       <c r="O123" s="7"/>
@@ -5095,19 +5030,19 @@
       <c r="Y123" s="7"/>
       <c r="Z123" s="7"/>
     </row>
-    <row r="124" ht="24.75" customHeight="1">
-      <c r="A124" s="57"/>
-      <c r="B124" s="31"/>
-      <c r="C124" s="31"/>
-      <c r="D124" s="58"/>
-      <c r="E124" s="54"/>
-      <c r="F124" s="59"/>
-      <c r="G124" s="60"/>
-      <c r="H124" s="60"/>
-      <c r="I124" s="60"/>
-      <c r="J124" s="60"/>
-      <c r="K124" s="60"/>
-      <c r="L124" s="60"/>
+    <row r="124" ht="19.5" customHeight="1">
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="7"/>
+      <c r="D124" s="7"/>
+      <c r="E124" s="7"/>
+      <c r="F124" s="7"/>
+      <c r="G124" s="7"/>
+      <c r="H124" s="7"/>
+      <c r="I124" s="7"/>
+      <c r="J124" s="7"/>
+      <c r="K124" s="7"/>
+      <c r="L124" s="7"/>
       <c r="M124" s="7"/>
       <c r="N124" s="7"/>
       <c r="O124" s="7"/>
@@ -5123,19 +5058,19 @@
       <c r="Y124" s="7"/>
       <c r="Z124" s="7"/>
     </row>
-    <row r="125" ht="24.75" customHeight="1">
-      <c r="A125" s="57"/>
-      <c r="B125" s="31"/>
-      <c r="C125" s="31"/>
-      <c r="D125" s="58"/>
-      <c r="E125" s="54"/>
-      <c r="F125" s="59"/>
-      <c r="G125" s="60"/>
-      <c r="H125" s="60"/>
-      <c r="I125" s="60"/>
-      <c r="J125" s="60"/>
-      <c r="K125" s="60"/>
-      <c r="L125" s="60"/>
+    <row r="125" ht="19.5" customHeight="1">
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="7"/>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7"/>
+      <c r="G125" s="7"/>
+      <c r="H125" s="7"/>
+      <c r="I125" s="7"/>
+      <c r="J125" s="7"/>
+      <c r="K125" s="7"/>
+      <c r="L125" s="7"/>
       <c r="M125" s="7"/>
       <c r="N125" s="7"/>
       <c r="O125" s="7"/>
@@ -5151,19 +5086,19 @@
       <c r="Y125" s="7"/>
       <c r="Z125" s="7"/>
     </row>
-    <row r="126" ht="24.75" customHeight="1">
-      <c r="A126" s="57"/>
-      <c r="B126" s="31"/>
-      <c r="C126" s="31"/>
-      <c r="D126" s="58"/>
-      <c r="E126" s="54"/>
-      <c r="F126" s="59"/>
-      <c r="G126" s="60"/>
-      <c r="H126" s="60"/>
-      <c r="I126" s="60"/>
-      <c r="J126" s="60"/>
-      <c r="K126" s="60"/>
-      <c r="L126" s="60"/>
+    <row r="126" ht="19.5" customHeight="1">
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+      <c r="F126" s="7"/>
+      <c r="G126" s="7"/>
+      <c r="H126" s="7"/>
+      <c r="I126" s="7"/>
+      <c r="J126" s="7"/>
+      <c r="K126" s="7"/>
+      <c r="L126" s="7"/>
       <c r="M126" s="7"/>
       <c r="N126" s="7"/>
       <c r="O126" s="7"/>
@@ -5179,19 +5114,19 @@
       <c r="Y126" s="7"/>
       <c r="Z126" s="7"/>
     </row>
-    <row r="127" ht="24.75" customHeight="1">
-      <c r="A127" s="57"/>
-      <c r="B127" s="31"/>
-      <c r="C127" s="31"/>
-      <c r="D127" s="58"/>
-      <c r="E127" s="54"/>
-      <c r="F127" s="59"/>
-      <c r="G127" s="60"/>
-      <c r="H127" s="60"/>
-      <c r="I127" s="60"/>
-      <c r="J127" s="60"/>
-      <c r="K127" s="60"/>
-      <c r="L127" s="60"/>
+    <row r="127" ht="19.5" customHeight="1">
+      <c r="A127" s="7"/>
+      <c r="B127" s="7"/>
+      <c r="C127" s="7"/>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7"/>
+      <c r="G127" s="7"/>
+      <c r="H127" s="7"/>
+      <c r="I127" s="7"/>
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+      <c r="L127" s="7"/>
       <c r="M127" s="7"/>
       <c r="N127" s="7"/>
       <c r="O127" s="7"/>
@@ -5207,19 +5142,19 @@
       <c r="Y127" s="7"/>
       <c r="Z127" s="7"/>
     </row>
-    <row r="128" ht="24.75" customHeight="1">
-      <c r="A128" s="57"/>
-      <c r="B128" s="31"/>
-      <c r="C128" s="31"/>
-      <c r="D128" s="58"/>
-      <c r="E128" s="54"/>
-      <c r="F128" s="59"/>
-      <c r="G128" s="60"/>
-      <c r="H128" s="60"/>
-      <c r="I128" s="60"/>
-      <c r="J128" s="60"/>
-      <c r="K128" s="60"/>
-      <c r="L128" s="60"/>
+    <row r="128" ht="19.5" customHeight="1">
+      <c r="A128" s="7"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="7"/>
+      <c r="D128" s="7"/>
+      <c r="E128" s="7"/>
+      <c r="F128" s="7"/>
+      <c r="G128" s="7"/>
+      <c r="H128" s="7"/>
+      <c r="I128" s="7"/>
+      <c r="J128" s="7"/>
+      <c r="K128" s="7"/>
+      <c r="L128" s="7"/>
       <c r="M128" s="7"/>
       <c r="N128" s="7"/>
       <c r="O128" s="7"/>
@@ -5235,19 +5170,19 @@
       <c r="Y128" s="7"/>
       <c r="Z128" s="7"/>
     </row>
-    <row r="129" ht="26.25" customHeight="1">
-      <c r="A129" s="61"/>
-      <c r="B129" s="62"/>
-      <c r="C129" s="62"/>
-      <c r="D129" s="63"/>
-      <c r="E129" s="64"/>
-      <c r="F129" s="65"/>
-      <c r="G129" s="66"/>
-      <c r="H129" s="66"/>
-      <c r="I129" s="66"/>
-      <c r="J129" s="66"/>
-      <c r="K129" s="66"/>
-      <c r="L129" s="66"/>
+    <row r="129" ht="19.5" customHeight="1">
+      <c r="A129" s="7"/>
+      <c r="B129" s="7"/>
+      <c r="C129" s="7"/>
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7"/>
+      <c r="G129" s="7"/>
+      <c r="H129" s="7"/>
+      <c r="I129" s="7"/>
+      <c r="J129" s="7"/>
+      <c r="K129" s="7"/>
+      <c r="L129" s="7"/>
       <c r="M129" s="7"/>
       <c r="N129" s="7"/>
       <c r="O129" s="7"/>
@@ -5263,19 +5198,19 @@
       <c r="Y129" s="7"/>
       <c r="Z129" s="7"/>
     </row>
-    <row r="130" ht="28.5" customHeight="1">
-      <c r="A130" s="67"/>
-      <c r="B130" s="68"/>
-      <c r="C130" s="68"/>
-      <c r="D130" s="69"/>
-      <c r="E130" s="70"/>
-      <c r="F130" s="71"/>
-      <c r="G130" s="72"/>
-      <c r="H130" s="72"/>
-      <c r="I130" s="72"/>
-      <c r="J130" s="72"/>
-      <c r="K130" s="72"/>
-      <c r="L130" s="72"/>
+    <row r="130" ht="19.5" customHeight="1">
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="7"/>
+      <c r="D130" s="7"/>
+      <c r="E130" s="7"/>
+      <c r="F130" s="7"/>
+      <c r="G130" s="7"/>
+      <c r="H130" s="7"/>
+      <c r="I130" s="7"/>
+      <c r="J130" s="7"/>
+      <c r="K130" s="7"/>
+      <c r="L130" s="7"/>
       <c r="M130" s="7"/>
       <c r="N130" s="7"/>
       <c r="O130" s="7"/>
@@ -5291,29 +5226,19 @@
       <c r="Y130" s="7"/>
       <c r="Z130" s="7"/>
     </row>
-    <row r="131" ht="26.25" customHeight="1">
-      <c r="A131" s="73"/>
-      <c r="B131" s="74"/>
-      <c r="C131" s="74"/>
-      <c r="D131" s="75"/>
-      <c r="E131" s="76"/>
-      <c r="F131" s="77"/>
-      <c r="G131" s="78" t="s">
-        <v>104</v>
-      </c>
-      <c r="H131" s="79"/>
-      <c r="I131" s="78" t="s">
-        <v>105</v>
-      </c>
-      <c r="J131" s="78" t="s">
-        <v>106</v>
-      </c>
-      <c r="K131" s="78" t="s">
-        <v>107</v>
-      </c>
-      <c r="L131" s="78" t="s">
-        <v>108</v>
-      </c>
+    <row r="131" ht="19.5" customHeight="1">
+      <c r="A131" s="7"/>
+      <c r="B131" s="7"/>
+      <c r="C131" s="7"/>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+      <c r="F131" s="7"/>
+      <c r="G131" s="7"/>
+      <c r="H131" s="7"/>
+      <c r="I131" s="7"/>
+      <c r="J131" s="7"/>
+      <c r="K131" s="7"/>
+      <c r="L131" s="7"/>
       <c r="M131" s="7"/>
       <c r="N131" s="7"/>
       <c r="O131" s="7"/>
@@ -5329,25 +5254,19 @@
       <c r="Y131" s="7"/>
       <c r="Z131" s="7"/>
     </row>
-    <row r="132" ht="43.5" customHeight="1">
-      <c r="A132" s="80"/>
-      <c r="B132" s="81"/>
-      <c r="C132" s="81"/>
-      <c r="D132" s="82"/>
-      <c r="E132" s="83"/>
-      <c r="F132" s="84"/>
-      <c r="G132" s="85" t="s">
-        <v>109</v>
-      </c>
-      <c r="H132" s="85" t="s">
-        <v>109</v>
-      </c>
-      <c r="I132" s="85" t="s">
-        <v>110</v>
-      </c>
-      <c r="J132" s="86"/>
-      <c r="K132" s="86"/>
-      <c r="L132" s="86"/>
+    <row r="132" ht="19.5" customHeight="1">
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="7"/>
+      <c r="D132" s="7"/>
+      <c r="E132" s="7"/>
+      <c r="F132" s="7"/>
+      <c r="G132" s="7"/>
+      <c r="H132" s="7"/>
+      <c r="I132" s="7"/>
+      <c r="J132" s="7"/>
+      <c r="K132" s="7"/>
+      <c r="L132" s="7"/>
       <c r="M132" s="7"/>
       <c r="N132" s="7"/>
       <c r="O132" s="7"/>
@@ -5363,25 +5282,19 @@
       <c r="Y132" s="7"/>
       <c r="Z132" s="7"/>
     </row>
-    <row r="133" ht="43.5" customHeight="1">
-      <c r="A133" s="80"/>
-      <c r="B133" s="81"/>
-      <c r="C133" s="81"/>
-      <c r="D133" s="82"/>
-      <c r="E133" s="83"/>
-      <c r="F133" s="84"/>
-      <c r="G133" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="H133" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="I133" s="85" t="s">
-        <v>113</v>
-      </c>
-      <c r="J133" s="86"/>
-      <c r="K133" s="86"/>
-      <c r="L133" s="86"/>
+    <row r="133" ht="19.5" customHeight="1">
+      <c r="A133" s="7"/>
+      <c r="B133" s="7"/>
+      <c r="C133" s="7"/>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7"/>
+      <c r="G133" s="7"/>
+      <c r="H133" s="7"/>
+      <c r="I133" s="7"/>
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+      <c r="L133" s="7"/>
       <c r="M133" s="7"/>
       <c r="N133" s="7"/>
       <c r="O133" s="7"/>
@@ -5397,21 +5310,19 @@
       <c r="Y133" s="7"/>
       <c r="Z133" s="7"/>
     </row>
-    <row r="134" ht="24.75" customHeight="1">
-      <c r="A134" s="80"/>
-      <c r="B134" s="81"/>
-      <c r="C134" s="81"/>
-      <c r="D134" s="82"/>
-      <c r="E134" s="83"/>
-      <c r="F134" s="84"/>
-      <c r="G134" s="85" t="s">
-        <v>114</v>
-      </c>
-      <c r="H134" s="86"/>
-      <c r="I134" s="86"/>
-      <c r="J134" s="86"/>
-      <c r="K134" s="86"/>
-      <c r="L134" s="86"/>
+    <row r="134" ht="19.5" customHeight="1">
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="7"/>
+      <c r="D134" s="7"/>
+      <c r="E134" s="7"/>
+      <c r="F134" s="7"/>
+      <c r="G134" s="7"/>
+      <c r="H134" s="7"/>
+      <c r="I134" s="7"/>
+      <c r="J134" s="7"/>
+      <c r="K134" s="7"/>
+      <c r="L134" s="7"/>
       <c r="M134" s="7"/>
       <c r="N134" s="7"/>
       <c r="O134" s="7"/>
@@ -29199,734 +29110,6 @@
       <c r="Y983" s="7"/>
       <c r="Z983" s="7"/>
     </row>
-    <row r="984" ht="19.5" customHeight="1">
-      <c r="A984" s="7"/>
-      <c r="B984" s="7"/>
-      <c r="C984" s="7"/>
-      <c r="D984" s="7"/>
-      <c r="E984" s="7"/>
-      <c r="F984" s="7"/>
-      <c r="G984" s="7"/>
-      <c r="H984" s="7"/>
-      <c r="I984" s="7"/>
-      <c r="J984" s="7"/>
-      <c r="K984" s="7"/>
-      <c r="L984" s="7"/>
-      <c r="M984" s="7"/>
-      <c r="N984" s="7"/>
-      <c r="O984" s="7"/>
-      <c r="P984" s="7"/>
-      <c r="Q984" s="7"/>
-      <c r="R984" s="7"/>
-      <c r="S984" s="7"/>
-      <c r="T984" s="7"/>
-      <c r="U984" s="7"/>
-      <c r="V984" s="7"/>
-      <c r="W984" s="7"/>
-      <c r="X984" s="7"/>
-      <c r="Y984" s="7"/>
-      <c r="Z984" s="7"/>
-    </row>
-    <row r="985" ht="19.5" customHeight="1">
-      <c r="A985" s="7"/>
-      <c r="B985" s="7"/>
-      <c r="C985" s="7"/>
-      <c r="D985" s="7"/>
-      <c r="E985" s="7"/>
-      <c r="F985" s="7"/>
-      <c r="G985" s="7"/>
-      <c r="H985" s="7"/>
-      <c r="I985" s="7"/>
-      <c r="J985" s="7"/>
-      <c r="K985" s="7"/>
-      <c r="L985" s="7"/>
-      <c r="M985" s="7"/>
-      <c r="N985" s="7"/>
-      <c r="O985" s="7"/>
-      <c r="P985" s="7"/>
-      <c r="Q985" s="7"/>
-      <c r="R985" s="7"/>
-      <c r="S985" s="7"/>
-      <c r="T985" s="7"/>
-      <c r="U985" s="7"/>
-      <c r="V985" s="7"/>
-      <c r="W985" s="7"/>
-      <c r="X985" s="7"/>
-      <c r="Y985" s="7"/>
-      <c r="Z985" s="7"/>
-    </row>
-    <row r="986" ht="19.5" customHeight="1">
-      <c r="A986" s="7"/>
-      <c r="B986" s="7"/>
-      <c r="C986" s="7"/>
-      <c r="D986" s="7"/>
-      <c r="E986" s="7"/>
-      <c r="F986" s="7"/>
-      <c r="G986" s="7"/>
-      <c r="H986" s="7"/>
-      <c r="I986" s="7"/>
-      <c r="J986" s="7"/>
-      <c r="K986" s="7"/>
-      <c r="L986" s="7"/>
-      <c r="M986" s="7"/>
-      <c r="N986" s="7"/>
-      <c r="O986" s="7"/>
-      <c r="P986" s="7"/>
-      <c r="Q986" s="7"/>
-      <c r="R986" s="7"/>
-      <c r="S986" s="7"/>
-      <c r="T986" s="7"/>
-      <c r="U986" s="7"/>
-      <c r="V986" s="7"/>
-      <c r="W986" s="7"/>
-      <c r="X986" s="7"/>
-      <c r="Y986" s="7"/>
-      <c r="Z986" s="7"/>
-    </row>
-    <row r="987" ht="19.5" customHeight="1">
-      <c r="A987" s="7"/>
-      <c r="B987" s="7"/>
-      <c r="C987" s="7"/>
-      <c r="D987" s="7"/>
-      <c r="E987" s="7"/>
-      <c r="F987" s="7"/>
-      <c r="G987" s="7"/>
-      <c r="H987" s="7"/>
-      <c r="I987" s="7"/>
-      <c r="J987" s="7"/>
-      <c r="K987" s="7"/>
-      <c r="L987" s="7"/>
-      <c r="M987" s="7"/>
-      <c r="N987" s="7"/>
-      <c r="O987" s="7"/>
-      <c r="P987" s="7"/>
-      <c r="Q987" s="7"/>
-      <c r="R987" s="7"/>
-      <c r="S987" s="7"/>
-      <c r="T987" s="7"/>
-      <c r="U987" s="7"/>
-      <c r="V987" s="7"/>
-      <c r="W987" s="7"/>
-      <c r="X987" s="7"/>
-      <c r="Y987" s="7"/>
-      <c r="Z987" s="7"/>
-    </row>
-    <row r="988" ht="19.5" customHeight="1">
-      <c r="A988" s="7"/>
-      <c r="B988" s="7"/>
-      <c r="C988" s="7"/>
-      <c r="D988" s="7"/>
-      <c r="E988" s="7"/>
-      <c r="F988" s="7"/>
-      <c r="G988" s="7"/>
-      <c r="H988" s="7"/>
-      <c r="I988" s="7"/>
-      <c r="J988" s="7"/>
-      <c r="K988" s="7"/>
-      <c r="L988" s="7"/>
-      <c r="M988" s="7"/>
-      <c r="N988" s="7"/>
-      <c r="O988" s="7"/>
-      <c r="P988" s="7"/>
-      <c r="Q988" s="7"/>
-      <c r="R988" s="7"/>
-      <c r="S988" s="7"/>
-      <c r="T988" s="7"/>
-      <c r="U988" s="7"/>
-      <c r="V988" s="7"/>
-      <c r="W988" s="7"/>
-      <c r="X988" s="7"/>
-      <c r="Y988" s="7"/>
-      <c r="Z988" s="7"/>
-    </row>
-    <row r="989" ht="19.5" customHeight="1">
-      <c r="A989" s="7"/>
-      <c r="B989" s="7"/>
-      <c r="C989" s="7"/>
-      <c r="D989" s="7"/>
-      <c r="E989" s="7"/>
-      <c r="F989" s="7"/>
-      <c r="G989" s="7"/>
-      <c r="H989" s="7"/>
-      <c r="I989" s="7"/>
-      <c r="J989" s="7"/>
-      <c r="K989" s="7"/>
-      <c r="L989" s="7"/>
-      <c r="M989" s="7"/>
-      <c r="N989" s="7"/>
-      <c r="O989" s="7"/>
-      <c r="P989" s="7"/>
-      <c r="Q989" s="7"/>
-      <c r="R989" s="7"/>
-      <c r="S989" s="7"/>
-      <c r="T989" s="7"/>
-      <c r="U989" s="7"/>
-      <c r="V989" s="7"/>
-      <c r="W989" s="7"/>
-      <c r="X989" s="7"/>
-      <c r="Y989" s="7"/>
-      <c r="Z989" s="7"/>
-    </row>
-    <row r="990" ht="19.5" customHeight="1">
-      <c r="A990" s="7"/>
-      <c r="B990" s="7"/>
-      <c r="C990" s="7"/>
-      <c r="D990" s="7"/>
-      <c r="E990" s="7"/>
-      <c r="F990" s="7"/>
-      <c r="G990" s="7"/>
-      <c r="H990" s="7"/>
-      <c r="I990" s="7"/>
-      <c r="J990" s="7"/>
-      <c r="K990" s="7"/>
-      <c r="L990" s="7"/>
-      <c r="M990" s="7"/>
-      <c r="N990" s="7"/>
-      <c r="O990" s="7"/>
-      <c r="P990" s="7"/>
-      <c r="Q990" s="7"/>
-      <c r="R990" s="7"/>
-      <c r="S990" s="7"/>
-      <c r="T990" s="7"/>
-      <c r="U990" s="7"/>
-      <c r="V990" s="7"/>
-      <c r="W990" s="7"/>
-      <c r="X990" s="7"/>
-      <c r="Y990" s="7"/>
-      <c r="Z990" s="7"/>
-    </row>
-    <row r="991" ht="19.5" customHeight="1">
-      <c r="A991" s="7"/>
-      <c r="B991" s="7"/>
-      <c r="C991" s="7"/>
-      <c r="D991" s="7"/>
-      <c r="E991" s="7"/>
-      <c r="F991" s="7"/>
-      <c r="G991" s="7"/>
-      <c r="H991" s="7"/>
-      <c r="I991" s="7"/>
-      <c r="J991" s="7"/>
-      <c r="K991" s="7"/>
-      <c r="L991" s="7"/>
-      <c r="M991" s="7"/>
-      <c r="N991" s="7"/>
-      <c r="O991" s="7"/>
-      <c r="P991" s="7"/>
-      <c r="Q991" s="7"/>
-      <c r="R991" s="7"/>
-      <c r="S991" s="7"/>
-      <c r="T991" s="7"/>
-      <c r="U991" s="7"/>
-      <c r="V991" s="7"/>
-      <c r="W991" s="7"/>
-      <c r="X991" s="7"/>
-      <c r="Y991" s="7"/>
-      <c r="Z991" s="7"/>
-    </row>
-    <row r="992" ht="19.5" customHeight="1">
-      <c r="A992" s="7"/>
-      <c r="B992" s="7"/>
-      <c r="C992" s="7"/>
-      <c r="D992" s="7"/>
-      <c r="E992" s="7"/>
-      <c r="F992" s="7"/>
-      <c r="G992" s="7"/>
-      <c r="H992" s="7"/>
-      <c r="I992" s="7"/>
-      <c r="J992" s="7"/>
-      <c r="K992" s="7"/>
-      <c r="L992" s="7"/>
-      <c r="M992" s="7"/>
-      <c r="N992" s="7"/>
-      <c r="O992" s="7"/>
-      <c r="P992" s="7"/>
-      <c r="Q992" s="7"/>
-      <c r="R992" s="7"/>
-      <c r="S992" s="7"/>
-      <c r="T992" s="7"/>
-      <c r="U992" s="7"/>
-      <c r="V992" s="7"/>
-      <c r="W992" s="7"/>
-      <c r="X992" s="7"/>
-      <c r="Y992" s="7"/>
-      <c r="Z992" s="7"/>
-    </row>
-    <row r="993" ht="19.5" customHeight="1">
-      <c r="A993" s="7"/>
-      <c r="B993" s="7"/>
-      <c r="C993" s="7"/>
-      <c r="D993" s="7"/>
-      <c r="E993" s="7"/>
-      <c r="F993" s="7"/>
-      <c r="G993" s="7"/>
-      <c r="H993" s="7"/>
-      <c r="I993" s="7"/>
-      <c r="J993" s="7"/>
-      <c r="K993" s="7"/>
-      <c r="L993" s="7"/>
-      <c r="M993" s="7"/>
-      <c r="N993" s="7"/>
-      <c r="O993" s="7"/>
-      <c r="P993" s="7"/>
-      <c r="Q993" s="7"/>
-      <c r="R993" s="7"/>
-      <c r="S993" s="7"/>
-      <c r="T993" s="7"/>
-      <c r="U993" s="7"/>
-      <c r="V993" s="7"/>
-      <c r="W993" s="7"/>
-      <c r="X993" s="7"/>
-      <c r="Y993" s="7"/>
-      <c r="Z993" s="7"/>
-    </row>
-    <row r="994" ht="19.5" customHeight="1">
-      <c r="A994" s="7"/>
-      <c r="B994" s="7"/>
-      <c r="C994" s="7"/>
-      <c r="D994" s="7"/>
-      <c r="E994" s="7"/>
-      <c r="F994" s="7"/>
-      <c r="G994" s="7"/>
-      <c r="H994" s="7"/>
-      <c r="I994" s="7"/>
-      <c r="J994" s="7"/>
-      <c r="K994" s="7"/>
-      <c r="L994" s="7"/>
-      <c r="M994" s="7"/>
-      <c r="N994" s="7"/>
-      <c r="O994" s="7"/>
-      <c r="P994" s="7"/>
-      <c r="Q994" s="7"/>
-      <c r="R994" s="7"/>
-      <c r="S994" s="7"/>
-      <c r="T994" s="7"/>
-      <c r="U994" s="7"/>
-      <c r="V994" s="7"/>
-      <c r="W994" s="7"/>
-      <c r="X994" s="7"/>
-      <c r="Y994" s="7"/>
-      <c r="Z994" s="7"/>
-    </row>
-    <row r="995" ht="19.5" customHeight="1">
-      <c r="A995" s="7"/>
-      <c r="B995" s="7"/>
-      <c r="C995" s="7"/>
-      <c r="D995" s="7"/>
-      <c r="E995" s="7"/>
-      <c r="F995" s="7"/>
-      <c r="G995" s="7"/>
-      <c r="H995" s="7"/>
-      <c r="I995" s="7"/>
-      <c r="J995" s="7"/>
-      <c r="K995" s="7"/>
-      <c r="L995" s="7"/>
-      <c r="M995" s="7"/>
-      <c r="N995" s="7"/>
-      <c r="O995" s="7"/>
-      <c r="P995" s="7"/>
-      <c r="Q995" s="7"/>
-      <c r="R995" s="7"/>
-      <c r="S995" s="7"/>
-      <c r="T995" s="7"/>
-      <c r="U995" s="7"/>
-      <c r="V995" s="7"/>
-      <c r="W995" s="7"/>
-      <c r="X995" s="7"/>
-      <c r="Y995" s="7"/>
-      <c r="Z995" s="7"/>
-    </row>
-    <row r="996" ht="19.5" customHeight="1">
-      <c r="A996" s="7"/>
-      <c r="B996" s="7"/>
-      <c r="C996" s="7"/>
-      <c r="D996" s="7"/>
-      <c r="E996" s="7"/>
-      <c r="F996" s="7"/>
-      <c r="G996" s="7"/>
-      <c r="H996" s="7"/>
-      <c r="I996" s="7"/>
-      <c r="J996" s="7"/>
-      <c r="K996" s="7"/>
-      <c r="L996" s="7"/>
-      <c r="M996" s="7"/>
-      <c r="N996" s="7"/>
-      <c r="O996" s="7"/>
-      <c r="P996" s="7"/>
-      <c r="Q996" s="7"/>
-      <c r="R996" s="7"/>
-      <c r="S996" s="7"/>
-      <c r="T996" s="7"/>
-      <c r="U996" s="7"/>
-      <c r="V996" s="7"/>
-      <c r="W996" s="7"/>
-      <c r="X996" s="7"/>
-      <c r="Y996" s="7"/>
-      <c r="Z996" s="7"/>
-    </row>
-    <row r="997" ht="19.5" customHeight="1">
-      <c r="A997" s="7"/>
-      <c r="B997" s="7"/>
-      <c r="C997" s="7"/>
-      <c r="D997" s="7"/>
-      <c r="E997" s="7"/>
-      <c r="F997" s="7"/>
-      <c r="G997" s="7"/>
-      <c r="H997" s="7"/>
-      <c r="I997" s="7"/>
-      <c r="J997" s="7"/>
-      <c r="K997" s="7"/>
-      <c r="L997" s="7"/>
-      <c r="M997" s="7"/>
-      <c r="N997" s="7"/>
-      <c r="O997" s="7"/>
-      <c r="P997" s="7"/>
-      <c r="Q997" s="7"/>
-      <c r="R997" s="7"/>
-      <c r="S997" s="7"/>
-      <c r="T997" s="7"/>
-      <c r="U997" s="7"/>
-      <c r="V997" s="7"/>
-      <c r="W997" s="7"/>
-      <c r="X997" s="7"/>
-      <c r="Y997" s="7"/>
-      <c r="Z997" s="7"/>
-    </row>
-    <row r="998" ht="19.5" customHeight="1">
-      <c r="A998" s="7"/>
-      <c r="B998" s="7"/>
-      <c r="C998" s="7"/>
-      <c r="D998" s="7"/>
-      <c r="E998" s="7"/>
-      <c r="F998" s="7"/>
-      <c r="G998" s="7"/>
-      <c r="H998" s="7"/>
-      <c r="I998" s="7"/>
-      <c r="J998" s="7"/>
-      <c r="K998" s="7"/>
-      <c r="L998" s="7"/>
-      <c r="M998" s="7"/>
-      <c r="N998" s="7"/>
-      <c r="O998" s="7"/>
-      <c r="P998" s="7"/>
-      <c r="Q998" s="7"/>
-      <c r="R998" s="7"/>
-      <c r="S998" s="7"/>
-      <c r="T998" s="7"/>
-      <c r="U998" s="7"/>
-      <c r="V998" s="7"/>
-      <c r="W998" s="7"/>
-      <c r="X998" s="7"/>
-      <c r="Y998" s="7"/>
-      <c r="Z998" s="7"/>
-    </row>
-    <row r="999" ht="19.5" customHeight="1">
-      <c r="A999" s="7"/>
-      <c r="B999" s="7"/>
-      <c r="C999" s="7"/>
-      <c r="D999" s="7"/>
-      <c r="E999" s="7"/>
-      <c r="F999" s="7"/>
-      <c r="G999" s="7"/>
-      <c r="H999" s="7"/>
-      <c r="I999" s="7"/>
-      <c r="J999" s="7"/>
-      <c r="K999" s="7"/>
-      <c r="L999" s="7"/>
-      <c r="M999" s="7"/>
-      <c r="N999" s="7"/>
-      <c r="O999" s="7"/>
-      <c r="P999" s="7"/>
-      <c r="Q999" s="7"/>
-      <c r="R999" s="7"/>
-      <c r="S999" s="7"/>
-      <c r="T999" s="7"/>
-      <c r="U999" s="7"/>
-      <c r="V999" s="7"/>
-      <c r="W999" s="7"/>
-      <c r="X999" s="7"/>
-      <c r="Y999" s="7"/>
-      <c r="Z999" s="7"/>
-    </row>
-    <row r="1000" ht="19.5" customHeight="1">
-      <c r="A1000" s="7"/>
-      <c r="B1000" s="7"/>
-      <c r="C1000" s="7"/>
-      <c r="D1000" s="7"/>
-      <c r="E1000" s="7"/>
-      <c r="F1000" s="7"/>
-      <c r="G1000" s="7"/>
-      <c r="H1000" s="7"/>
-      <c r="I1000" s="7"/>
-      <c r="J1000" s="7"/>
-      <c r="K1000" s="7"/>
-      <c r="L1000" s="7"/>
-      <c r="M1000" s="7"/>
-      <c r="N1000" s="7"/>
-      <c r="O1000" s="7"/>
-      <c r="P1000" s="7"/>
-      <c r="Q1000" s="7"/>
-      <c r="R1000" s="7"/>
-      <c r="S1000" s="7"/>
-      <c r="T1000" s="7"/>
-      <c r="U1000" s="7"/>
-      <c r="V1000" s="7"/>
-      <c r="W1000" s="7"/>
-      <c r="X1000" s="7"/>
-      <c r="Y1000" s="7"/>
-      <c r="Z1000" s="7"/>
-    </row>
-    <row r="1001" ht="19.5" customHeight="1">
-      <c r="A1001" s="7"/>
-      <c r="B1001" s="7"/>
-      <c r="C1001" s="7"/>
-      <c r="D1001" s="7"/>
-      <c r="E1001" s="7"/>
-      <c r="F1001" s="7"/>
-      <c r="G1001" s="7"/>
-      <c r="H1001" s="7"/>
-      <c r="I1001" s="7"/>
-      <c r="J1001" s="7"/>
-      <c r="K1001" s="7"/>
-      <c r="L1001" s="7"/>
-      <c r="M1001" s="7"/>
-      <c r="N1001" s="7"/>
-      <c r="O1001" s="7"/>
-      <c r="P1001" s="7"/>
-      <c r="Q1001" s="7"/>
-      <c r="R1001" s="7"/>
-      <c r="S1001" s="7"/>
-      <c r="T1001" s="7"/>
-      <c r="U1001" s="7"/>
-      <c r="V1001" s="7"/>
-      <c r="W1001" s="7"/>
-      <c r="X1001" s="7"/>
-      <c r="Y1001" s="7"/>
-      <c r="Z1001" s="7"/>
-    </row>
-    <row r="1002" ht="19.5" customHeight="1">
-      <c r="A1002" s="7"/>
-      <c r="B1002" s="7"/>
-      <c r="C1002" s="7"/>
-      <c r="D1002" s="7"/>
-      <c r="E1002" s="7"/>
-      <c r="F1002" s="7"/>
-      <c r="G1002" s="7"/>
-      <c r="H1002" s="7"/>
-      <c r="I1002" s="7"/>
-      <c r="J1002" s="7"/>
-      <c r="K1002" s="7"/>
-      <c r="L1002" s="7"/>
-      <c r="M1002" s="7"/>
-      <c r="N1002" s="7"/>
-      <c r="O1002" s="7"/>
-      <c r="P1002" s="7"/>
-      <c r="Q1002" s="7"/>
-      <c r="R1002" s="7"/>
-      <c r="S1002" s="7"/>
-      <c r="T1002" s="7"/>
-      <c r="U1002" s="7"/>
-      <c r="V1002" s="7"/>
-      <c r="W1002" s="7"/>
-      <c r="X1002" s="7"/>
-      <c r="Y1002" s="7"/>
-      <c r="Z1002" s="7"/>
-    </row>
-    <row r="1003" ht="19.5" customHeight="1">
-      <c r="A1003" s="7"/>
-      <c r="B1003" s="7"/>
-      <c r="C1003" s="7"/>
-      <c r="D1003" s="7"/>
-      <c r="E1003" s="7"/>
-      <c r="F1003" s="7"/>
-      <c r="G1003" s="7"/>
-      <c r="H1003" s="7"/>
-      <c r="I1003" s="7"/>
-      <c r="J1003" s="7"/>
-      <c r="K1003" s="7"/>
-      <c r="L1003" s="7"/>
-      <c r="M1003" s="7"/>
-      <c r="N1003" s="7"/>
-      <c r="O1003" s="7"/>
-      <c r="P1003" s="7"/>
-      <c r="Q1003" s="7"/>
-      <c r="R1003" s="7"/>
-      <c r="S1003" s="7"/>
-      <c r="T1003" s="7"/>
-      <c r="U1003" s="7"/>
-      <c r="V1003" s="7"/>
-      <c r="W1003" s="7"/>
-      <c r="X1003" s="7"/>
-      <c r="Y1003" s="7"/>
-      <c r="Z1003" s="7"/>
-    </row>
-    <row r="1004" ht="19.5" customHeight="1">
-      <c r="A1004" s="7"/>
-      <c r="B1004" s="7"/>
-      <c r="C1004" s="7"/>
-      <c r="D1004" s="7"/>
-      <c r="E1004" s="7"/>
-      <c r="F1004" s="7"/>
-      <c r="G1004" s="7"/>
-      <c r="H1004" s="7"/>
-      <c r="I1004" s="7"/>
-      <c r="J1004" s="7"/>
-      <c r="K1004" s="7"/>
-      <c r="L1004" s="7"/>
-      <c r="M1004" s="7"/>
-      <c r="N1004" s="7"/>
-      <c r="O1004" s="7"/>
-      <c r="P1004" s="7"/>
-      <c r="Q1004" s="7"/>
-      <c r="R1004" s="7"/>
-      <c r="S1004" s="7"/>
-      <c r="T1004" s="7"/>
-      <c r="U1004" s="7"/>
-      <c r="V1004" s="7"/>
-      <c r="W1004" s="7"/>
-      <c r="X1004" s="7"/>
-      <c r="Y1004" s="7"/>
-      <c r="Z1004" s="7"/>
-    </row>
-    <row r="1005" ht="19.5" customHeight="1">
-      <c r="A1005" s="7"/>
-      <c r="B1005" s="7"/>
-      <c r="C1005" s="7"/>
-      <c r="D1005" s="7"/>
-      <c r="E1005" s="7"/>
-      <c r="F1005" s="7"/>
-      <c r="G1005" s="7"/>
-      <c r="H1005" s="7"/>
-      <c r="I1005" s="7"/>
-      <c r="J1005" s="7"/>
-      <c r="K1005" s="7"/>
-      <c r="L1005" s="7"/>
-      <c r="M1005" s="7"/>
-      <c r="N1005" s="7"/>
-      <c r="O1005" s="7"/>
-      <c r="P1005" s="7"/>
-      <c r="Q1005" s="7"/>
-      <c r="R1005" s="7"/>
-      <c r="S1005" s="7"/>
-      <c r="T1005" s="7"/>
-      <c r="U1005" s="7"/>
-      <c r="V1005" s="7"/>
-      <c r="W1005" s="7"/>
-      <c r="X1005" s="7"/>
-      <c r="Y1005" s="7"/>
-      <c r="Z1005" s="7"/>
-    </row>
-    <row r="1006" ht="19.5" customHeight="1">
-      <c r="A1006" s="7"/>
-      <c r="B1006" s="7"/>
-      <c r="C1006" s="7"/>
-      <c r="D1006" s="7"/>
-      <c r="E1006" s="7"/>
-      <c r="F1006" s="7"/>
-      <c r="G1006" s="7"/>
-      <c r="H1006" s="7"/>
-      <c r="I1006" s="7"/>
-      <c r="J1006" s="7"/>
-      <c r="K1006" s="7"/>
-      <c r="L1006" s="7"/>
-      <c r="M1006" s="7"/>
-      <c r="N1006" s="7"/>
-      <c r="O1006" s="7"/>
-      <c r="P1006" s="7"/>
-      <c r="Q1006" s="7"/>
-      <c r="R1006" s="7"/>
-      <c r="S1006" s="7"/>
-      <c r="T1006" s="7"/>
-      <c r="U1006" s="7"/>
-      <c r="V1006" s="7"/>
-      <c r="W1006" s="7"/>
-      <c r="X1006" s="7"/>
-      <c r="Y1006" s="7"/>
-      <c r="Z1006" s="7"/>
-    </row>
-    <row r="1007" ht="19.5" customHeight="1">
-      <c r="A1007" s="7"/>
-      <c r="B1007" s="7"/>
-      <c r="C1007" s="7"/>
-      <c r="D1007" s="7"/>
-      <c r="E1007" s="7"/>
-      <c r="F1007" s="7"/>
-      <c r="G1007" s="7"/>
-      <c r="H1007" s="7"/>
-      <c r="I1007" s="7"/>
-      <c r="J1007" s="7"/>
-      <c r="K1007" s="7"/>
-      <c r="L1007" s="7"/>
-      <c r="M1007" s="7"/>
-      <c r="N1007" s="7"/>
-      <c r="O1007" s="7"/>
-      <c r="P1007" s="7"/>
-      <c r="Q1007" s="7"/>
-      <c r="R1007" s="7"/>
-      <c r="S1007" s="7"/>
-      <c r="T1007" s="7"/>
-      <c r="U1007" s="7"/>
-      <c r="V1007" s="7"/>
-      <c r="W1007" s="7"/>
-      <c r="X1007" s="7"/>
-      <c r="Y1007" s="7"/>
-      <c r="Z1007" s="7"/>
-    </row>
-    <row r="1008" ht="19.5" customHeight="1">
-      <c r="A1008" s="7"/>
-      <c r="B1008" s="7"/>
-      <c r="C1008" s="7"/>
-      <c r="D1008" s="7"/>
-      <c r="E1008" s="7"/>
-      <c r="F1008" s="7"/>
-      <c r="G1008" s="7"/>
-      <c r="H1008" s="7"/>
-      <c r="I1008" s="7"/>
-      <c r="J1008" s="7"/>
-      <c r="K1008" s="7"/>
-      <c r="L1008" s="7"/>
-      <c r="M1008" s="7"/>
-      <c r="N1008" s="7"/>
-      <c r="O1008" s="7"/>
-      <c r="P1008" s="7"/>
-      <c r="Q1008" s="7"/>
-      <c r="R1008" s="7"/>
-      <c r="S1008" s="7"/>
-      <c r="T1008" s="7"/>
-      <c r="U1008" s="7"/>
-      <c r="V1008" s="7"/>
-      <c r="W1008" s="7"/>
-      <c r="X1008" s="7"/>
-      <c r="Y1008" s="7"/>
-      <c r="Z1008" s="7"/>
-    </row>
-    <row r="1009" ht="19.5" customHeight="1">
-      <c r="A1009" s="7"/>
-      <c r="B1009" s="7"/>
-      <c r="C1009" s="7"/>
-      <c r="D1009" s="7"/>
-      <c r="E1009" s="7"/>
-      <c r="F1009" s="7"/>
-      <c r="G1009" s="7"/>
-      <c r="H1009" s="7"/>
-      <c r="I1009" s="7"/>
-      <c r="J1009" s="7"/>
-      <c r="K1009" s="7"/>
-      <c r="L1009" s="7"/>
-      <c r="M1009" s="7"/>
-      <c r="N1009" s="7"/>
-      <c r="O1009" s="7"/>
-      <c r="P1009" s="7"/>
-      <c r="Q1009" s="7"/>
-      <c r="R1009" s="7"/>
-      <c r="S1009" s="7"/>
-      <c r="T1009" s="7"/>
-      <c r="U1009" s="7"/>
-      <c r="V1009" s="7"/>
-      <c r="W1009" s="7"/>
-      <c r="X1009" s="7"/>
-      <c r="Y1009" s="7"/>
-      <c r="Z1009" s="7"/>
-    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.5" right="0.5" top="0.75"/>

</xml_diff>